<commit_message>
[FIX] xlsx: import new lines in sharedStrings
When implementing the multiline text feature, we forgot to change the
xlsx import, that explicitly removed new lines from the sharedStrings
because we didn't support it at the time.

There was also a bug where the whitespace was not preserved in the
sharedStrings, because we extracted the text from the `<si>` element
instead of the `<t>` element that had the attribute xml:space="preserve".

And for multi-line cells to be considered as such by Excel, they need
to have the style `wrapText="1"`.

Task: 4044862
X-original-commit: 207b1c42dc92bd1d2db834a838a22e70566f20c7
Part-of: odoo/o-spreadsheet#5410
Signed-off-by: Rémi Rahir (rar) <rar@odoo.com>
Signed-off-by: Adrien Minne (adrm) <adrm@odoo.com>
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA4A409-66E7-4CFC-A548-ECD1D6D1B504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{157AC437-DB84-431C-BDD0-6A0421B0B149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23295" yWindow="195" windowWidth="21600" windowHeight="11385" firstSheet="13" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23295" yWindow="195" windowWidth="21600" windowHeight="11385" firstSheet="13" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,9 @@
   <externalReferences>
     <externalReference r:id="rId15"/>
   </externalReferences>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId16"/>
+    <pivotCache cacheId="3563" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="435">
   <si>
     <t>CF =42</t>
   </si>
@@ -1307,6 +1307,9 @@
   <si>
     <t>This text have
  a newLine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      with whitespace before</t>
   </si>
   <si>
     <t>Decimal</t>
@@ -1372,7 +1375,7 @@
     <numFmt numFmtId="168" formatCode="#,##0&quot; EUR €&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;€&quot;#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2372,7 +2375,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2385,6 +2387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2392,6 +2395,157 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
   <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike/>
+        <u/>
+        <color theme="7"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="lightTrellis">
+          <fgColor theme="4"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2798,157 +2952,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike/>
-        <u/>
-        <color theme="7"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="lightTrellis">
-          <fgColor theme="4"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -3370,7 +3373,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3474,7 +3477,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7572,7 +7575,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="3563" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7722,7 +7725,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -7734,22 +7737,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="7">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7859,9 +7862,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7899,7 +7902,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8005,7 +8008,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8147,7 +8150,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8164,7 +8167,7 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -8173,7 +8176,7 @@
     <col min="6" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1">
       <c r="A1" s="21"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -8182,7 +8185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="27.75">
       <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
@@ -8195,25 +8198,25 @@
       <c r="H2" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="119"/>
+      <c r="I2" s="123"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1">
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="117">
         <v>8</v>
       </c>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="120">
+      <c r="K3" s="119">
         <v>5</v>
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -8226,50 +8229,50 @@
       <c r="G4" s="117">
         <v>9</v>
       </c>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="121"/>
+      <c r="K4" s="120"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1">
       <c r="C5" s="117">
         <v>42</v>
       </c>
       <c r="G5" s="117">
         <v>15</v>
       </c>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="121"/>
+      <c r="K5" s="120"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1">
       <c r="G6" s="117">
         <v>22</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="121"/>
+      <c r="K6" s="120"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1">
       <c r="C7" s="117">
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="121"/>
+      <c r="K7" s="120"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1">
       <c r="G8" s="117">
         <v>30</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="122"/>
+      <c r="K8" s="121"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17.25" customHeight="1">
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
@@ -8279,7 +8282,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1">
       <c r="C10" s="117">
         <f>SUM(C4:C7)</f>
         <v>57.4</v>
@@ -8288,13 +8291,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17.25" customHeight="1">
       <c r="C11" s="117">
         <f>-(3+C7*SUM(C4:C7))</f>
         <v>-175.2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="17.25" customHeight="1">
       <c r="C12" s="117">
         <f>SUM(C9:C11)</f>
         <v>-63.399999999999991</v>
@@ -8303,13 +8306,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1">
       <c r="G13" s="117">
         <f>A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12+A13+A14+A15+A16+A17+A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17.25" customHeight="1">
       <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
@@ -8318,32 +8321,32 @@
         <v>#CYCLE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="17.25" customHeight="1">
       <c r="C15" s="117" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="17.25" customHeight="1">
       <c r="C16" s="117" t="str">
         <f>C15</f>
         <v>=(+</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1">
       <c r="C17" s="117" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1">
       <c r="C18" s="117" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1">
       <c r="E19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
         <v>15</v>
@@ -8357,7 +8360,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -8367,7 +8370,7 @@
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1">
       <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
@@ -8381,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1">
       <c r="C24" s="16">
         <v>10</v>
       </c>
@@ -8392,7 +8395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1">
       <c r="C25" s="16">
         <v>10.122999999999999</v>
       </c>
@@ -8403,7 +8406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1">
       <c r="B26" s="117" t="s">
         <v>20</v>
       </c>
@@ -8417,7 +8420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1">
       <c r="A27" s="117" t="s">
         <v>22</v>
       </c>
@@ -8434,7 +8437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1">
       <c r="A28" s="117" t="s">
         <v>23</v>
       </c>
@@ -8451,7 +8454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1">
       <c r="A29" s="117" t="s">
         <v>24</v>
       </c>
@@ -8468,7 +8471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1">
       <c r="A30" s="117" t="s">
         <v>25</v>
       </c>
@@ -8485,7 +8488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1">
       <c r="A31" s="117" t="s">
         <v>26</v>
       </c>
@@ -8502,7 +8505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1">
       <c r="A32" s="117" t="s">
         <v>27</v>
       </c>
@@ -8519,7 +8522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="17.25" customHeight="1">
       <c r="A33" s="117" t="s">
         <v>28</v>
       </c>
@@ -8536,7 +8539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="17.25" customHeight="1">
       <c r="A34" s="117" t="s">
         <v>29</v>
       </c>
@@ -8547,7 +8550,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="17.25" customHeight="1">
       <c r="A35" s="117" t="s">
         <v>30</v>
       </c>
@@ -8564,7 +8567,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8614,7 +8617,7 @@
       <selection sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8626,12 +8629,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8645,7 +8648,7 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
@@ -8665,7 +8668,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8676,11 +8679,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025F2510-D243-4DA1-81DE-BBDDA9BC3681}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
@@ -8689,36 +8692,36 @@
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="114" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B1" s="115" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C1" s="115" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D1" s="115" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E1" s="115" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F1" s="115" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="G1" s="115" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="H1" s="115" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="I1" s="116" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="104">
         <v>4</v>
       </c>
@@ -8729,7 +8732,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="105" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E2" s="106">
         <v>45575</v>
@@ -8738,7 +8741,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G2" s="107" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="H2" s="106">
         <v>45292</v>
@@ -8747,7 +8750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="104">
         <v>3</v>
       </c>
@@ -8758,7 +8761,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="105" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E3" s="106">
         <v>45576</v>
@@ -8767,16 +8770,16 @@
         <v>0.57638888888888884</v>
       </c>
       <c r="G3" s="107" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H3" s="106">
         <v>45231</v>
       </c>
       <c r="I3" s="108" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="104">
         <v>9</v>
       </c>
@@ -8787,7 +8790,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="105" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E4" s="106">
         <v>45574</v>
@@ -8796,7 +8799,7 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="G4" s="107" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H4" s="106">
         <v>45325</v>
@@ -8805,7 +8808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="104">
         <v>5</v>
       </c>
@@ -8816,7 +8819,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="105" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E5" s="106">
         <v>45573</v>
@@ -8825,7 +8828,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="G5" s="105" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="H5" s="106">
         <v>45084</v>
@@ -8834,7 +8837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="109">
         <v>7</v>
       </c>
@@ -8845,7 +8848,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="110" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E6" s="111">
         <v>45566</v>
@@ -8854,13 +8857,13 @@
         <v>0.5229166666666667</v>
       </c>
       <c r="G6" s="110" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H6" s="111">
         <v>45420</v>
       </c>
       <c r="I6" s="113" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -8912,12 +8915,12 @@
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="17.25" customHeight="1">
       <c r="A1" s="117" t="s">
         <v>31</v>
       </c>
@@ -8952,7 +8955,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1">
       <c r="A2" s="117" t="s">
         <v>41</v>
       </c>
@@ -8998,7 +9001,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1">
       <c r="A3" s="117" t="s">
         <v>43</v>
       </c>
@@ -9044,7 +9047,7 @@
         <v>1217.7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="17.25" customHeight="1">
       <c r="A4" s="117" t="s">
         <v>45</v>
       </c>
@@ -9090,7 +9093,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1">
       <c r="A5" s="117" t="s">
         <v>47</v>
       </c>
@@ -9136,7 +9139,7 @@
         <v>1246.7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="17.25" customHeight="1">
       <c r="A6" s="117" t="s">
         <v>49</v>
       </c>
@@ -9182,7 +9185,7 @@
         <v>1213.7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="17.25" customHeight="1">
       <c r="A7" s="117" t="s">
         <v>52</v>
       </c>
@@ -9216,7 +9219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="17.25" customHeight="1">
       <c r="A8" s="117" t="s">
         <v>54</v>
       </c>
@@ -9250,7 +9253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="17.25" customHeight="1">
       <c r="A9" s="117" t="s">
         <v>56</v>
       </c>
@@ -9281,7 +9284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="17.25" customHeight="1">
       <c r="A10" s="117" t="s">
         <v>58</v>
       </c>
@@ -9297,7 +9300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="17.25" customHeight="1">
       <c r="A11" s="117" t="s">
         <v>59</v>
       </c>
@@ -9316,7 +9319,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="17.25" customHeight="1">
       <c r="A12" s="117" t="s">
         <v>61</v>
       </c>
@@ -9347,7 +9350,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="17.25" customHeight="1">
       <c r="A13" s="117" t="s">
         <v>62</v>
       </c>
@@ -9378,7 +9381,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="17.25" customHeight="1">
       <c r="A14" s="117" t="s">
         <v>67</v>
       </c>
@@ -9394,7 +9397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="17.25" customHeight="1">
       <c r="A15" s="117" t="s">
         <v>68</v>
       </c>
@@ -9410,7 +9413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="17.25" customHeight="1">
       <c r="A16" s="117" t="s">
         <v>69</v>
       </c>
@@ -9426,7 +9429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1">
       <c r="A17" s="117" t="s">
         <v>70</v>
       </c>
@@ -9442,7 +9445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1">
       <c r="A18" s="117" t="s">
         <v>71</v>
       </c>
@@ -9458,7 +9461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1">
       <c r="A19" s="117" t="s">
         <v>72</v>
       </c>
@@ -9474,7 +9477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1">
       <c r="A20" s="117" t="s">
         <v>73</v>
       </c>
@@ -9490,7 +9493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1">
       <c r="A21" s="117" t="s">
         <v>74</v>
       </c>
@@ -9506,7 +9509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1">
       <c r="A22" s="117" t="s">
         <v>76</v>
       </c>
@@ -9522,7 +9525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1">
       <c r="A23" s="117" t="s">
         <v>77</v>
       </c>
@@ -9538,7 +9541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="17.25" customHeight="1">
       <c r="A24" s="117" t="s">
         <v>78</v>
       </c>
@@ -9555,7 +9558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="17.25" customHeight="1">
       <c r="A25" s="117" t="s">
         <v>79</v>
       </c>
@@ -9571,7 +9574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="17.25" customHeight="1">
       <c r="A26" s="117" t="s">
         <v>81</v>
       </c>
@@ -9587,7 +9590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="17.25" customHeight="1">
       <c r="A27" s="117" t="s">
         <v>82</v>
       </c>
@@ -9603,7 +9606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="17.25" customHeight="1">
       <c r="A28" s="117" t="s">
         <v>83</v>
       </c>
@@ -9620,7 +9623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="17.25" customHeight="1">
       <c r="A29" s="117" t="s">
         <v>84</v>
       </c>
@@ -9636,7 +9639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17.25" customHeight="1">
       <c r="A30" s="117" t="s">
         <v>85</v>
       </c>
@@ -9652,7 +9655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="17.25" customHeight="1">
       <c r="A31" s="117" t="s">
         <v>86</v>
       </c>
@@ -9668,7 +9671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="17.25" customHeight="1">
       <c r="A32" s="117" t="s">
         <v>87</v>
       </c>
@@ -9684,7 +9687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17.25" customHeight="1">
       <c r="A33" s="117" t="s">
         <v>88</v>
       </c>
@@ -9700,7 +9703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="17.25" customHeight="1">
       <c r="A34" s="117" t="s">
         <v>89</v>
       </c>
@@ -9716,7 +9719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17.25" customHeight="1">
       <c r="A35" s="117" t="s">
         <v>90</v>
       </c>
@@ -9732,7 +9735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="17.25" customHeight="1">
       <c r="A36" s="117" t="s">
         <v>91</v>
       </c>
@@ -9748,7 +9751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="17.25" customHeight="1">
       <c r="A37" s="117" t="s">
         <v>92</v>
       </c>
@@ -9764,7 +9767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="17.25" customHeight="1">
       <c r="A38" s="117" t="s">
         <v>93</v>
       </c>
@@ -9781,7 +9784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="17.25" customHeight="1">
       <c r="A39" s="117" t="s">
         <v>94</v>
       </c>
@@ -9797,7 +9800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="17.25" customHeight="1">
       <c r="A40" s="117" t="s">
         <v>95</v>
       </c>
@@ -9813,7 +9816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="17.25" customHeight="1">
       <c r="A41" s="117" t="s">
         <v>96</v>
       </c>
@@ -9829,7 +9832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="17.25" customHeight="1">
       <c r="A42" s="117" t="s">
         <v>97</v>
       </c>
@@ -9845,7 +9848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="17.25" customHeight="1">
       <c r="A43" s="117" t="s">
         <v>98</v>
       </c>
@@ -9861,7 +9864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="17.25" customHeight="1">
       <c r="A44" s="117" t="s">
         <v>99</v>
       </c>
@@ -9877,7 +9880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="17.25" customHeight="1">
       <c r="A45" s="117" t="s">
         <v>100</v>
       </c>
@@ -9893,7 +9896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="17.25" customHeight="1">
       <c r="A46" s="117" t="s">
         <v>101</v>
       </c>
@@ -9909,7 +9912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="17.25" customHeight="1">
       <c r="A47" s="117" t="s">
         <v>102</v>
       </c>
@@ -9925,7 +9928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="17.25" customHeight="1">
       <c r="A48" s="117" t="s">
         <v>103</v>
       </c>
@@ -9941,7 +9944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="17.25" customHeight="1">
       <c r="A49" s="117" t="s">
         <v>104</v>
       </c>
@@ -9957,7 +9960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="17.25" customHeight="1">
       <c r="A50" s="117" t="s">
         <v>105</v>
       </c>
@@ -9974,7 +9977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="17.25" customHeight="1">
       <c r="A51" s="117" t="s">
         <v>106</v>
       </c>
@@ -9991,7 +9994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="17.25" customHeight="1">
       <c r="A52" s="117" t="s">
         <v>107</v>
       </c>
@@ -10007,7 +10010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1">
       <c r="A53" s="117" t="s">
         <v>108</v>
       </c>
@@ -10023,7 +10026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="17.25" customHeight="1">
       <c r="A54" s="117" t="s">
         <v>109</v>
       </c>
@@ -10039,7 +10042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1">
       <c r="A55" s="117" t="s">
         <v>110</v>
       </c>
@@ -10055,7 +10058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1">
       <c r="A56" s="117" t="s">
         <v>111</v>
       </c>
@@ -10071,7 +10074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1">
       <c r="A57" s="117" t="s">
         <v>112</v>
       </c>
@@ -10087,7 +10090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1">
       <c r="A58" s="117" t="s">
         <v>113</v>
       </c>
@@ -10103,7 +10106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1">
       <c r="A59" s="117" t="s">
         <v>114</v>
       </c>
@@ -10119,7 +10122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1">
       <c r="A60" s="117" t="s">
         <v>115</v>
       </c>
@@ -10135,7 +10138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1">
       <c r="A61" s="117" t="s">
         <v>116</v>
       </c>
@@ -10151,7 +10154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1">
       <c r="A62" s="117" t="s">
         <v>117</v>
       </c>
@@ -10167,7 +10170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="17.25" customHeight="1">
       <c r="A63" s="117" t="s">
         <v>118</v>
       </c>
@@ -10183,7 +10186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="17.25" customHeight="1">
       <c r="A64" s="117" t="s">
         <v>119</v>
       </c>
@@ -10199,7 +10202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="17.25" customHeight="1">
       <c r="A65" s="117" t="s">
         <v>120</v>
       </c>
@@ -10215,7 +10218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="17.25" customHeight="1">
       <c r="A66" s="117" t="s">
         <v>121</v>
       </c>
@@ -10231,7 +10234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="17.25" customHeight="1">
       <c r="A67" s="117" t="s">
         <v>122</v>
       </c>
@@ -10247,7 +10250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="17.25" customHeight="1">
       <c r="A68" s="117" t="s">
         <v>123</v>
       </c>
@@ -10263,7 +10266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="17.25" customHeight="1">
       <c r="A69" s="117" t="s">
         <v>125</v>
       </c>
@@ -10279,7 +10282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="17.25" customHeight="1">
       <c r="A70" s="117" t="s">
         <v>127</v>
       </c>
@@ -10295,7 +10298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="17.25" customHeight="1">
       <c r="A71" s="117" t="s">
         <v>129</v>
       </c>
@@ -10311,7 +10314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="17.25" customHeight="1">
       <c r="A72" s="117" t="s">
         <v>130</v>
       </c>
@@ -10327,7 +10330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="17.25" customHeight="1">
       <c r="A73" s="117" t="s">
         <v>131</v>
       </c>
@@ -10343,7 +10346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="17.25" customHeight="1">
       <c r="A74" s="117" t="s">
         <v>132</v>
       </c>
@@ -10359,7 +10362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="17.25" customHeight="1">
       <c r="A75" s="117" t="s">
         <v>133</v>
       </c>
@@ -10375,7 +10378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="17.25" customHeight="1">
       <c r="A76" s="117" t="s">
         <v>134</v>
       </c>
@@ -10391,7 +10394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="17.25" customHeight="1">
       <c r="A77" s="117" t="s">
         <v>135</v>
       </c>
@@ -10407,7 +10410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="17.25" customHeight="1">
       <c r="A78" s="117" t="s">
         <v>136</v>
       </c>
@@ -10423,7 +10426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="17.25" customHeight="1">
       <c r="A79" s="117" t="s">
         <v>137</v>
       </c>
@@ -10439,7 +10442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="17.25" customHeight="1">
       <c r="A80" s="117" t="s">
         <v>138</v>
       </c>
@@ -10455,7 +10458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="17.25" customHeight="1">
       <c r="A81" s="117" t="s">
         <v>139</v>
       </c>
@@ -10471,7 +10474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="17.25" customHeight="1">
       <c r="A82" s="117" t="s">
         <v>141</v>
       </c>
@@ -10487,7 +10490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="17.25" customHeight="1">
       <c r="A83" s="117" t="s">
         <v>142</v>
       </c>
@@ -10503,7 +10506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="17.25" customHeight="1">
       <c r="A84" s="117" t="s">
         <v>143</v>
       </c>
@@ -10519,7 +10522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="17.25" customHeight="1">
       <c r="A85" s="117" t="s">
         <v>144</v>
       </c>
@@ -10535,7 +10538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="17.25" customHeight="1">
       <c r="A86" s="117" t="s">
         <v>146</v>
       </c>
@@ -10551,7 +10554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="17.25" customHeight="1">
       <c r="A87" s="117" t="s">
         <v>147</v>
       </c>
@@ -10567,7 +10570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="17.25" customHeight="1">
       <c r="A88" s="117" t="s">
         <v>148</v>
       </c>
@@ -10583,7 +10586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="17.25" customHeight="1">
       <c r="A89" s="117" t="s">
         <v>149</v>
       </c>
@@ -10599,7 +10602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="17.25" customHeight="1">
       <c r="A90" s="117" t="s">
         <v>150</v>
       </c>
@@ -10615,7 +10618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="17.25" customHeight="1">
       <c r="A91" s="117" t="s">
         <v>151</v>
       </c>
@@ -10631,7 +10634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1">
       <c r="A92" s="117" t="s">
         <v>152</v>
       </c>
@@ -10647,7 +10650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1">
       <c r="A93" s="117" t="s">
         <v>153</v>
       </c>
@@ -10663,7 +10666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1">
       <c r="A94" s="117" t="s">
         <v>154</v>
       </c>
@@ -10679,7 +10682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1">
       <c r="A95" s="117" t="s">
         <v>155</v>
       </c>
@@ -10695,7 +10698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1">
       <c r="A96" s="117" t="s">
         <v>156</v>
       </c>
@@ -10711,7 +10714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="17.25" customHeight="1">
       <c r="A97" s="117" t="s">
         <v>157</v>
       </c>
@@ -10727,7 +10730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="17.25" customHeight="1">
       <c r="A98" s="117" t="s">
         <v>158</v>
       </c>
@@ -10743,7 +10746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="17.25" customHeight="1">
       <c r="A99" s="117" t="s">
         <v>159</v>
       </c>
@@ -10759,20 +10762,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="17.25" customHeight="1">
       <c r="A100" s="117" t="s">
         <v>160</v>
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45594.46900636574</v>
+        <v>45663.51402037037</v>
       </c>
       <c r="D100" s="117">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="17.25" customHeight="1">
       <c r="A101" s="117" t="s">
         <v>161</v>
       </c>
@@ -10788,7 +10791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="17.25" customHeight="1">
       <c r="A102" s="117" t="s">
         <v>162</v>
       </c>
@@ -10804,7 +10807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="17.25" customHeight="1">
       <c r="A103" s="117" t="s">
         <v>163</v>
       </c>
@@ -10820,7 +10823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="17.25" customHeight="1">
       <c r="A104" s="117" t="s">
         <v>164</v>
       </c>
@@ -10836,7 +10839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="17.25" customHeight="1">
       <c r="A105" s="117" t="s">
         <v>165</v>
       </c>
@@ -10852,7 +10855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="17.25" customHeight="1">
       <c r="A106" s="117" t="s">
         <v>166</v>
       </c>
@@ -10868,7 +10871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="17.25" customHeight="1">
       <c r="A107" s="117" t="s">
         <v>167</v>
       </c>
@@ -10884,7 +10887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="17.25" customHeight="1">
       <c r="A108" s="117" t="s">
         <v>168</v>
       </c>
@@ -10900,7 +10903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="17.25" customHeight="1">
       <c r="A109" s="117" t="s">
         <v>169</v>
       </c>
@@ -10916,7 +10919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="17.25" customHeight="1">
       <c r="A110" s="117" t="s">
         <v>170</v>
       </c>
@@ -10932,7 +10935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="17.25" customHeight="1">
       <c r="A111" s="117" t="s">
         <v>171</v>
       </c>
@@ -10948,12 +10951,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="17.25" customHeight="1">
       <c r="A112" s="117"/>
       <c r="B112" s="117"/>
       <c r="D112" s="117"/>
     </row>
-    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="17.25" customHeight="1">
       <c r="A113" s="117" t="s">
         <v>172</v>
       </c>
@@ -10969,7 +10972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="17.25" customHeight="1">
       <c r="A114" s="117" t="s">
         <v>173</v>
       </c>
@@ -10985,7 +10988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="17.25" customHeight="1">
       <c r="A115" s="117" t="s">
         <v>175</v>
       </c>
@@ -11001,7 +11004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="17.25" customHeight="1">
       <c r="A116" s="117" t="s">
         <v>177</v>
       </c>
@@ -11017,7 +11020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="17.25" customHeight="1">
       <c r="A117" s="117" t="s">
         <v>178</v>
       </c>
@@ -11033,7 +11036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="17.25" customHeight="1">
       <c r="A118" s="117" t="s">
         <v>179</v>
       </c>
@@ -11049,7 +11052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="17.25" customHeight="1">
       <c r="A119" s="117" t="s">
         <v>180</v>
       </c>
@@ -11065,7 +11068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="17.25" customHeight="1">
       <c r="A120" s="117" t="s">
         <v>181</v>
       </c>
@@ -11081,7 +11084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="17.25" customHeight="1">
       <c r="A121" s="117" t="s">
         <v>182</v>
       </c>
@@ -11097,7 +11100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="17.25" customHeight="1">
       <c r="A122" s="117" t="s">
         <v>183</v>
       </c>
@@ -11113,7 +11116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="17.25" customHeight="1">
       <c r="A123" s="117" t="s">
         <v>184</v>
       </c>
@@ -11129,7 +11132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="17.25" customHeight="1">
       <c r="A124" s="117" t="s">
         <v>185</v>
       </c>
@@ -11145,7 +11148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="17.25" customHeight="1">
       <c r="A125" s="117" t="s">
         <v>186</v>
       </c>
@@ -11161,7 +11164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="17.25" customHeight="1">
       <c r="A126" s="117" t="s">
         <v>187</v>
       </c>
@@ -11177,7 +11180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="17.25" customHeight="1">
       <c r="A127" s="117" t="s">
         <v>188</v>
       </c>
@@ -11193,7 +11196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="17.25" customHeight="1">
       <c r="A128" s="117" t="s">
         <v>189</v>
       </c>
@@ -11209,7 +11212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="17.25" customHeight="1">
       <c r="A129" s="117" t="s">
         <v>190</v>
       </c>
@@ -11225,7 +11228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="17.25" customHeight="1">
       <c r="A130" s="117" t="s">
         <v>191</v>
       </c>
@@ -11241,7 +11244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="17.25" customHeight="1">
       <c r="A131" s="117" t="s">
         <v>192</v>
       </c>
@@ -11257,7 +11260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="17.25" customHeight="1">
       <c r="A132" s="117" t="s">
         <v>193</v>
       </c>
@@ -11273,7 +11276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="17.25" customHeight="1">
       <c r="A133" s="117" t="s">
         <v>194</v>
       </c>
@@ -11289,7 +11292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="17.25" customHeight="1">
       <c r="A134" s="117" t="s">
         <v>195</v>
       </c>
@@ -11305,7 +11308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="17.25" customHeight="1">
       <c r="A135" s="117" t="s">
         <v>196</v>
       </c>
@@ -11321,7 +11324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="17.25" customHeight="1">
       <c r="A136" s="117" t="s">
         <v>198</v>
       </c>
@@ -11337,7 +11340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="17.25" customHeight="1">
       <c r="A137" s="117" t="s">
         <v>199</v>
       </c>
@@ -11353,7 +11356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="17.25" customHeight="1">
       <c r="A138" s="117" t="s">
         <v>200</v>
       </c>
@@ -11369,7 +11372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="17.25" customHeight="1">
       <c r="A139" s="117" t="s">
         <v>201</v>
       </c>
@@ -11385,7 +11388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="17.25" customHeight="1">
       <c r="A140" s="117" t="s">
         <v>202</v>
       </c>
@@ -11401,7 +11404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="17.25" customHeight="1">
       <c r="A141" s="117" t="s">
         <v>203</v>
       </c>
@@ -11417,7 +11420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="17.25" customHeight="1">
       <c r="A142" s="117" t="s">
         <v>205</v>
       </c>
@@ -11433,7 +11436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="17.25" customHeight="1">
       <c r="A143" s="117" t="s">
         <v>206</v>
       </c>
@@ -11449,20 +11452,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="17.25" customHeight="1">
       <c r="A144" s="117" t="s">
         <v>207</v>
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45594</v>
+        <v>45663</v>
       </c>
       <c r="D144" s="117">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="17.25" customHeight="1">
       <c r="A145" s="117" t="s">
         <v>208</v>
       </c>
@@ -11478,7 +11481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="17.25" customHeight="1">
       <c r="A146" s="117" t="s">
         <v>210</v>
       </c>
@@ -11494,7 +11497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="17.25" customHeight="1">
       <c r="A147" s="117" t="s">
         <v>211</v>
       </c>
@@ -11510,7 +11513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="17.25" customHeight="1">
       <c r="A148" s="117" t="s">
         <v>213</v>
       </c>
@@ -11526,7 +11529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="17.25" customHeight="1">
       <c r="A149" s="117" t="s">
         <v>214</v>
       </c>
@@ -11542,7 +11545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" ht="17.25" customHeight="1">
       <c r="A150" s="117" t="s">
         <v>215</v>
       </c>
@@ -11558,7 +11561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="17.25" customHeight="1">
       <c r="A151" s="117" t="s">
         <v>216</v>
       </c>
@@ -11574,7 +11577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="17.25" customHeight="1">
       <c r="A152" s="117" t="s">
         <v>217</v>
       </c>
@@ -11590,7 +11593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="17.25" customHeight="1">
       <c r="A153" s="117" t="s">
         <v>218</v>
       </c>
@@ -11606,7 +11609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" ht="17.25" customHeight="1">
       <c r="A154" s="117" t="s">
         <v>219</v>
       </c>
@@ -11623,7 +11626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="17.25" customHeight="1">
       <c r="A155" s="117" t="s">
         <v>220</v>
       </c>
@@ -11639,7 +11642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="17.25" customHeight="1">
       <c r="A156" s="117" t="s">
         <v>221</v>
       </c>
@@ -11655,7 +11658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" ht="17.25" customHeight="1">
       <c r="A157" s="117" t="s">
         <v>222</v>
       </c>
@@ -11671,7 +11674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" ht="17.25" customHeight="1">
       <c r="A158" s="117" t="s">
         <v>223</v>
       </c>
@@ -11687,7 +11690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="17.25" customHeight="1">
       <c r="A159" s="117" t="s">
         <v>224</v>
       </c>
@@ -11703,7 +11706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" ht="17.25" customHeight="1">
       <c r="A160" s="117" t="s">
         <v>225</v>
       </c>
@@ -11719,7 +11722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" ht="17.25" customHeight="1">
       <c r="A161" s="117" t="s">
         <v>226</v>
       </c>
@@ -11735,7 +11738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="17.25" customHeight="1">
       <c r="A162" s="117" t="s">
         <v>227</v>
       </c>
@@ -11751,7 +11754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" ht="17.25" customHeight="1">
       <c r="A163" s="117" t="s">
         <v>229</v>
       </c>
@@ -11769,10 +11772,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11792,7 +11795,7 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
@@ -11802,17 +11805,17 @@
     <col min="15" max="18" width="9.140625" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>230</v>
       </c>
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="122" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="123"/>
+      <c r="E1" s="122"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -11820,19 +11823,19 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="D3" s="85" t="s">
         <v>235</v>
       </c>
@@ -11840,25 +11843,25 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="75" customHeight="1">
       <c r="A5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="17" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="18" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:8" outlineLevel="1"/>
+    <row r="11" spans="1:8" outlineLevel="1"/>
+    <row r="12" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="13" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="14" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="15" spans="1:8" outlineLevel="1" collapsed="1"/>
+    <row r="16" spans="1:8" outlineLevel="1"/>
+    <row r="17" outlineLevel="1"/>
+    <row r="18" outlineLevel="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:E2"/>
@@ -11880,14 +11883,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1">
       <c r="A1" s="68" t="s">
         <v>239</v>
       </c>
@@ -11909,7 +11912,7 @@
       </c>
       <c r="M1" s="36"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="40" t="s">
         <v>245</v>
       </c>
@@ -11935,7 +11938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="41" t="s">
         <v>252</v>
       </c>
@@ -11958,7 +11961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15">
       <c r="A4" s="42" t="s">
         <v>256</v>
       </c>
@@ -11984,7 +11987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="43" t="s">
         <v>262</v>
       </c>
@@ -12004,7 +12007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="44" t="s">
         <v>266</v>
       </c>
@@ -12027,7 +12030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="45" t="s">
         <v>271</v>
       </c>
@@ -12047,7 +12050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="21">
       <c r="A8" s="46" t="s">
         <v>275</v>
       </c>
@@ -12070,7 +12073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="47" t="s">
         <v>280</v>
       </c>
@@ -12087,7 +12090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="48" t="s">
         <v>283</v>
       </c>
@@ -12095,7 +12098,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1">
       <c r="A11" s="49" t="s">
         <v>285</v>
       </c>
@@ -12104,7 +12107,7 @@
       </c>
       <c r="F11" s="36"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1">
       <c r="A12" s="50" t="s">
         <v>287</v>
       </c>
@@ -12118,7 +12121,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A13" s="51" t="s">
         <v>290</v>
       </c>
@@ -12129,7 +12132,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A14" s="52" t="s">
         <v>291</v>
       </c>
@@ -12143,7 +12146,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A15" s="53" t="s">
         <v>293</v>
       </c>
@@ -12154,7 +12157,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
       <c r="A16" s="54" t="s">
         <v>294</v>
       </c>
@@ -12168,12 +12171,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.5" thickBot="1">
       <c r="A17" s="55" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.5" thickBot="1">
       <c r="A18" s="74" t="s">
         <v>297</v>
       </c>
@@ -12185,7 +12188,7 @@
       </c>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13.5" thickBot="1">
       <c r="A19" s="75" t="s">
         <v>300</v>
       </c>
@@ -12196,7 +12199,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="51.75" thickBot="1">
       <c r="A20" s="76" t="s">
         <v>303</v>
       </c>
@@ -12210,12 +12213,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.5" thickBot="1">
       <c r="A21" s="77" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.5" thickBot="1">
       <c r="A22" s="78" t="s">
         <v>307</v>
       </c>
@@ -12224,13 +12227,13 @@
       </c>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.5" thickBot="1">
       <c r="A23" s="79" t="s">
         <v>309</v>
       </c>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="A24" s="80" t="s">
         <v>310</v>
       </c>
@@ -12239,20 +12242,20 @@
       </c>
       <c r="E24" s="21"/>
     </row>
-    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C26" s="67" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C28" s="88" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="13.5" thickTop="1"/>
+    <row r="30" spans="1:6">
       <c r="C30" s="87" t="s">
         <v>314</v>
       </c>
@@ -12271,13 +12274,13 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.5" thickBot="1">
       <c r="A1" s="37" t="s">
         <v>315</v>
       </c>
@@ -12294,7 +12297,7 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="38" t="s">
         <v>319</v>
       </c>
@@ -12317,7 +12320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="38" t="s">
         <v>321</v>
       </c>
@@ -12340,7 +12343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="38" t="s">
         <v>325</v>
       </c>
@@ -12360,7 +12363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="38" t="s">
         <v>328</v>
       </c>
@@ -12384,7 +12387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="38" t="s">
         <v>330</v>
       </c>
@@ -12407,7 +12410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="38" t="s">
         <v>333</v>
       </c>
@@ -12433,7 +12436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="38" t="s">
         <v>337</v>
       </c>
@@ -12444,7 +12447,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="38" t="s">
         <v>339</v>
       </c>
@@ -12453,7 +12456,7 @@
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.5" thickBot="1">
       <c r="A10" s="38" t="s">
         <v>340</v>
       </c>
@@ -12471,7 +12474,7 @@
       <c r="I10" s="36"/>
       <c r="J10" s="36"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="38" t="s">
         <v>342</v>
       </c>
@@ -12494,13 +12497,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="38" t="s">
         <v>344</v>
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45594</v>
+        <v>45663</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -12519,7 +12522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="38" t="s">
         <v>346</v>
       </c>
@@ -12542,7 +12545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="38" t="s">
         <v>348</v>
       </c>
@@ -12568,7 +12571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="38" t="s">
         <v>350</v>
       </c>
@@ -12588,7 +12591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="38" t="s">
         <v>352</v>
       </c>
@@ -12611,7 +12614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="38" t="s">
         <v>354</v>
       </c>
@@ -12634,7 +12637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="38" t="s">
         <v>356</v>
       </c>
@@ -12657,7 +12660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="38" t="s">
         <v>358</v>
       </c>
@@ -12680,7 +12683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="38" t="s">
         <v>360</v>
       </c>
@@ -12703,7 +12706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="38" t="s">
         <v>362</v>
       </c>
@@ -12729,7 +12732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="38" t="s">
         <v>364</v>
       </c>
@@ -12755,7 +12758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="38" t="s">
         <v>366</v>
       </c>
@@ -12781,7 +12784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="G24" s="34" t="s">
         <v>368</v>
       </c>
@@ -12798,7 +12801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="38" t="s">
         <v>369</v>
       </c>
@@ -12824,7 +12827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="G26" s="34" t="s">
         <v>371</v>
       </c>
@@ -12844,7 +12847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="21" t="s">
         <v>372</v>
       </c>
@@ -12870,7 +12873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="G28" s="34" t="s">
         <v>374</v>
       </c>
@@ -12890,7 +12893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="G29" s="34" t="s">
         <v>375</v>
       </c>
@@ -12910,7 +12913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="G30" s="34" t="s">
         <v>376</v>
       </c>
@@ -12930,7 +12933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="13.5" thickBot="1">
       <c r="G31" s="35" t="s">
         <v>377</v>
       </c>
@@ -12944,7 +12947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="G32" s="34" t="s">
         <v>378</v>
       </c>
@@ -12958,7 +12961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:10">
       <c r="G33" s="34" t="s">
         <v>379</v>
       </c>
@@ -12972,7 +12975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:10">
       <c r="G34" s="34" t="s">
         <v>380</v>
       </c>
@@ -12986,7 +12989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:10">
       <c r="G35" s="34" t="s">
         <v>381</v>
       </c>
@@ -13000,7 +13003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:10">
       <c r="G36" s="34" t="s">
         <v>382</v>
       </c>
@@ -13014,7 +13017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:10">
       <c r="G37" s="34" t="s">
         <v>383</v>
       </c>
@@ -13028,110 +13031,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="7:10">
       <c r="G39" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="22" priority="58">
+    <cfRule type="expression" dxfId="40" priority="58">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="21" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="20" priority="114"/>
+    <cfRule type="aboveAverage" dxfId="38" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="19" priority="73" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="37" priority="73" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="18" priority="71">
+    <cfRule type="containsBlanks" dxfId="36" priority="71">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="17" priority="70">
+    <cfRule type="containsErrors" dxfId="35" priority="70">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="16" priority="69" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="34" priority="69" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="15" priority="67" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="33" priority="67" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="66">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="13" priority="65">
+    <cfRule type="notContainsErrors" dxfId="31" priority="65">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="12" priority="64" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="30" priority="64" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="11" priority="63" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="29" priority="63" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="10" priority="115" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="115" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="9" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="45" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="8" priority="56" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="56" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -13165,10 +13168,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="1" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="0" priority="96"/>
+    <cfRule type="uniqueValues" dxfId="18" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="44">
@@ -13596,7 +13599,7 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
@@ -13608,12 +13611,12 @@
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15">
       <c r="C3" s="17" t="s">
         <v>35</v>
       </c>
@@ -13639,7 +13642,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="C4" s="117" t="s">
         <v>42</v>
       </c>
@@ -13670,7 +13673,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="C5" s="117" t="s">
         <v>44</v>
       </c>
@@ -13701,7 +13704,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="C6" s="117" t="s">
         <v>391</v>
       </c>
@@ -13734,7 +13737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="B8" t="s">
         <v>392</v>
       </c>
@@ -13745,7 +13748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="C9">
         <v>3</v>
       </c>
@@ -13753,7 +13756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="B11" t="s">
         <v>393</v>
       </c>
@@ -13764,7 +13767,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="C12">
         <v>3</v>
       </c>
@@ -13772,7 +13775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="B14" t="s">
         <v>396</v>
       </c>
@@ -13783,7 +13786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="C15">
         <v>3</v>
       </c>
@@ -13791,7 +13794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
         <v>397</v>
       </c>
@@ -13802,7 +13805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="C18">
         <v>3</v>
       </c>
@@ -13810,7 +13813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
         <v>398</v>
       </c>
@@ -13821,7 +13824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="C21">
         <v>3</v>
       </c>
@@ -13829,7 +13832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4">
       <c r="B23" t="s">
         <v>399</v>
       </c>
@@ -13840,7 +13843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4">
       <c r="C24">
         <v>3</v>
       </c>
@@ -13848,7 +13851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4">
       <c r="B26" t="s">
         <v>400</v>
       </c>
@@ -13859,7 +13862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4">
       <c r="C27">
         <v>3</v>
       </c>
@@ -13867,7 +13870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4">
       <c r="C28" t="s">
         <v>391</v>
       </c>
@@ -13876,7 +13879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
         <v>401</v>
       </c>
@@ -13887,7 +13890,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4" hidden="1">
       <c r="C31" t="s">
         <v>404</v>
       </c>
@@ -13895,7 +13898,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4">
       <c r="C32" t="s">
         <v>405</v>
       </c>
@@ -13903,7 +13906,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
         <v>406</v>
       </c>
@@ -13933,7 +13936,7 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -13954,7 +13957,7 @@
     <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15">
       <c r="A1" s="92" t="s">
         <v>407</v>
       </c>
@@ -13964,7 +13967,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="117"/>
       <c r="B2" s="117"/>
       <c r="C2" s="117"/>
@@ -13972,7 +13975,7 @@
       <c r="E2" s="117"/>
       <c r="F2" s="117"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="117"/>
       <c r="B3" s="117"/>
       <c r="C3" s="89" t="s">
@@ -13982,7 +13985,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="117"/>
       <c r="B4" s="117"/>
       <c r="C4" s="89" t="s">
@@ -14016,7 +14019,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="117"/>
       <c r="B5" s="117"/>
       <c r="C5" s="90" t="s">
@@ -14029,7 +14032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="117"/>
       <c r="B6" s="117"/>
       <c r="C6" s="91">
@@ -14042,7 +14045,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="117"/>
       <c r="B7" s="117"/>
       <c r="C7" s="90" t="s">
@@ -14055,7 +14058,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="117"/>
       <c r="B8" s="117"/>
       <c r="C8" s="91">
@@ -14068,7 +14071,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="117"/>
       <c r="B9" s="117"/>
       <c r="C9" s="90" t="s">
@@ -14081,7 +14084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="117"/>
       <c r="B10" s="117"/>
       <c r="C10" s="91">
@@ -14094,7 +14097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="C11" s="90" t="s">
         <v>44</v>
       </c>
@@ -14105,7 +14108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="C12" s="91">
         <v>23000</v>
       </c>
@@ -14116,7 +14119,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="C13" s="90" t="s">
         <v>50</v>
       </c>
@@ -14127,7 +14130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="C14" s="91">
         <v>2</v>
       </c>
@@ -14138,7 +14141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="C15" s="90" t="s">
         <v>48</v>
       </c>
@@ -14149,7 +14152,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="C16" s="91">
         <v>50024</v>
       </c>
@@ -14160,7 +14163,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:12">
       <c r="C17" s="90" t="s">
         <v>53</v>
       </c>
@@ -14171,7 +14174,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:12">
       <c r="C18" s="91">
         <v>189576</v>
       </c>
@@ -14182,7 +14185,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:12">
       <c r="C19" s="90" t="s">
         <v>57</v>
       </c>
@@ -14193,7 +14196,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:12">
       <c r="C20" s="91">
         <v>5000</v>
       </c>
@@ -14204,7 +14207,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:12">
       <c r="C21" s="90" t="s">
         <v>411</v>
       </c>
@@ -14250,29 +14253,29 @@
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>413</v>
       </c>
       <c r="B2" s="117"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>415</v>
       </c>
@@ -14285,17 +14288,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE31E21-0350-44E7-AF13-4CA140505B30}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="51">
       <c r="A1" s="99" t="s">
         <v>416</v>
+      </c>
+      <c r="B1" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] chart: support import/export of dataset trendlines
This commit introduces the ability to import and export trendlines
associated with datasets in chart configurations.

closes odoo/o-spreadsheet#5318

Task: 4319957
Signed-off-by: Rémi Rahir (rar) <rar@odoo.com>
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28723"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ABEBB5E-CC42-4D3F-B076-13470D76BC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4533F51F-F931-45DF-A942-2AE56A765B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
   </externalReferences>
   <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3062" r:id="rId16"/>
+    <pivotCache cacheId="5712" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3117,6 +3117,22 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="4472C4"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$27:$A$35</c:f>
@@ -3660,6 +3676,19 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="1"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="ED7D31"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$27:$A$35</c:f>
@@ -5068,6 +5097,19 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="A5A5A5"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$27:$B$35</c:f>
@@ -5381,6 +5423,20 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="1"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="70AD47"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$27:$A$35</c:f>
@@ -6193,6 +6249,19 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FFC000"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:strRef>
               <c:f>Sheet1!A27:A35</c:f>
@@ -7902,7 +7971,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="3062" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="5712" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -11106,7 +11175,7 @@
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45736.475918171294</v>
+        <v>45741.742819212966</v>
       </c>
       <c r="D100" s="117">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -11796,7 +11865,7 @@
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="D144" s="117">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
@@ -12841,7 +12910,7 @@
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45741</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -14622,7 +14691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[FIX] xlsx: fix conversion of table formulas
There was some issues with our conversion of table-specific formulas:

- the keyword #ALL didn't include the table headers
- we didn't support ranges with only a keyword (eg. tableName[#ALL])
- we didn't support range with multiple parts
(eg. tableName[[#This Row],[Col1]:[Col2]])
- we didn't support ranges with multiple keywords
(eg tableName[[#Data],[#Headers], [Col1]])
- we only converted formulas that were inside of tables, but there can
be table formulas that are not in any table
- we didn't consider the case where the formula wasn't on the same
sheet as the referenced table

Task: 4095599
X-original-commit: 1c31c3932ddd896963fda29cebaf54346e2f247f
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28619"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0219CD72-FC93-4738-B246-ADCEF801BFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BC587FB-DC30-486B-B048-D0D4A1601548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,9 @@
   <externalReferences>
     <externalReference r:id="rId14"/>
   </externalReferences>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId15"/>
+    <pivotCache cacheId="834" r:id="rId15"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="423">
   <si>
     <t>CF =42</t>
   </si>
@@ -1233,6 +1233,21 @@
   </si>
   <si>
     <t>BasicTable</t>
+  </si>
+  <si>
+    <t>Total table</t>
+  </si>
+  <si>
+    <t>Column of table of other sheet</t>
+  </si>
+  <si>
+    <t>Multiple columns total</t>
+  </si>
+  <si>
+    <t>Multiple Columns</t>
+  </si>
+  <si>
+    <t>Multiple keywords</t>
   </si>
   <si>
     <t>Header</t>
@@ -1324,7 +1339,7 @@
     <numFmt numFmtId="169" formatCode="#,##0&quot; EUR €&quot;"/>
     <numFmt numFmtId="170" formatCode="&quot;€&quot;#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1481,6 +1496,12 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="28">
@@ -2014,7 +2035,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2201,7 +2222,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2214,13 +2234,238 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike/>
+        <u/>
+        <color theme="7"/>
+      </font>
+      <numFmt numFmtId="171" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="lightTrellis">
+          <fgColor theme="4"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2627,157 +2872,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike/>
-        <u/>
-        <color theme="7"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="lightTrellis">
-          <fgColor theme="4"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -2792,8 +2886,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{33B8EB55-D8D8-4B00-B5CF-C84A8AC9E775}">
-      <tableStyleElement type="wholeTable" dxfId="45"/>
-      <tableStyleElement type="firstRowStripe" dxfId="44"/>
+      <tableStyleElement type="wholeTable" dxfId="49"/>
+      <tableStyleElement type="firstRowStripe" dxfId="48"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3198,7 +3292,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3302,7 +3396,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5848,7 +5942,7 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5921,7 +6015,7 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6945,7 +7039,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="834" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7095,7 +7189,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -7107,22 +7201,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="7">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7137,6 +7231,17 @@
     <tableColumn id="2" xr3:uid="{2050F373-1538-4D53-8D8B-FBE687F1DDF5}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C86BE001-1566-49B5-98DB-0DEBDC9E0D8D}" name="Table10" displayName="Table10" ref="A7:B12" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A7:B12" xr:uid="{C86BE001-1566-49B5-98DB-0DEBDC9E0D8D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C4D15F5D-ABE4-48FC-A099-795341958524}" name="Col1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{51559469-EFF4-4F4F-91AC-5E8CB6A03BDF}" name="Col2" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -7232,9 +7337,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7272,7 +7377,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7378,7 +7483,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7520,7 +7625,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7534,7 +7639,7 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -7543,7 +7648,7 @@
     <col min="6" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1">
       <c r="A1" s="22"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -7552,7 +7657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="27.75">
       <c r="B2" s="23" t="s">
         <v>2</v>
       </c>
@@ -7565,25 +7670,25 @@
       <c r="H2" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="106"/>
+      <c r="I2" s="111"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1">
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2">
         <v>8</v>
       </c>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="107">
+      <c r="K3" s="106">
         <v>5</v>
       </c>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1">
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
@@ -7596,50 +7701,50 @@
       <c r="G4" s="2">
         <v>9</v>
       </c>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="108"/>
+      <c r="K4" s="107"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1">
       <c r="C5" s="2">
         <v>42</v>
       </c>
       <c r="G5" s="2">
         <v>15</v>
       </c>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="108"/>
+      <c r="K5" s="107"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1">
       <c r="G6" s="2">
         <v>22</v>
       </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="108"/>
+      <c r="K6" s="107"/>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1">
       <c r="C7" s="2">
         <v>3</v>
       </c>
       <c r="J7" s="6"/>
-      <c r="K7" s="108"/>
+      <c r="K7" s="107"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1">
       <c r="G8" s="2">
         <v>30</v>
       </c>
       <c r="J8" s="6"/>
-      <c r="K8" s="109"/>
+      <c r="K8" s="108"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17.25" customHeight="1">
       <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
@@ -7649,7 +7754,7 @@
       </c>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1">
       <c r="C10" s="2">
         <f>SUM(C4:C7)</f>
         <v>57.4</v>
@@ -7658,13 +7763,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17.25" customHeight="1">
       <c r="C11" s="2">
         <f>-(3+C7*SUM(C4:C7))</f>
         <v>-175.2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="17.25" customHeight="1">
       <c r="C12" s="2">
         <f>SUM(C9:C11)</f>
         <v>-63.399999999999991</v>
@@ -7673,13 +7778,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1">
       <c r="G13" s="2">
         <f>A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12+A13+A14+A15+A16+A17+A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17.25" customHeight="1">
       <c r="B14" s="12" t="s">
         <v>11</v>
       </c>
@@ -7688,32 +7793,32 @@
         <v>#CYCLE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="17.25" customHeight="1">
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="17.25" customHeight="1">
       <c r="C16" s="2" t="str">
         <f>C15</f>
         <v>=(+</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1">
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1">
       <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1">
       <c r="E19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1">
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
         <v>15</v>
@@ -7727,7 +7832,7 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>18</v>
       </c>
@@ -7737,7 +7842,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>19</v>
       </c>
@@ -7751,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1">
       <c r="C24" s="17">
         <v>10</v>
       </c>
@@ -7762,7 +7867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1">
       <c r="C25" s="17">
         <v>10.122999999999999</v>
       </c>
@@ -7773,7 +7878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1">
       <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
@@ -7787,7 +7892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -7804,7 +7909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
@@ -7821,7 +7926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
@@ -7838,7 +7943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
@@ -7855,7 +7960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
@@ -7872,7 +7977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
@@ -7889,7 +7994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="17.25" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
@@ -7906,7 +8011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="17.25" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
@@ -7917,7 +8022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="17.25" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
@@ -7934,7 +8039,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7984,7 +8089,7 @@
       <selection sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7995,13 +8100,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8015,7 +8120,7 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
@@ -8035,7 +8140,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8050,12 +8155,12 @@
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="17.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -8090,7 +8195,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -8136,7 +8241,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -8182,7 +8287,7 @@
         <v>1217.7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -8228,7 +8333,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -8274,7 +8379,7 @@
         <v>1246.7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="17.25" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -8320,7 +8425,7 @@
         <v>1213.7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="17.25" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -8354,7 +8459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="17.25" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -8388,7 +8493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="17.25" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -8419,7 +8524,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="17.25" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
@@ -8435,7 +8540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="17.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
@@ -8454,7 +8559,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="17.25" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
@@ -8485,7 +8590,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="17.25" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
@@ -8516,7 +8621,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="17.25" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>67</v>
       </c>
@@ -8532,7 +8637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="17.25" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>68</v>
       </c>
@@ -8548,7 +8653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="17.25" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>69</v>
       </c>
@@ -8564,7 +8669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
@@ -8580,7 +8685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>71</v>
       </c>
@@ -8596,7 +8701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>72</v>
       </c>
@@ -8612,7 +8717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>73</v>
       </c>
@@ -8628,7 +8733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
@@ -8644,7 +8749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>76</v>
       </c>
@@ -8660,7 +8765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>77</v>
       </c>
@@ -8676,7 +8781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="17.25" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>78</v>
       </c>
@@ -8693,7 +8798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="17.25" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>79</v>
       </c>
@@ -8709,7 +8814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="17.25" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>81</v>
       </c>
@@ -8725,7 +8830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="17.25" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>82</v>
       </c>
@@ -8741,7 +8846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="17.25" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>83</v>
       </c>
@@ -8758,7 +8863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="17.25" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>84</v>
       </c>
@@ -8774,7 +8879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17.25" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>85</v>
       </c>
@@ -8790,7 +8895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="17.25" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>86</v>
       </c>
@@ -8806,7 +8911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="17.25" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>87</v>
       </c>
@@ -8822,7 +8927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17.25" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>88</v>
       </c>
@@ -8838,7 +8943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="17.25" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>89</v>
       </c>
@@ -8854,7 +8959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17.25" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>90</v>
       </c>
@@ -8870,7 +8975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="17.25" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>91</v>
       </c>
@@ -8886,7 +8991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="17.25" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>92</v>
       </c>
@@ -8902,7 +9007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="17.25" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>93</v>
       </c>
@@ -8919,7 +9024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="17.25" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>94</v>
       </c>
@@ -8935,7 +9040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="17.25" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>95</v>
       </c>
@@ -8951,7 +9056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="17.25" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>96</v>
       </c>
@@ -8967,7 +9072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="17.25" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>97</v>
       </c>
@@ -8983,7 +9088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="17.25" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>98</v>
       </c>
@@ -8999,7 +9104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="17.25" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>99</v>
       </c>
@@ -9015,7 +9120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="17.25" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>100</v>
       </c>
@@ -9031,7 +9136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="17.25" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>101</v>
       </c>
@@ -9047,7 +9152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="17.25" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>102</v>
       </c>
@@ -9063,7 +9168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="17.25" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>103</v>
       </c>
@@ -9079,7 +9184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="17.25" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
@@ -9095,7 +9200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="17.25" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>105</v>
       </c>
@@ -9112,7 +9217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="17.25" customHeight="1">
       <c r="A51" s="2" t="s">
         <v>106</v>
       </c>
@@ -9129,7 +9234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="17.25" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>107</v>
       </c>
@@ -9145,7 +9250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1">
       <c r="A53" s="2" t="s">
         <v>108</v>
       </c>
@@ -9161,7 +9266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="17.25" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>109</v>
       </c>
@@ -9177,7 +9282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>110</v>
       </c>
@@ -9193,7 +9298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>111</v>
       </c>
@@ -9209,7 +9314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
@@ -9225,7 +9330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>113</v>
       </c>
@@ -9241,7 +9346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>114</v>
       </c>
@@ -9257,7 +9362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>115</v>
       </c>
@@ -9273,7 +9378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>116</v>
       </c>
@@ -9289,7 +9394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>117</v>
       </c>
@@ -9305,7 +9410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="17.25" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>118</v>
       </c>
@@ -9321,7 +9426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="17.25" customHeight="1">
       <c r="A64" s="2" t="s">
         <v>119</v>
       </c>
@@ -9337,7 +9442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="17.25" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>120</v>
       </c>
@@ -9353,7 +9458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="17.25" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>121</v>
       </c>
@@ -9369,7 +9474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="17.25" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>122</v>
       </c>
@@ -9385,7 +9490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="17.25" customHeight="1">
       <c r="A68" s="2" t="s">
         <v>123</v>
       </c>
@@ -9401,7 +9506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="17.25" customHeight="1">
       <c r="A69" s="2" t="s">
         <v>125</v>
       </c>
@@ -9417,7 +9522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="17.25" customHeight="1">
       <c r="A70" s="2" t="s">
         <v>127</v>
       </c>
@@ -9433,7 +9538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="17.25" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>129</v>
       </c>
@@ -9449,7 +9554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="17.25" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>130</v>
       </c>
@@ -9465,7 +9570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="17.25" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>131</v>
       </c>
@@ -9481,7 +9586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="17.25" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>132</v>
       </c>
@@ -9497,7 +9602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="17.25" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>133</v>
       </c>
@@ -9513,7 +9618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="17.25" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>134</v>
       </c>
@@ -9529,7 +9634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="17.25" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>135</v>
       </c>
@@ -9545,7 +9650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="17.25" customHeight="1">
       <c r="A78" s="2" t="s">
         <v>136</v>
       </c>
@@ -9561,7 +9666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="17.25" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>137</v>
       </c>
@@ -9577,7 +9682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="17.25" customHeight="1">
       <c r="A80" s="2" t="s">
         <v>138</v>
       </c>
@@ -9593,7 +9698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="17.25" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>139</v>
       </c>
@@ -9609,7 +9714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="17.25" customHeight="1">
       <c r="A82" s="2" t="s">
         <v>141</v>
       </c>
@@ -9625,7 +9730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="17.25" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>142</v>
       </c>
@@ -9641,7 +9746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="17.25" customHeight="1">
       <c r="A84" s="2" t="s">
         <v>143</v>
       </c>
@@ -9657,7 +9762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="17.25" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>144</v>
       </c>
@@ -9673,7 +9778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="17.25" customHeight="1">
       <c r="A86" s="2" t="s">
         <v>146</v>
       </c>
@@ -9689,7 +9794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="17.25" customHeight="1">
       <c r="A87" s="2" t="s">
         <v>147</v>
       </c>
@@ -9705,7 +9810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="17.25" customHeight="1">
       <c r="A88" s="2" t="s">
         <v>148</v>
       </c>
@@ -9721,7 +9826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="17.25" customHeight="1">
       <c r="A89" s="2" t="s">
         <v>149</v>
       </c>
@@ -9737,7 +9842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="17.25" customHeight="1">
       <c r="A90" s="2" t="s">
         <v>150</v>
       </c>
@@ -9753,7 +9858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="17.25" customHeight="1">
       <c r="A91" s="2" t="s">
         <v>151</v>
       </c>
@@ -9769,7 +9874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1">
       <c r="A92" s="2" t="s">
         <v>152</v>
       </c>
@@ -9785,7 +9890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1">
       <c r="A93" s="2" t="s">
         <v>153</v>
       </c>
@@ -9801,7 +9906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1">
       <c r="A94" s="2" t="s">
         <v>154</v>
       </c>
@@ -9817,7 +9922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1">
       <c r="A95" s="2" t="s">
         <v>155</v>
       </c>
@@ -9833,7 +9938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1">
       <c r="A96" s="2" t="s">
         <v>156</v>
       </c>
@@ -9849,7 +9954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="17.25" customHeight="1">
       <c r="A97" s="2" t="s">
         <v>157</v>
       </c>
@@ -9865,7 +9970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="17.25" customHeight="1">
       <c r="A98" s="2" t="s">
         <v>158</v>
       </c>
@@ -9881,7 +9986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="17.25" customHeight="1">
       <c r="A99" s="2" t="s">
         <v>159</v>
       </c>
@@ -9897,20 +10002,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="17.25" customHeight="1">
       <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B100" s="20">
         <f ca="1">NOW()</f>
-        <v>45643.379599189815</v>
+        <v>45715.516800810183</v>
       </c>
       <c r="D100" s="2">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="17.25" customHeight="1">
       <c r="A101" s="2" t="s">
         <v>161</v>
       </c>
@@ -9926,7 +10031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="17.25" customHeight="1">
       <c r="A102" s="2" t="s">
         <v>162</v>
       </c>
@@ -9942,7 +10047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="17.25" customHeight="1">
       <c r="A103" s="2" t="s">
         <v>163</v>
       </c>
@@ -9958,7 +10063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="17.25" customHeight="1">
       <c r="A104" s="2" t="s">
         <v>164</v>
       </c>
@@ -9974,7 +10079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="17.25" customHeight="1">
       <c r="A105" s="2" t="s">
         <v>165</v>
       </c>
@@ -9990,7 +10095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="17.25" customHeight="1">
       <c r="A106" s="2" t="s">
         <v>166</v>
       </c>
@@ -10006,7 +10111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="17.25" customHeight="1">
       <c r="A107" s="2" t="s">
         <v>167</v>
       </c>
@@ -10022,7 +10127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="17.25" customHeight="1">
       <c r="A108" s="2" t="s">
         <v>168</v>
       </c>
@@ -10038,7 +10143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="17.25" customHeight="1">
       <c r="A109" s="2" t="s">
         <v>169</v>
       </c>
@@ -10054,7 +10159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="17.25" customHeight="1">
       <c r="A110" s="2" t="s">
         <v>170</v>
       </c>
@@ -10070,7 +10175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="17.25" customHeight="1">
       <c r="A111" s="2" t="s">
         <v>171</v>
       </c>
@@ -10086,12 +10191,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="17.25" customHeight="1">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="17.25" customHeight="1">
       <c r="A113" s="2" t="s">
         <v>172</v>
       </c>
@@ -10107,7 +10212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="17.25" customHeight="1">
       <c r="A114" s="2" t="s">
         <v>173</v>
       </c>
@@ -10123,7 +10228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="17.25" customHeight="1">
       <c r="A115" s="2" t="s">
         <v>175</v>
       </c>
@@ -10139,7 +10244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="17.25" customHeight="1">
       <c r="A116" s="2" t="s">
         <v>177</v>
       </c>
@@ -10155,7 +10260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="17.25" customHeight="1">
       <c r="A117" s="2" t="s">
         <v>178</v>
       </c>
@@ -10171,7 +10276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="17.25" customHeight="1">
       <c r="A118" s="2" t="s">
         <v>179</v>
       </c>
@@ -10187,7 +10292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="17.25" customHeight="1">
       <c r="A119" s="2" t="s">
         <v>180</v>
       </c>
@@ -10203,7 +10308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="17.25" customHeight="1">
       <c r="A120" s="2" t="s">
         <v>181</v>
       </c>
@@ -10219,7 +10324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="17.25" customHeight="1">
       <c r="A121" s="2" t="s">
         <v>182</v>
       </c>
@@ -10235,7 +10340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="17.25" customHeight="1">
       <c r="A122" s="2" t="s">
         <v>183</v>
       </c>
@@ -10251,7 +10356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="17.25" customHeight="1">
       <c r="A123" s="2" t="s">
         <v>184</v>
       </c>
@@ -10267,7 +10372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="17.25" customHeight="1">
       <c r="A124" s="2" t="s">
         <v>185</v>
       </c>
@@ -10283,7 +10388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="17.25" customHeight="1">
       <c r="A125" s="2" t="s">
         <v>186</v>
       </c>
@@ -10299,7 +10404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="17.25" customHeight="1">
       <c r="A126" s="2" t="s">
         <v>187</v>
       </c>
@@ -10315,7 +10420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="17.25" customHeight="1">
       <c r="A127" s="2" t="s">
         <v>188</v>
       </c>
@@ -10331,7 +10436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="17.25" customHeight="1">
       <c r="A128" s="2" t="s">
         <v>189</v>
       </c>
@@ -10347,7 +10452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="17.25" customHeight="1">
       <c r="A129" s="2" t="s">
         <v>190</v>
       </c>
@@ -10363,7 +10468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="17.25" customHeight="1">
       <c r="A130" s="2" t="s">
         <v>191</v>
       </c>
@@ -10379,7 +10484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="17.25" customHeight="1">
       <c r="A131" s="2" t="s">
         <v>192</v>
       </c>
@@ -10395,7 +10500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="17.25" customHeight="1">
       <c r="A132" s="2" t="s">
         <v>193</v>
       </c>
@@ -10411,7 +10516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="17.25" customHeight="1">
       <c r="A133" s="2" t="s">
         <v>194</v>
       </c>
@@ -10427,7 +10532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="17.25" customHeight="1">
       <c r="A134" s="2" t="s">
         <v>195</v>
       </c>
@@ -10443,7 +10548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="17.25" customHeight="1">
       <c r="A135" s="2" t="s">
         <v>196</v>
       </c>
@@ -10459,7 +10564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="17.25" customHeight="1">
       <c r="A136" s="2" t="s">
         <v>198</v>
       </c>
@@ -10475,7 +10580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="17.25" customHeight="1">
       <c r="A137" s="2" t="s">
         <v>199</v>
       </c>
@@ -10491,7 +10596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="17.25" customHeight="1">
       <c r="A138" s="2" t="s">
         <v>200</v>
       </c>
@@ -10507,7 +10612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="17.25" customHeight="1">
       <c r="A139" s="2" t="s">
         <v>201</v>
       </c>
@@ -10523,7 +10628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="17.25" customHeight="1">
       <c r="A140" s="2" t="s">
         <v>202</v>
       </c>
@@ -10539,7 +10644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="17.25" customHeight="1">
       <c r="A141" s="2" t="s">
         <v>203</v>
       </c>
@@ -10555,7 +10660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="17.25" customHeight="1">
       <c r="A142" s="2" t="s">
         <v>205</v>
       </c>
@@ -10571,7 +10676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="17.25" customHeight="1">
       <c r="A143" s="2" t="s">
         <v>206</v>
       </c>
@@ -10587,20 +10692,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="17.25" customHeight="1">
       <c r="A144" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B144" s="19">
         <f ca="1">TODAY()</f>
-        <v>45643</v>
+        <v>45715</v>
       </c>
       <c r="D144" s="2">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="17.25" customHeight="1">
       <c r="A145" s="2" t="s">
         <v>208</v>
       </c>
@@ -10616,7 +10721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="17.25" customHeight="1">
       <c r="A146" s="2" t="s">
         <v>210</v>
       </c>
@@ -10632,7 +10737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="17.25" customHeight="1">
       <c r="A147" s="2" t="s">
         <v>211</v>
       </c>
@@ -10648,7 +10753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="17.25" customHeight="1">
       <c r="A148" s="2" t="s">
         <v>213</v>
       </c>
@@ -10664,7 +10769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="17.25" customHeight="1">
       <c r="A149" s="2" t="s">
         <v>214</v>
       </c>
@@ -10680,7 +10785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" ht="17.25" customHeight="1">
       <c r="A150" s="2" t="s">
         <v>215</v>
       </c>
@@ -10696,7 +10801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="17.25" customHeight="1">
       <c r="A151" s="2" t="s">
         <v>216</v>
       </c>
@@ -10712,7 +10817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="17.25" customHeight="1">
       <c r="A152" s="2" t="s">
         <v>217</v>
       </c>
@@ -10728,7 +10833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="17.25" customHeight="1">
       <c r="A153" s="2" t="s">
         <v>218</v>
       </c>
@@ -10744,7 +10849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" ht="17.25" customHeight="1">
       <c r="A154" s="2" t="s">
         <v>219</v>
       </c>
@@ -10761,7 +10866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="17.25" customHeight="1">
       <c r="A155" s="2" t="s">
         <v>220</v>
       </c>
@@ -10777,7 +10882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="17.25" customHeight="1">
       <c r="A156" s="2" t="s">
         <v>221</v>
       </c>
@@ -10793,7 +10898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" ht="17.25" customHeight="1">
       <c r="A157" s="2" t="s">
         <v>222</v>
       </c>
@@ -10809,7 +10914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" ht="17.25" customHeight="1">
       <c r="A158" s="2" t="s">
         <v>223</v>
       </c>
@@ -10825,7 +10930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="17.25" customHeight="1">
       <c r="A159" s="2" t="s">
         <v>224</v>
       </c>
@@ -10841,7 +10946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" ht="17.25" customHeight="1">
       <c r="A160" s="2" t="s">
         <v>225</v>
       </c>
@@ -10857,7 +10962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" ht="17.25" customHeight="1">
       <c r="A161" s="2" t="s">
         <v>226</v>
       </c>
@@ -10873,7 +10978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="17.25" customHeight="1">
       <c r="A162" s="2" t="s">
         <v>227</v>
       </c>
@@ -10889,7 +10994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" ht="17.25" customHeight="1">
       <c r="A163" s="2" t="s">
         <v>229</v>
       </c>
@@ -10907,10 +11012,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10929,7 +11034,7 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
@@ -10939,17 +11044,17 @@
     <col min="15" max="18" width="9.140625" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>230</v>
       </c>
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="110" t="s">
+      <c r="D1" s="109" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="110"/>
+      <c r="E1" s="109"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -10957,19 +11062,19 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="D3" s="86" t="s">
         <v>235</v>
       </c>
@@ -10977,25 +11082,25 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="75" customHeight="1">
       <c r="A5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="17" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="18" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:8" outlineLevel="1"/>
+    <row r="11" spans="1:8" outlineLevel="1"/>
+    <row r="12" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="13" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="14" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="15" spans="1:8" outlineLevel="1" collapsed="1"/>
+    <row r="16" spans="1:8" outlineLevel="1"/>
+    <row r="17" outlineLevel="1"/>
+    <row r="18" outlineLevel="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:E2"/>
@@ -11017,14 +11122,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1">
       <c r="A1" s="69" t="s">
         <v>239</v>
       </c>
@@ -11046,7 +11151,7 @@
       </c>
       <c r="M1" s="37"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="41" t="s">
         <v>245</v>
       </c>
@@ -11072,7 +11177,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="42" t="s">
         <v>252</v>
       </c>
@@ -11095,7 +11200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15">
       <c r="A4" s="43" t="s">
         <v>256</v>
       </c>
@@ -11121,7 +11226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="44" t="s">
         <v>262</v>
       </c>
@@ -11141,7 +11246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="45" t="s">
         <v>266</v>
       </c>
@@ -11164,7 +11269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="46" t="s">
         <v>271</v>
       </c>
@@ -11184,7 +11289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="21">
       <c r="A8" s="47" t="s">
         <v>275</v>
       </c>
@@ -11207,7 +11312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="48" t="s">
         <v>280</v>
       </c>
@@ -11224,7 +11329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="49" t="s">
         <v>283</v>
       </c>
@@ -11232,7 +11337,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1">
       <c r="A11" s="50" t="s">
         <v>285</v>
       </c>
@@ -11241,7 +11346,7 @@
       </c>
       <c r="F11" s="37"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1">
       <c r="A12" s="51" t="s">
         <v>287</v>
       </c>
@@ -11255,7 +11360,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A13" s="52" t="s">
         <v>290</v>
       </c>
@@ -11266,7 +11371,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A14" s="53" t="s">
         <v>291</v>
       </c>
@@ -11280,7 +11385,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A15" s="54" t="s">
         <v>293</v>
       </c>
@@ -11291,7 +11396,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
       <c r="A16" s="55" t="s">
         <v>294</v>
       </c>
@@ -11305,12 +11410,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.5" thickBot="1">
       <c r="A17" s="56" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.5" thickBot="1">
       <c r="A18" s="75" t="s">
         <v>297</v>
       </c>
@@ -11322,7 +11427,7 @@
       </c>
       <c r="F18" s="37"/>
     </row>
-    <row r="19" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13.5" thickBot="1">
       <c r="A19" s="76" t="s">
         <v>300</v>
       </c>
@@ -11333,7 +11438,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="51.75" thickBot="1">
       <c r="A20" s="77" t="s">
         <v>303</v>
       </c>
@@ -11347,12 +11452,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.5" thickBot="1">
       <c r="A21" s="78" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.5" thickBot="1">
       <c r="A22" s="79" t="s">
         <v>307</v>
       </c>
@@ -11361,13 +11466,13 @@
       </c>
       <c r="E22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.5" thickBot="1">
       <c r="A23" s="80" t="s">
         <v>309</v>
       </c>
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="A24" s="81" t="s">
         <v>310</v>
       </c>
@@ -11376,20 +11481,20 @@
       </c>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C26" s="68" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C28" s="89" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="13.5" thickTop="1"/>
+    <row r="30" spans="1:6">
       <c r="C30" s="88" t="s">
         <v>314</v>
       </c>
@@ -11408,13 +11513,13 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.5" thickBot="1">
       <c r="A1" s="38" t="s">
         <v>315</v>
       </c>
@@ -11431,7 +11536,7 @@
       <c r="I1" s="37"/>
       <c r="J1" s="37"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="39" t="s">
         <v>319</v>
       </c>
@@ -11454,7 +11559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="39" t="s">
         <v>321</v>
       </c>
@@ -11477,7 +11582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="39" t="s">
         <v>325</v>
       </c>
@@ -11497,7 +11602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="39" t="s">
         <v>328</v>
       </c>
@@ -11521,7 +11626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="39" t="s">
         <v>330</v>
       </c>
@@ -11544,7 +11649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="39" t="s">
         <v>333</v>
       </c>
@@ -11570,7 +11675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="39" t="s">
         <v>337</v>
       </c>
@@ -11581,7 +11686,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="39" t="s">
         <v>339</v>
       </c>
@@ -11590,7 +11695,7 @@
       </c>
       <c r="C9" s="22"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.5" thickBot="1">
       <c r="A10" s="39" t="s">
         <v>340</v>
       </c>
@@ -11608,7 +11713,7 @@
       <c r="I10" s="37"/>
       <c r="J10" s="37"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="39" t="s">
         <v>342</v>
       </c>
@@ -11631,13 +11736,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="39" t="s">
         <v>344</v>
       </c>
       <c r="B12" s="40">
         <f ca="1">TODAY()</f>
-        <v>45643</v>
+        <v>45715</v>
       </c>
       <c r="C12" s="40">
         <f>DATE(2010,10,2)</f>
@@ -11656,7 +11761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="39" t="s">
         <v>346</v>
       </c>
@@ -11679,7 +11784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="39" t="s">
         <v>348</v>
       </c>
@@ -11705,7 +11810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="39" t="s">
         <v>350</v>
       </c>
@@ -11725,7 +11830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="39" t="s">
         <v>352</v>
       </c>
@@ -11748,7 +11853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="39" t="s">
         <v>354</v>
       </c>
@@ -11771,7 +11876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="39" t="s">
         <v>356</v>
       </c>
@@ -11794,7 +11899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="39" t="s">
         <v>358</v>
       </c>
@@ -11817,7 +11922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="39" t="s">
         <v>360</v>
       </c>
@@ -11840,7 +11945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="39" t="s">
         <v>362</v>
       </c>
@@ -11866,7 +11971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="39" t="s">
         <v>364</v>
       </c>
@@ -11892,7 +11997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="39" t="s">
         <v>366</v>
       </c>
@@ -11918,7 +12023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="G24" s="35" t="s">
         <v>368</v>
       </c>
@@ -11935,7 +12040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="39" t="s">
         <v>369</v>
       </c>
@@ -11961,7 +12066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="G26" s="35" t="s">
         <v>371</v>
       </c>
@@ -11981,7 +12086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="22" t="s">
         <v>372</v>
       </c>
@@ -12007,7 +12112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="G28" s="35" t="s">
         <v>374</v>
       </c>
@@ -12027,7 +12132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="G29" s="35" t="s">
         <v>375</v>
       </c>
@@ -12047,7 +12152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="G30" s="35" t="s">
         <v>376</v>
       </c>
@@ -12067,7 +12172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="13.5" thickBot="1">
       <c r="G31" s="36" t="s">
         <v>377</v>
       </c>
@@ -12081,7 +12186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="G32" s="35" t="s">
         <v>378</v>
       </c>
@@ -12095,7 +12200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:10">
       <c r="G33" s="35" t="s">
         <v>379</v>
       </c>
@@ -12109,7 +12214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:10">
       <c r="G34" s="35" t="s">
         <v>380</v>
       </c>
@@ -12123,7 +12228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:10">
       <c r="G35" s="35" t="s">
         <v>381</v>
       </c>
@@ -12137,7 +12242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:10">
       <c r="G36" s="35" t="s">
         <v>382</v>
       </c>
@@ -12151,7 +12256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:10">
       <c r="G37" s="35" t="s">
         <v>383</v>
       </c>
@@ -12165,110 +12270,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="7:10">
       <c r="G39" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="22" priority="58">
+    <cfRule type="expression" dxfId="44" priority="58">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="21" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="20" priority="114"/>
+    <cfRule type="aboveAverage" dxfId="42" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="19" priority="73" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="41" priority="73" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="18" priority="71">
+    <cfRule type="containsBlanks" dxfId="40" priority="71">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="17" priority="70">
+    <cfRule type="containsErrors" dxfId="39" priority="70">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="16" priority="69" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="38" priority="69" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="15" priority="67" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="37" priority="67" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="66">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="13" priority="65">
+    <cfRule type="notContainsErrors" dxfId="35" priority="65">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="12" priority="64" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="34" priority="64" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="11" priority="63" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="33" priority="63" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="10" priority="115" rank="1"/>
+    <cfRule type="top10" dxfId="32" priority="115" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="9" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="45" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="8" priority="56" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="56" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -12302,10 +12407,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="1" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="0" priority="96"/>
+    <cfRule type="uniqueValues" dxfId="22" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="44">
@@ -12729,11 +12834,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CCC4B1-5C65-4837-AA26-56CCF06B63BB}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
@@ -12745,12 +12850,12 @@
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15">
       <c r="C3" s="18" t="s">
         <v>35</v>
       </c>
@@ -12776,7 +12881,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
         <v>42</v>
       </c>
@@ -12807,7 +12912,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
@@ -12838,7 +12943,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
         <v>391</v>
       </c>
@@ -12871,7 +12976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="B8" t="s">
         <v>392</v>
       </c>
@@ -12881,27 +12986,62 @@
       <c r="D8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>393</v>
+      </c>
+      <c r="G8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H8" t="s">
+        <v>395</v>
+      </c>
+      <c r="I8" t="s">
+        <v>396</v>
+      </c>
+      <c r="J8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f>SUM(Table3[#All])</f>
+        <v>396</v>
+      </c>
+      <c r="G9">
+        <f>SUM(Table10[Col2])</f>
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <f>SUM(Table3[[#Totals],[Age]:[Rank]])</f>
+        <v>51</v>
+      </c>
+      <c r="I9">
+        <f>SUM(Table3[[Age]:[Rank]])</f>
+        <v>51</v>
+      </c>
+      <c r="J9">
+        <f>SUM(Table3[[#Data],[#Totals],[Rank]])</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="C11" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="D11" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="C12">
         <v>3</v>
       </c>
@@ -12909,9 +13049,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="B14" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -12920,7 +13060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="C15">
         <v>3</v>
       </c>
@@ -12928,9 +13068,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -12939,7 +13079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="C18">
         <v>3</v>
       </c>
@@ -12947,9 +13087,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -12958,7 +13098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="C21">
         <v>3</v>
       </c>
@@ -12966,9 +13106,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -12977,7 +13117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4">
       <c r="C24">
         <v>3</v>
       </c>
@@ -12985,9 +13125,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -12996,7 +13136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4">
       <c r="C27">
         <v>3</v>
       </c>
@@ -13004,7 +13144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4">
       <c r="C28" t="s">
         <v>391</v>
       </c>
@@ -13013,36 +13153,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="C30" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="D30" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" hidden="1">
       <c r="C31" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="D31" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
       <c r="C32" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="D32" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -13070,7 +13210,7 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -13091,9 +13231,9 @@
     <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15">
       <c r="A1" s="93" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -13101,7 +13241,7 @@
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -13109,21 +13249,21 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="90" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="D3" s="90" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="90" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="D4">
         <v>12.1</v>
@@ -13150,10 +13290,10 @@
         <v>12052</v>
       </c>
       <c r="L4" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="91" t="s">
@@ -13166,7 +13306,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="92">
@@ -13179,7 +13319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="91" t="s">
@@ -13192,7 +13332,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="92">
@@ -13205,7 +13345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="91" t="s">
@@ -13218,7 +13358,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="92">
@@ -13231,7 +13371,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="C11" s="91" t="s">
         <v>44</v>
       </c>
@@ -13242,7 +13382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="C12" s="92">
         <v>23000</v>
       </c>
@@ -13253,7 +13393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="C13" s="91" t="s">
         <v>50</v>
       </c>
@@ -13264,7 +13404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="C14" s="92">
         <v>2</v>
       </c>
@@ -13275,7 +13415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="C15" s="91" t="s">
         <v>48</v>
       </c>
@@ -13286,7 +13426,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="C16" s="92">
         <v>50024</v>
       </c>
@@ -13297,7 +13437,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:12">
       <c r="C17" s="91" t="s">
         <v>53</v>
       </c>
@@ -13308,7 +13448,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:12">
       <c r="C18" s="92">
         <v>189576</v>
       </c>
@@ -13319,7 +13459,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:12">
       <c r="C19" s="91" t="s">
         <v>57</v>
       </c>
@@ -13330,7 +13470,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:12">
       <c r="C20" s="92">
         <v>5000</v>
       </c>
@@ -13341,9 +13481,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:12">
       <c r="C21" s="91" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="D21">
         <v>9</v>
@@ -13387,31 +13527,31 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -13422,23 +13562,74 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE31E21-0350-44E7-AF13-4CA140505B30}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="38.25">
       <c r="A1" s="100" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B1" t="s">
-        <v>417</v>
+        <v>422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="110" t="s">
+        <v>407</v>
+      </c>
+      <c r="B7" s="110" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="110">
+        <v>1</v>
+      </c>
+      <c r="B8" s="110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="110">
+        <v>2</v>
+      </c>
+      <c r="B9" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="110">
+        <v>3</v>
+      </c>
+      <c r="B10" s="110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="110">
+        <v>4</v>
+      </c>
+      <c r="B11" s="110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="110">
+        <v>5</v>
+      </c>
+      <c r="B12" s="110">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[IMP] chart: allow multiples labels
Task Description

This PR aims to allow the usage of multiple ranges for a chart
labels. This is a necessary step to have a full compatibility
to the new treemap chart when switch from chart type, as well
as a good way to "categorize" the labels with, for example, the
first label ranges being the main category ("Art", "Sciences", ...)
and the second label being the real label ("Math", "Chemistry",
"Drawing", "Theatre", ...).

Related Task

Task: 4460827
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{157AC437-DB84-431C-BDD0-6A0421B0B149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A172513-7452-45A7-99A7-2C64F618926D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23295" yWindow="195" windowWidth="21600" windowHeight="11385" firstSheet="13" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23295" yWindow="195" windowWidth="21600" windowHeight="11385" firstSheet="8" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
   </externalReferences>
   <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3563" r:id="rId16"/>
+    <pivotCache cacheId="2082" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2375,6 +2375,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2387,10 +2388,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
@@ -2417,7 +2417,7 @@
         <u/>
         <color theme="7"/>
       </font>
-      <numFmt numFmtId="170" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="lightTrellis">
           <fgColor theme="4"/>
@@ -2995,7 +2995,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3103,39 +3103,61 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$27:$A$35</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$G$2:$G$10,Sheet1!$A$27:$A$35</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Emily Anderson (Emmy)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sophie Allen (Saffi)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Chloe Adams</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Megan Alexander (Meg)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Lucy Arnold (Lulu)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Hannah Alvarez</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Jessica Alcock (Jess)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Charlotte Anaya</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Lauren Anthony</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Emily Anderson (Emmy)</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Sophie Allen (Saffi)</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Chloe Adams</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Megan Alexander (Meg)</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Lucy Arnold (Lulu)</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Hannah Alvarez</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Jessica Alcock (Jess)</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Charlotte Anaya</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Lauren Anthony</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>22</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>30</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3222,39 +3244,61 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$27:$A$35</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$G$2:$G$10,Sheet1!$A$27:$A$35</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Emily Anderson (Emmy)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sophie Allen (Saffi)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Chloe Adams</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Megan Alexander (Meg)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Lucy Arnold (Lulu)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Hannah Alvarez</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Jessica Alcock (Jess)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Charlotte Anaya</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Lauren Anthony</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Emily Anderson (Emmy)</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Sophie Allen (Saffi)</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Chloe Adams</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Megan Alexander (Meg)</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Lucy Arnold (Lulu)</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Hannah Alvarez</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Jessica Alcock (Jess)</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Charlotte Anaya</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Lauren Anthony</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>22</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>30</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3596,7 +3640,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -4028,7 +4072,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -4646,7 +4690,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5012,7 +5056,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -5311,7 +5355,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5747,7 +5791,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6149,7 +6193,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -7575,7 +7619,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="3563" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="2082" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -8164,7 +8208,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
@@ -8198,7 +8242,7 @@
       <c r="H2" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="123"/>
+      <c r="I2" s="119"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="17.25" customHeight="1">
@@ -8208,10 +8252,10 @@
       <c r="G3" s="117">
         <v>8</v>
       </c>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="119"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="119">
+      <c r="K3" s="120">
         <v>5</v>
       </c>
       <c r="L3" s="6"/>
@@ -8229,10 +8273,10 @@
       <c r="G4" s="117">
         <v>9</v>
       </c>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="120"/>
+      <c r="K4" s="121"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="17.25" customHeight="1">
@@ -8242,10 +8286,10 @@
       <c r="G5" s="117">
         <v>15</v>
       </c>
-      <c r="H5" s="123"/>
-      <c r="I5" s="123"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="120"/>
+      <c r="K5" s="121"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" ht="17.25" customHeight="1">
@@ -8253,7 +8297,7 @@
         <v>22</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="120"/>
+      <c r="K6" s="121"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="17.25" customHeight="1">
@@ -8261,7 +8305,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="120"/>
+      <c r="K7" s="121"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="17.25" customHeight="1">
@@ -8269,7 +8313,7 @@
         <v>30</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="121"/>
+      <c r="K8" s="122"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="17.25" customHeight="1">
@@ -8911,7 +8955,7 @@
   </sheetPr>
   <dimension ref="A1:R163"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
@@ -10768,7 +10812,7 @@
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45663.51402037037</v>
+        <v>45691.340992476849</v>
       </c>
       <c r="D100" s="117">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -11458,7 +11502,7 @@
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45663</v>
+        <v>45691</v>
       </c>
       <c r="D144" s="117">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
@@ -11812,10 +11856,10 @@
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="122" t="s">
+      <c r="D1" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="122"/>
+      <c r="E1" s="123"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -11828,8 +11872,8 @@
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
@@ -12503,7 +12547,7 @@
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45663</v>
+        <v>45691</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -14249,7 +14293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
@@ -14290,7 +14334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE31E21-0350-44E7-AF13-4CA140505B30}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[FIX] xlsx: correctly import labels from scatter charts
When importing an XLSX file containing a scatter chart with textual labels, the labels were
not imported correctly. Instead, the actual range was used as labels by default, leading to
incorrect visualization.

Steps to reproduce:
    1. Create an Excel file
    2.Insert a scatter chart with textual labels.
    3. Export the file as XLSX.
    4. Import the file into o-spreadsheet.
    5. The labels are not imported; instead, the data range is incorrectly used as labels.

Unlike MS Excel’s behavior, this commit fixes the issue by taking the textual labels of
scatter charts into account, without necessarily converting them to numerical labels.

closes odoo/o-spreadsheet#5884

Task: 4626572
X-original-commit: c983748dda11d36e629dbff75113685e5fe7648d
Signed-off-by: Adrien Minne (adrm) <adrm@odoo.com>
Signed-off-by: Mehdi Rachico (mera) <mera@odoo.com>
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28706"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F15F33D-0A5F-4E8A-8973-B5E6D3A30B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C3FAEF4-9495-4537-B722-A5A16F9D6A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,9 @@
   <externalReferences>
     <externalReference r:id="rId15"/>
   </externalReferences>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId16"/>
+    <pivotCache cacheId="5972" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1236,6 +1236,21 @@
     <t>BasicTable</t>
   </si>
   <si>
+    <t>Total table</t>
+  </si>
+  <si>
+    <t>Column of table of other sheet</t>
+  </si>
+  <si>
+    <t>Multiple columns total</t>
+  </si>
+  <si>
+    <t>Multiple Columns</t>
+  </si>
+  <si>
+    <t>Multiple keywords</t>
+  </si>
+  <si>
     <t>Header</t>
   </si>
   <si>
@@ -1361,21 +1376,6 @@
   </si>
   <si>
     <t>A1234556</t>
-  </si>
-  <si>
-    <t>Total table</t>
-  </si>
-  <si>
-    <t>Column of table of other sheet</t>
-  </si>
-  <si>
-    <t>Multiple columns total</t>
-  </si>
-  <si>
-    <t>Multiple Columns</t>
-  </si>
-  <si>
-    <t>Multiple keywords</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1390,7 @@
     <numFmt numFmtId="168" formatCode="#,##0&quot; EUR €&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;€&quot;#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2390,7 +2390,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2403,6 +2402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2410,6 +2410,157 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
   <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike/>
+        <u/>
+        <color theme="7"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="lightTrellis">
+          <fgColor theme="4"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2816,157 +2967,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike/>
-        <u/>
-        <color theme="7"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="lightTrellis">
-          <fgColor theme="4"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -6162,6 +6162,311 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2200"/>
+              <a:t>scatter chart with textual labels</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!A27:A35</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Emily Anderson (Emmy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sophie Allen (Saffi)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chloe Adams</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Megan Alexander (Meg)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lucy Arnold (Lulu)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hannah Alvarez</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jessica Alcock (Jess)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Charlotte Anaya</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lauren Anthony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D820-45B8-B7E8-F475A1A65785}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="17781237"/>
+        <c:axId val="88853993"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="17781237"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="1"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1000" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88853993"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="88853993"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="1"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1000" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17781237"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr sz="1000" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln cmpd="sng">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7331,6 +7636,47 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D2716A1-A175-44F9-BBD0-26D27F88F15C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E2B20B98-FA84-44C9-8DBB-5852658E9967}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7590,7 +7936,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="5972" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -7740,7 +8086,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -7752,22 +8098,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="7">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7888,9 +8234,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7928,7 +8274,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8034,7 +8380,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8176,7 +8522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8193,7 +8539,7 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -8202,7 +8548,7 @@
     <col min="6" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1">
       <c r="A1" s="21"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -8211,7 +8557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="27.75">
       <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
@@ -8224,25 +8570,25 @@
       <c r="H2" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="119"/>
+      <c r="I2" s="123"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1">
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="117">
         <v>8</v>
       </c>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="120">
+      <c r="K3" s="119">
         <v>5</v>
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -8255,50 +8601,50 @@
       <c r="G4" s="117">
         <v>9</v>
       </c>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="121"/>
+      <c r="K4" s="120"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1">
       <c r="C5" s="117">
         <v>42</v>
       </c>
       <c r="G5" s="117">
         <v>15</v>
       </c>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="121"/>
+      <c r="K5" s="120"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1">
       <c r="G6" s="117">
         <v>22</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="121"/>
+      <c r="K6" s="120"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1">
       <c r="C7" s="117">
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="121"/>
+      <c r="K7" s="120"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1">
       <c r="G8" s="117">
         <v>30</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="122"/>
+      <c r="K8" s="121"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17.25" customHeight="1">
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
@@ -8308,7 +8654,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1">
       <c r="C10" s="117">
         <f>SUM(C4:C7)</f>
         <v>57.4</v>
@@ -8317,13 +8663,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17.25" customHeight="1">
       <c r="C11" s="117">
         <f>-(3+C7*SUM(C4:C7))</f>
         <v>-175.2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="17.25" customHeight="1">
       <c r="C12" s="117">
         <f>SUM(C9:C11)</f>
         <v>-63.399999999999991</v>
@@ -8332,13 +8678,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1">
       <c r="G13" s="117">
         <f>A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12+A13+A14+A15+A16+A17+A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17.25" customHeight="1">
       <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
@@ -8347,32 +8693,32 @@
         <v>#CYCLE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="17.25" customHeight="1">
       <c r="C15" s="117" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="17.25" customHeight="1">
       <c r="C16" s="117" t="str">
         <f>C15</f>
         <v>=(+</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1">
       <c r="C17" s="117" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1">
       <c r="C18" s="117" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1">
       <c r="E19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
         <v>15</v>
@@ -8386,7 +8732,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -8396,7 +8742,7 @@
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1">
       <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
@@ -8410,7 +8756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1">
       <c r="C24" s="16">
         <v>10</v>
       </c>
@@ -8421,7 +8767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1">
       <c r="C25" s="16">
         <v>10.122999999999999</v>
       </c>
@@ -8432,7 +8778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1">
       <c r="B26" s="117" t="s">
         <v>20</v>
       </c>
@@ -8446,7 +8792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1">
       <c r="A27" s="117" t="s">
         <v>22</v>
       </c>
@@ -8463,7 +8809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1">
       <c r="A28" s="117" t="s">
         <v>23</v>
       </c>
@@ -8480,7 +8826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1">
       <c r="A29" s="117" t="s">
         <v>24</v>
       </c>
@@ -8497,7 +8843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1">
       <c r="A30" s="117" t="s">
         <v>25</v>
       </c>
@@ -8514,7 +8860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1">
       <c r="A31" s="117" t="s">
         <v>26</v>
       </c>
@@ -8531,7 +8877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1">
       <c r="A32" s="117" t="s">
         <v>27</v>
       </c>
@@ -8548,7 +8894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="17.25" customHeight="1">
       <c r="A33" s="117" t="s">
         <v>28</v>
       </c>
@@ -8565,7 +8911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="17.25" customHeight="1">
       <c r="A34" s="117" t="s">
         <v>29</v>
       </c>
@@ -8576,7 +8922,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="17.25" customHeight="1">
       <c r="A35" s="117" t="s">
         <v>30</v>
       </c>
@@ -8593,7 +8939,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8643,7 +8989,7 @@
       <selection sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8655,12 +9001,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8674,7 +9020,7 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
@@ -8694,7 +9040,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8709,7 +9055,7 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
@@ -8718,36 +9064,36 @@
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="114" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B1" s="115" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="C1" s="115" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="D1" s="115" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="E1" s="115" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="F1" s="115" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="G1" s="115" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="H1" s="115" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="I1" s="116" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="104">
         <v>4</v>
       </c>
@@ -8758,7 +9104,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="105" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="E2" s="106">
         <v>45575</v>
@@ -8767,7 +9113,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G2" s="107" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="H2" s="106">
         <v>45292</v>
@@ -8776,7 +9122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="104">
         <v>3</v>
       </c>
@@ -8787,7 +9133,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="105" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="E3" s="106">
         <v>45576</v>
@@ -8796,16 +9142,16 @@
         <v>0.57638888888888884</v>
       </c>
       <c r="G3" s="107" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="H3" s="106">
         <v>45231</v>
       </c>
       <c r="I3" s="108" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="104">
         <v>9</v>
       </c>
@@ -8816,7 +9162,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="105" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="E4" s="106">
         <v>45574</v>
@@ -8825,7 +9171,7 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="G4" s="107" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="H4" s="106">
         <v>45325</v>
@@ -8834,7 +9180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="104">
         <v>5</v>
       </c>
@@ -8845,7 +9191,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="105" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="E5" s="106">
         <v>45573</v>
@@ -8854,7 +9200,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="G5" s="105" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="H5" s="106">
         <v>45084</v>
@@ -8863,7 +9209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="109">
         <v>7</v>
       </c>
@@ -8874,7 +9220,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="110" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="E6" s="111">
         <v>45566</v>
@@ -8883,13 +9229,13 @@
         <v>0.5229166666666667</v>
       </c>
       <c r="G6" s="110" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="H6" s="111">
         <v>45420</v>
       </c>
       <c r="I6" s="113" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -8941,12 +9287,12 @@
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="17.25" customHeight="1">
       <c r="A1" s="117" t="s">
         <v>31</v>
       </c>
@@ -8981,7 +9327,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1">
       <c r="A2" s="117" t="s">
         <v>41</v>
       </c>
@@ -9027,7 +9373,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1">
       <c r="A3" s="117" t="s">
         <v>43</v>
       </c>
@@ -9073,7 +9419,7 @@
         <v>1217.7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="17.25" customHeight="1">
       <c r="A4" s="117" t="s">
         <v>45</v>
       </c>
@@ -9119,7 +9465,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1">
       <c r="A5" s="117" t="s">
         <v>47</v>
       </c>
@@ -9165,7 +9511,7 @@
         <v>1246.7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="17.25" customHeight="1">
       <c r="A6" s="117" t="s">
         <v>49</v>
       </c>
@@ -9211,7 +9557,7 @@
         <v>1213.7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="17.25" customHeight="1">
       <c r="A7" s="117" t="s">
         <v>52</v>
       </c>
@@ -9245,7 +9591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="17.25" customHeight="1">
       <c r="A8" s="117" t="s">
         <v>54</v>
       </c>
@@ -9279,7 +9625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="17.25" customHeight="1">
       <c r="A9" s="117" t="s">
         <v>56</v>
       </c>
@@ -9310,7 +9656,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="17.25" customHeight="1">
       <c r="A10" s="117" t="s">
         <v>58</v>
       </c>
@@ -9326,7 +9672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="17.25" customHeight="1">
       <c r="A11" s="117" t="s">
         <v>59</v>
       </c>
@@ -9345,7 +9691,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="17.25" customHeight="1">
       <c r="A12" s="117" t="s">
         <v>61</v>
       </c>
@@ -9376,7 +9722,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="17.25" customHeight="1">
       <c r="A13" s="117" t="s">
         <v>62</v>
       </c>
@@ -9407,7 +9753,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="17.25" customHeight="1">
       <c r="A14" s="117" t="s">
         <v>67</v>
       </c>
@@ -9423,7 +9769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="17.25" customHeight="1">
       <c r="A15" s="117" t="s">
         <v>68</v>
       </c>
@@ -9439,7 +9785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="17.25" customHeight="1">
       <c r="A16" s="117" t="s">
         <v>69</v>
       </c>
@@ -9455,7 +9801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1">
       <c r="A17" s="117" t="s">
         <v>70</v>
       </c>
@@ -9471,7 +9817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1">
       <c r="A18" s="117" t="s">
         <v>71</v>
       </c>
@@ -9487,7 +9833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1">
       <c r="A19" s="117" t="s">
         <v>72</v>
       </c>
@@ -9503,7 +9849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1">
       <c r="A20" s="117" t="s">
         <v>73</v>
       </c>
@@ -9519,7 +9865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1">
       <c r="A21" s="117" t="s">
         <v>74</v>
       </c>
@@ -9535,7 +9881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1">
       <c r="A22" s="117" t="s">
         <v>76</v>
       </c>
@@ -9551,7 +9897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1">
       <c r="A23" s="117" t="s">
         <v>77</v>
       </c>
@@ -9567,7 +9913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="17.25" customHeight="1">
       <c r="A24" s="117" t="s">
         <v>78</v>
       </c>
@@ -9584,7 +9930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="17.25" customHeight="1">
       <c r="A25" s="117" t="s">
         <v>79</v>
       </c>
@@ -9600,7 +9946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="17.25" customHeight="1">
       <c r="A26" s="117" t="s">
         <v>81</v>
       </c>
@@ -9616,7 +9962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="17.25" customHeight="1">
       <c r="A27" s="117" t="s">
         <v>82</v>
       </c>
@@ -9632,7 +9978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="17.25" customHeight="1">
       <c r="A28" s="117" t="s">
         <v>83</v>
       </c>
@@ -9649,7 +9995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="17.25" customHeight="1">
       <c r="A29" s="117" t="s">
         <v>84</v>
       </c>
@@ -9665,7 +10011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17.25" customHeight="1">
       <c r="A30" s="117" t="s">
         <v>85</v>
       </c>
@@ -9681,7 +10027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="17.25" customHeight="1">
       <c r="A31" s="117" t="s">
         <v>86</v>
       </c>
@@ -9697,7 +10043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="17.25" customHeight="1">
       <c r="A32" s="117" t="s">
         <v>87</v>
       </c>
@@ -9713,7 +10059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17.25" customHeight="1">
       <c r="A33" s="117" t="s">
         <v>88</v>
       </c>
@@ -9729,7 +10075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="17.25" customHeight="1">
       <c r="A34" s="117" t="s">
         <v>89</v>
       </c>
@@ -9745,7 +10091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17.25" customHeight="1">
       <c r="A35" s="117" t="s">
         <v>90</v>
       </c>
@@ -9761,7 +10107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="17.25" customHeight="1">
       <c r="A36" s="117" t="s">
         <v>91</v>
       </c>
@@ -9777,7 +10123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="17.25" customHeight="1">
       <c r="A37" s="117" t="s">
         <v>92</v>
       </c>
@@ -9793,7 +10139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="17.25" customHeight="1">
       <c r="A38" s="117" t="s">
         <v>93</v>
       </c>
@@ -9810,7 +10156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="17.25" customHeight="1">
       <c r="A39" s="117" t="s">
         <v>94</v>
       </c>
@@ -9826,7 +10172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="17.25" customHeight="1">
       <c r="A40" s="117" t="s">
         <v>95</v>
       </c>
@@ -9842,7 +10188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="17.25" customHeight="1">
       <c r="A41" s="117" t="s">
         <v>96</v>
       </c>
@@ -9858,7 +10204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="17.25" customHeight="1">
       <c r="A42" s="117" t="s">
         <v>97</v>
       </c>
@@ -9874,7 +10220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="17.25" customHeight="1">
       <c r="A43" s="117" t="s">
         <v>98</v>
       </c>
@@ -9890,7 +10236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="17.25" customHeight="1">
       <c r="A44" s="117" t="s">
         <v>99</v>
       </c>
@@ -9906,7 +10252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="17.25" customHeight="1">
       <c r="A45" s="117" t="s">
         <v>100</v>
       </c>
@@ -9922,7 +10268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="17.25" customHeight="1">
       <c r="A46" s="117" t="s">
         <v>101</v>
       </c>
@@ -9938,7 +10284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="17.25" customHeight="1">
       <c r="A47" s="117" t="s">
         <v>102</v>
       </c>
@@ -9954,7 +10300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="17.25" customHeight="1">
       <c r="A48" s="117" t="s">
         <v>103</v>
       </c>
@@ -9970,7 +10316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="17.25" customHeight="1">
       <c r="A49" s="117" t="s">
         <v>104</v>
       </c>
@@ -9986,7 +10332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="17.25" customHeight="1">
       <c r="A50" s="117" t="s">
         <v>105</v>
       </c>
@@ -10003,7 +10349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="17.25" customHeight="1">
       <c r="A51" s="117" t="s">
         <v>106</v>
       </c>
@@ -10020,7 +10366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="17.25" customHeight="1">
       <c r="A52" s="117" t="s">
         <v>107</v>
       </c>
@@ -10036,7 +10382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1">
       <c r="A53" s="117" t="s">
         <v>108</v>
       </c>
@@ -10052,7 +10398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="17.25" customHeight="1">
       <c r="A54" s="117" t="s">
         <v>109</v>
       </c>
@@ -10068,7 +10414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1">
       <c r="A55" s="117" t="s">
         <v>110</v>
       </c>
@@ -10084,7 +10430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1">
       <c r="A56" s="117" t="s">
         <v>111</v>
       </c>
@@ -10100,7 +10446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1">
       <c r="A57" s="117" t="s">
         <v>112</v>
       </c>
@@ -10116,7 +10462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1">
       <c r="A58" s="117" t="s">
         <v>113</v>
       </c>
@@ -10132,7 +10478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1">
       <c r="A59" s="117" t="s">
         <v>114</v>
       </c>
@@ -10148,7 +10494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1">
       <c r="A60" s="117" t="s">
         <v>115</v>
       </c>
@@ -10164,7 +10510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1">
       <c r="A61" s="117" t="s">
         <v>116</v>
       </c>
@@ -10180,7 +10526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1">
       <c r="A62" s="117" t="s">
         <v>117</v>
       </c>
@@ -10196,7 +10542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="17.25" customHeight="1">
       <c r="A63" s="117" t="s">
         <v>118</v>
       </c>
@@ -10212,7 +10558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="17.25" customHeight="1">
       <c r="A64" s="117" t="s">
         <v>119</v>
       </c>
@@ -10228,7 +10574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="17.25" customHeight="1">
       <c r="A65" s="117" t="s">
         <v>120</v>
       </c>
@@ -10244,7 +10590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="17.25" customHeight="1">
       <c r="A66" s="117" t="s">
         <v>121</v>
       </c>
@@ -10260,7 +10606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="17.25" customHeight="1">
       <c r="A67" s="117" t="s">
         <v>122</v>
       </c>
@@ -10276,7 +10622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="17.25" customHeight="1">
       <c r="A68" s="117" t="s">
         <v>123</v>
       </c>
@@ -10292,7 +10638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="17.25" customHeight="1">
       <c r="A69" s="117" t="s">
         <v>125</v>
       </c>
@@ -10308,7 +10654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="17.25" customHeight="1">
       <c r="A70" s="117" t="s">
         <v>127</v>
       </c>
@@ -10324,7 +10670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="17.25" customHeight="1">
       <c r="A71" s="117" t="s">
         <v>129</v>
       </c>
@@ -10340,7 +10686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="17.25" customHeight="1">
       <c r="A72" s="117" t="s">
         <v>130</v>
       </c>
@@ -10356,7 +10702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="17.25" customHeight="1">
       <c r="A73" s="117" t="s">
         <v>131</v>
       </c>
@@ -10372,7 +10718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="17.25" customHeight="1">
       <c r="A74" s="117" t="s">
         <v>132</v>
       </c>
@@ -10388,7 +10734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="17.25" customHeight="1">
       <c r="A75" s="117" t="s">
         <v>133</v>
       </c>
@@ -10404,7 +10750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="17.25" customHeight="1">
       <c r="A76" s="117" t="s">
         <v>134</v>
       </c>
@@ -10420,7 +10766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="17.25" customHeight="1">
       <c r="A77" s="117" t="s">
         <v>135</v>
       </c>
@@ -10436,7 +10782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="17.25" customHeight="1">
       <c r="A78" s="117" t="s">
         <v>136</v>
       </c>
@@ -10452,7 +10798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="17.25" customHeight="1">
       <c r="A79" s="117" t="s">
         <v>137</v>
       </c>
@@ -10468,7 +10814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="17.25" customHeight="1">
       <c r="A80" s="117" t="s">
         <v>138</v>
       </c>
@@ -10484,7 +10830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="17.25" customHeight="1">
       <c r="A81" s="117" t="s">
         <v>139</v>
       </c>
@@ -10500,7 +10846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="17.25" customHeight="1">
       <c r="A82" s="117" t="s">
         <v>141</v>
       </c>
@@ -10516,7 +10862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="17.25" customHeight="1">
       <c r="A83" s="117" t="s">
         <v>142</v>
       </c>
@@ -10532,7 +10878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="17.25" customHeight="1">
       <c r="A84" s="117" t="s">
         <v>143</v>
       </c>
@@ -10548,7 +10894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="17.25" customHeight="1">
       <c r="A85" s="117" t="s">
         <v>144</v>
       </c>
@@ -10564,7 +10910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="17.25" customHeight="1">
       <c r="A86" s="117" t="s">
         <v>146</v>
       </c>
@@ -10580,7 +10926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="17.25" customHeight="1">
       <c r="A87" s="117" t="s">
         <v>147</v>
       </c>
@@ -10596,7 +10942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="17.25" customHeight="1">
       <c r="A88" s="117" t="s">
         <v>148</v>
       </c>
@@ -10612,7 +10958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="17.25" customHeight="1">
       <c r="A89" s="117" t="s">
         <v>149</v>
       </c>
@@ -10628,7 +10974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="17.25" customHeight="1">
       <c r="A90" s="117" t="s">
         <v>150</v>
       </c>
@@ -10644,7 +10990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="17.25" customHeight="1">
       <c r="A91" s="117" t="s">
         <v>151</v>
       </c>
@@ -10660,7 +11006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1">
       <c r="A92" s="117" t="s">
         <v>152</v>
       </c>
@@ -10676,7 +11022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1">
       <c r="A93" s="117" t="s">
         <v>153</v>
       </c>
@@ -10692,7 +11038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1">
       <c r="A94" s="117" t="s">
         <v>154</v>
       </c>
@@ -10708,7 +11054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1">
       <c r="A95" s="117" t="s">
         <v>155</v>
       </c>
@@ -10724,7 +11070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1">
       <c r="A96" s="117" t="s">
         <v>156</v>
       </c>
@@ -10740,7 +11086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="17.25" customHeight="1">
       <c r="A97" s="117" t="s">
         <v>157</v>
       </c>
@@ -10756,7 +11102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="17.25" customHeight="1">
       <c r="A98" s="117" t="s">
         <v>158</v>
       </c>
@@ -10772,7 +11118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="17.25" customHeight="1">
       <c r="A99" s="117" t="s">
         <v>159</v>
       </c>
@@ -10788,20 +11134,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="17.25" customHeight="1">
       <c r="A100" s="117" t="s">
         <v>160</v>
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45716.378380439812</v>
+        <v>45728.469061574076</v>
       </c>
       <c r="D100" s="117">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="17.25" customHeight="1">
       <c r="A101" s="117" t="s">
         <v>161</v>
       </c>
@@ -10817,7 +11163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="17.25" customHeight="1">
       <c r="A102" s="117" t="s">
         <v>162</v>
       </c>
@@ -10833,7 +11179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="17.25" customHeight="1">
       <c r="A103" s="117" t="s">
         <v>163</v>
       </c>
@@ -10849,7 +11195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="17.25" customHeight="1">
       <c r="A104" s="117" t="s">
         <v>164</v>
       </c>
@@ -10865,7 +11211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="17.25" customHeight="1">
       <c r="A105" s="117" t="s">
         <v>165</v>
       </c>
@@ -10881,7 +11227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="17.25" customHeight="1">
       <c r="A106" s="117" t="s">
         <v>166</v>
       </c>
@@ -10897,7 +11243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="17.25" customHeight="1">
       <c r="A107" s="117" t="s">
         <v>167</v>
       </c>
@@ -10913,7 +11259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="17.25" customHeight="1">
       <c r="A108" s="117" t="s">
         <v>168</v>
       </c>
@@ -10929,7 +11275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="17.25" customHeight="1">
       <c r="A109" s="117" t="s">
         <v>169</v>
       </c>
@@ -10945,7 +11291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="17.25" customHeight="1">
       <c r="A110" s="117" t="s">
         <v>170</v>
       </c>
@@ -10961,7 +11307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="17.25" customHeight="1">
       <c r="A111" s="117" t="s">
         <v>171</v>
       </c>
@@ -10977,12 +11323,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="17.25" customHeight="1">
       <c r="A112" s="117"/>
       <c r="B112" s="117"/>
       <c r="D112" s="117"/>
     </row>
-    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="17.25" customHeight="1">
       <c r="A113" s="117" t="s">
         <v>172</v>
       </c>
@@ -10998,7 +11344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="17.25" customHeight="1">
       <c r="A114" s="117" t="s">
         <v>173</v>
       </c>
@@ -11014,7 +11360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="17.25" customHeight="1">
       <c r="A115" s="117" t="s">
         <v>175</v>
       </c>
@@ -11030,7 +11376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="17.25" customHeight="1">
       <c r="A116" s="117" t="s">
         <v>177</v>
       </c>
@@ -11046,7 +11392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="17.25" customHeight="1">
       <c r="A117" s="117" t="s">
         <v>178</v>
       </c>
@@ -11062,7 +11408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="17.25" customHeight="1">
       <c r="A118" s="117" t="s">
         <v>179</v>
       </c>
@@ -11078,7 +11424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="17.25" customHeight="1">
       <c r="A119" s="117" t="s">
         <v>180</v>
       </c>
@@ -11094,7 +11440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="17.25" customHeight="1">
       <c r="A120" s="117" t="s">
         <v>181</v>
       </c>
@@ -11110,7 +11456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="17.25" customHeight="1">
       <c r="A121" s="117" t="s">
         <v>182</v>
       </c>
@@ -11126,7 +11472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="17.25" customHeight="1">
       <c r="A122" s="117" t="s">
         <v>183</v>
       </c>
@@ -11142,7 +11488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="17.25" customHeight="1">
       <c r="A123" s="117" t="s">
         <v>184</v>
       </c>
@@ -11158,7 +11504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="17.25" customHeight="1">
       <c r="A124" s="117" t="s">
         <v>185</v>
       </c>
@@ -11174,7 +11520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="17.25" customHeight="1">
       <c r="A125" s="117" t="s">
         <v>186</v>
       </c>
@@ -11190,7 +11536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="17.25" customHeight="1">
       <c r="A126" s="117" t="s">
         <v>187</v>
       </c>
@@ -11206,7 +11552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="17.25" customHeight="1">
       <c r="A127" s="117" t="s">
         <v>188</v>
       </c>
@@ -11222,7 +11568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="17.25" customHeight="1">
       <c r="A128" s="117" t="s">
         <v>189</v>
       </c>
@@ -11238,7 +11584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="17.25" customHeight="1">
       <c r="A129" s="117" t="s">
         <v>190</v>
       </c>
@@ -11254,7 +11600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="17.25" customHeight="1">
       <c r="A130" s="117" t="s">
         <v>191</v>
       </c>
@@ -11270,7 +11616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="17.25" customHeight="1">
       <c r="A131" s="117" t="s">
         <v>192</v>
       </c>
@@ -11286,7 +11632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="17.25" customHeight="1">
       <c r="A132" s="117" t="s">
         <v>193</v>
       </c>
@@ -11302,7 +11648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="17.25" customHeight="1">
       <c r="A133" s="117" t="s">
         <v>194</v>
       </c>
@@ -11318,7 +11664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="17.25" customHeight="1">
       <c r="A134" s="117" t="s">
         <v>195</v>
       </c>
@@ -11334,7 +11680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="17.25" customHeight="1">
       <c r="A135" s="117" t="s">
         <v>196</v>
       </c>
@@ -11350,7 +11696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="17.25" customHeight="1">
       <c r="A136" s="117" t="s">
         <v>198</v>
       </c>
@@ -11366,7 +11712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="17.25" customHeight="1">
       <c r="A137" s="117" t="s">
         <v>199</v>
       </c>
@@ -11382,7 +11728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="17.25" customHeight="1">
       <c r="A138" s="117" t="s">
         <v>200</v>
       </c>
@@ -11398,7 +11744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="17.25" customHeight="1">
       <c r="A139" s="117" t="s">
         <v>201</v>
       </c>
@@ -11414,7 +11760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="17.25" customHeight="1">
       <c r="A140" s="117" t="s">
         <v>202</v>
       </c>
@@ -11430,7 +11776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="17.25" customHeight="1">
       <c r="A141" s="117" t="s">
         <v>203</v>
       </c>
@@ -11446,7 +11792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="17.25" customHeight="1">
       <c r="A142" s="117" t="s">
         <v>205</v>
       </c>
@@ -11462,7 +11808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="17.25" customHeight="1">
       <c r="A143" s="117" t="s">
         <v>206</v>
       </c>
@@ -11478,20 +11824,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="17.25" customHeight="1">
       <c r="A144" s="117" t="s">
         <v>207</v>
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45716</v>
+        <v>45728</v>
       </c>
       <c r="D144" s="117">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="17.25" customHeight="1">
       <c r="A145" s="117" t="s">
         <v>208</v>
       </c>
@@ -11507,7 +11853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="17.25" customHeight="1">
       <c r="A146" s="117" t="s">
         <v>210</v>
       </c>
@@ -11523,7 +11869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="17.25" customHeight="1">
       <c r="A147" s="117" t="s">
         <v>211</v>
       </c>
@@ -11539,7 +11885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="17.25" customHeight="1">
       <c r="A148" s="117" t="s">
         <v>213</v>
       </c>
@@ -11555,7 +11901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="17.25" customHeight="1">
       <c r="A149" s="117" t="s">
         <v>214</v>
       </c>
@@ -11571,7 +11917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" ht="17.25" customHeight="1">
       <c r="A150" s="117" t="s">
         <v>215</v>
       </c>
@@ -11587,7 +11933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="17.25" customHeight="1">
       <c r="A151" s="117" t="s">
         <v>216</v>
       </c>
@@ -11603,7 +11949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="17.25" customHeight="1">
       <c r="A152" s="117" t="s">
         <v>217</v>
       </c>
@@ -11619,7 +11965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="17.25" customHeight="1">
       <c r="A153" s="117" t="s">
         <v>218</v>
       </c>
@@ -11635,7 +11981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" ht="17.25" customHeight="1">
       <c r="A154" s="117" t="s">
         <v>219</v>
       </c>
@@ -11652,7 +11998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="17.25" customHeight="1">
       <c r="A155" s="117" t="s">
         <v>220</v>
       </c>
@@ -11668,7 +12014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="17.25" customHeight="1">
       <c r="A156" s="117" t="s">
         <v>221</v>
       </c>
@@ -11684,7 +12030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" ht="17.25" customHeight="1">
       <c r="A157" s="117" t="s">
         <v>222</v>
       </c>
@@ -11700,7 +12046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" ht="17.25" customHeight="1">
       <c r="A158" s="117" t="s">
         <v>223</v>
       </c>
@@ -11716,7 +12062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="17.25" customHeight="1">
       <c r="A159" s="117" t="s">
         <v>224</v>
       </c>
@@ -11732,7 +12078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" ht="17.25" customHeight="1">
       <c r="A160" s="117" t="s">
         <v>225</v>
       </c>
@@ -11748,7 +12094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" ht="17.25" customHeight="1">
       <c r="A161" s="117" t="s">
         <v>226</v>
       </c>
@@ -11764,7 +12110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="17.25" customHeight="1">
       <c r="A162" s="117" t="s">
         <v>227</v>
       </c>
@@ -11780,7 +12126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" ht="17.25" customHeight="1">
       <c r="A163" s="117" t="s">
         <v>229</v>
       </c>
@@ -11798,10 +12144,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11821,7 +12167,7 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
@@ -11831,17 +12177,17 @@
     <col min="15" max="18" width="9.140625" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>230</v>
       </c>
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="122" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="123"/>
+      <c r="E1" s="122"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -11849,19 +12195,19 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="D3" s="85" t="s">
         <v>235</v>
       </c>
@@ -11869,25 +12215,25 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="75" customHeight="1">
       <c r="A5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="17" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="18" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:8" outlineLevel="1"/>
+    <row r="11" spans="1:8" outlineLevel="1"/>
+    <row r="12" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="13" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="14" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="15" spans="1:8" outlineLevel="1" collapsed="1"/>
+    <row r="16" spans="1:8" outlineLevel="1"/>
+    <row r="17" outlineLevel="1"/>
+    <row r="18" outlineLevel="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:E2"/>
@@ -11909,14 +12255,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1">
       <c r="A1" s="68" t="s">
         <v>239</v>
       </c>
@@ -11938,7 +12284,7 @@
       </c>
       <c r="M1" s="36"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="40" t="s">
         <v>245</v>
       </c>
@@ -11964,7 +12310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="41" t="s">
         <v>252</v>
       </c>
@@ -11987,7 +12333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15">
       <c r="A4" s="42" t="s">
         <v>256</v>
       </c>
@@ -12013,7 +12359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="43" t="s">
         <v>262</v>
       </c>
@@ -12033,7 +12379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="44" t="s">
         <v>266</v>
       </c>
@@ -12056,7 +12402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="45" t="s">
         <v>271</v>
       </c>
@@ -12076,7 +12422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="21">
       <c r="A8" s="46" t="s">
         <v>275</v>
       </c>
@@ -12099,7 +12445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="47" t="s">
         <v>280</v>
       </c>
@@ -12116,7 +12462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="48" t="s">
         <v>283</v>
       </c>
@@ -12124,7 +12470,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1">
       <c r="A11" s="49" t="s">
         <v>285</v>
       </c>
@@ -12133,7 +12479,7 @@
       </c>
       <c r="F11" s="36"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1">
       <c r="A12" s="50" t="s">
         <v>287</v>
       </c>
@@ -12147,7 +12493,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A13" s="51" t="s">
         <v>290</v>
       </c>
@@ -12158,7 +12504,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A14" s="52" t="s">
         <v>291</v>
       </c>
@@ -12172,7 +12518,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A15" s="53" t="s">
         <v>293</v>
       </c>
@@ -12183,7 +12529,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
       <c r="A16" s="54" t="s">
         <v>294</v>
       </c>
@@ -12197,12 +12543,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.5" thickBot="1">
       <c r="A17" s="55" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.5" thickBot="1">
       <c r="A18" s="74" t="s">
         <v>297</v>
       </c>
@@ -12214,7 +12560,7 @@
       </c>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13.5" thickBot="1">
       <c r="A19" s="75" t="s">
         <v>300</v>
       </c>
@@ -12225,7 +12571,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="51.75" thickBot="1">
       <c r="A20" s="76" t="s">
         <v>303</v>
       </c>
@@ -12239,12 +12585,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.5" thickBot="1">
       <c r="A21" s="77" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.5" thickBot="1">
       <c r="A22" s="78" t="s">
         <v>307</v>
       </c>
@@ -12253,13 +12599,13 @@
       </c>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.5" thickBot="1">
       <c r="A23" s="79" t="s">
         <v>309</v>
       </c>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="A24" s="80" t="s">
         <v>310</v>
       </c>
@@ -12268,20 +12614,20 @@
       </c>
       <c r="E24" s="21"/>
     </row>
-    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C26" s="67" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C28" s="88" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="13.5" thickTop="1"/>
+    <row r="30" spans="1:6">
       <c r="C30" s="87" t="s">
         <v>314</v>
       </c>
@@ -12300,13 +12646,13 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.5" thickBot="1">
       <c r="A1" s="37" t="s">
         <v>315</v>
       </c>
@@ -12323,7 +12669,7 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="38" t="s">
         <v>319</v>
       </c>
@@ -12346,7 +12692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="38" t="s">
         <v>321</v>
       </c>
@@ -12369,7 +12715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="38" t="s">
         <v>325</v>
       </c>
@@ -12389,7 +12735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="38" t="s">
         <v>328</v>
       </c>
@@ -12413,7 +12759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="38" t="s">
         <v>330</v>
       </c>
@@ -12436,7 +12782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="38" t="s">
         <v>333</v>
       </c>
@@ -12462,7 +12808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="38" t="s">
         <v>337</v>
       </c>
@@ -12473,7 +12819,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="38" t="s">
         <v>339</v>
       </c>
@@ -12482,7 +12828,7 @@
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.5" thickBot="1">
       <c r="A10" s="38" t="s">
         <v>340</v>
       </c>
@@ -12500,7 +12846,7 @@
       <c r="I10" s="36"/>
       <c r="J10" s="36"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="38" t="s">
         <v>342</v>
       </c>
@@ -12523,13 +12869,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="38" t="s">
         <v>344</v>
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45716</v>
+        <v>45728</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -12548,7 +12894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="38" t="s">
         <v>346</v>
       </c>
@@ -12571,7 +12917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="38" t="s">
         <v>348</v>
       </c>
@@ -12597,7 +12943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="38" t="s">
         <v>350</v>
       </c>
@@ -12617,7 +12963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="38" t="s">
         <v>352</v>
       </c>
@@ -12640,7 +12986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="38" t="s">
         <v>354</v>
       </c>
@@ -12663,7 +13009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="38" t="s">
         <v>356</v>
       </c>
@@ -12686,7 +13032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="38" t="s">
         <v>358</v>
       </c>
@@ -12709,7 +13055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="38" t="s">
         <v>360</v>
       </c>
@@ -12732,7 +13078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="38" t="s">
         <v>362</v>
       </c>
@@ -12758,7 +13104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="38" t="s">
         <v>364</v>
       </c>
@@ -12784,7 +13130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="38" t="s">
         <v>366</v>
       </c>
@@ -12810,7 +13156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="G24" s="34" t="s">
         <v>368</v>
       </c>
@@ -12827,7 +13173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="38" t="s">
         <v>369</v>
       </c>
@@ -12853,7 +13199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="G26" s="34" t="s">
         <v>371</v>
       </c>
@@ -12873,7 +13219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="21" t="s">
         <v>372</v>
       </c>
@@ -12899,7 +13245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="G28" s="34" t="s">
         <v>374</v>
       </c>
@@ -12919,7 +13265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="G29" s="34" t="s">
         <v>375</v>
       </c>
@@ -12939,7 +13285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="G30" s="34" t="s">
         <v>376</v>
       </c>
@@ -12959,7 +13305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="13.5" thickBot="1">
       <c r="G31" s="35" t="s">
         <v>377</v>
       </c>
@@ -12973,7 +13319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="G32" s="34" t="s">
         <v>378</v>
       </c>
@@ -12987,7 +13333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:10">
       <c r="G33" s="34" t="s">
         <v>379</v>
       </c>
@@ -13001,7 +13347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:10">
       <c r="G34" s="34" t="s">
         <v>380</v>
       </c>
@@ -13015,7 +13361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:10">
       <c r="G35" s="34" t="s">
         <v>381</v>
       </c>
@@ -13029,7 +13375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:10">
       <c r="G36" s="34" t="s">
         <v>382</v>
       </c>
@@ -13043,7 +13389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:10">
       <c r="G37" s="34" t="s">
         <v>383</v>
       </c>
@@ -13057,110 +13403,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="7:10">
       <c r="G39" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="22" priority="58">
+    <cfRule type="expression" dxfId="40" priority="58">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="21" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="20" priority="114"/>
+    <cfRule type="aboveAverage" dxfId="38" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="19" priority="73" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="37" priority="73" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="18" priority="71">
+    <cfRule type="containsBlanks" dxfId="36" priority="71">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="17" priority="70">
+    <cfRule type="containsErrors" dxfId="35" priority="70">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="16" priority="69" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="34" priority="69" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="15" priority="67" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="33" priority="67" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="66">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="13" priority="65">
+    <cfRule type="notContainsErrors" dxfId="31" priority="65">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="12" priority="64" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="30" priority="64" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="11" priority="63" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="29" priority="63" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="10" priority="115" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="115" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="9" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="45" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="8" priority="56" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="56" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -13194,10 +13540,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="1" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="0" priority="96"/>
+    <cfRule type="uniqueValues" dxfId="18" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="44">
@@ -13621,11 +13967,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CCC4B1-5C65-4837-AA26-56CCF06B63BB}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
@@ -13637,12 +13983,12 @@
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15">
       <c r="C3" s="17" t="s">
         <v>35</v>
       </c>
@@ -13668,7 +14014,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="C4" s="117" t="s">
         <v>42</v>
       </c>
@@ -13699,7 +14045,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="C5" s="117" t="s">
         <v>44</v>
       </c>
@@ -13730,7 +14076,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="C6" s="117" t="s">
         <v>391</v>
       </c>
@@ -13763,7 +14109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="B8" t="s">
         <v>392</v>
       </c>
@@ -13774,22 +14120,22 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>435</v>
+        <v>393</v>
       </c>
       <c r="G8" t="s">
-        <v>436</v>
+        <v>394</v>
       </c>
       <c r="H8" t="s">
-        <v>437</v>
+        <v>395</v>
       </c>
       <c r="I8" t="s">
-        <v>438</v>
+        <v>396</v>
       </c>
       <c r="J8" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="C9">
         <v>3</v>
       </c>
@@ -13817,18 +14163,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="B11" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="C11" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="D11" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="C12">
         <v>3</v>
       </c>
@@ -13836,9 +14182,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="B14" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -13847,7 +14193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="C15">
         <v>3</v>
       </c>
@@ -13855,9 +14201,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -13866,7 +14212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="C18">
         <v>3</v>
       </c>
@@ -13874,9 +14220,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -13885,7 +14231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="C21">
         <v>3</v>
       </c>
@@ -13893,9 +14239,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -13904,7 +14250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4">
       <c r="C24">
         <v>3</v>
       </c>
@@ -13912,9 +14258,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -13923,7 +14269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4">
       <c r="C27">
         <v>3</v>
       </c>
@@ -13931,7 +14277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4">
       <c r="C28" t="s">
         <v>391</v>
       </c>
@@ -13940,36 +14286,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="C30" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="D30" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" hidden="1">
       <c r="C31" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="D31" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
       <c r="C32" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="D32" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -13997,7 +14343,7 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -14018,9 +14364,9 @@
     <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15">
       <c r="A1" s="92" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -14028,7 +14374,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="117"/>
       <c r="B2" s="117"/>
       <c r="C2" s="117"/>
@@ -14036,21 +14382,21 @@
       <c r="E2" s="117"/>
       <c r="F2" s="117"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="117"/>
       <c r="B3" s="117"/>
       <c r="C3" s="89" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="D3" s="89" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="117"/>
       <c r="B4" s="117"/>
       <c r="C4" s="89" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="D4">
         <v>12.1</v>
@@ -14077,10 +14423,10 @@
         <v>12052</v>
       </c>
       <c r="L4" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="117"/>
       <c r="B5" s="117"/>
       <c r="C5" s="90" t="s">
@@ -14093,7 +14439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="117"/>
       <c r="B6" s="117"/>
       <c r="C6" s="91">
@@ -14106,7 +14452,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="117"/>
       <c r="B7" s="117"/>
       <c r="C7" s="90" t="s">
@@ -14119,7 +14465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="117"/>
       <c r="B8" s="117"/>
       <c r="C8" s="91">
@@ -14132,7 +14478,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="117"/>
       <c r="B9" s="117"/>
       <c r="C9" s="90" t="s">
@@ -14145,7 +14491,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="117"/>
       <c r="B10" s="117"/>
       <c r="C10" s="91">
@@ -14158,7 +14504,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="C11" s="90" t="s">
         <v>44</v>
       </c>
@@ -14169,7 +14515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="C12" s="91">
         <v>23000</v>
       </c>
@@ -14180,7 +14526,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="C13" s="90" t="s">
         <v>50</v>
       </c>
@@ -14191,7 +14537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="C14" s="91">
         <v>2</v>
       </c>
@@ -14202,7 +14548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="C15" s="90" t="s">
         <v>48</v>
       </c>
@@ -14213,7 +14559,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="C16" s="91">
         <v>50024</v>
       </c>
@@ -14224,7 +14570,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:12">
       <c r="C17" s="90" t="s">
         <v>53</v>
       </c>
@@ -14235,7 +14581,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:12">
       <c r="C18" s="91">
         <v>189576</v>
       </c>
@@ -14246,7 +14592,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:12">
       <c r="C19" s="90" t="s">
         <v>57</v>
       </c>
@@ -14257,7 +14603,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:12">
       <c r="C20" s="91">
         <v>5000</v>
       </c>
@@ -14268,9 +14614,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:12">
       <c r="C21" s="90" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="D21">
         <v>9</v>
@@ -14310,35 +14656,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="B2" s="117"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -14355,25 +14701,25 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="51">
       <c r="A1" s="99" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="B7" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -14381,7 +14727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -14389,7 +14735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -14397,7 +14743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -14405,7 +14751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
[FIX] xlsx: prevent unwanted legend when importing chart from excel
When creating an XLSX file with a chart that has no legend, the legend
unexpectedly appears after importing the file. This issue occurs due to
the default behavior of the import process, which adds a bottom legend
even if it was not initially set.

closes odoo/o-spreadsheet#5978

Task: 4632987
X-original-commit: 5acb8fc
Signed-off-by: Adrien Minne (adrm) <adrm@odoo.com>
Signed-off-by: Mehdi Rachico (mera) <mera@odoo.com>
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C3FAEF4-9495-4537-B722-A5A16F9D6A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ABEBB5E-CC42-4D3F-B076-13470D76BC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
   </externalReferences>
   <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5972" r:id="rId16"/>
+    <pivotCache cacheId="3062" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2390,6 +2390,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2402,7 +2403,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -4000,7 +4000,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -5283,7 +5283,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -5718,25 +5718,6 @@
         </a:solidFill>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr sz="1000" b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="1"/>
@@ -6426,23 +6407,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="l"/>
       <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr sz="1000" b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
@@ -7936,7 +7902,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="5972" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="3062" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -8570,7 +8536,7 @@
       <c r="H2" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="123"/>
+      <c r="I2" s="119"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="17.25" customHeight="1">
@@ -8580,10 +8546,10 @@
       <c r="G3" s="117">
         <v>8</v>
       </c>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="119"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="119">
+      <c r="K3" s="120">
         <v>5</v>
       </c>
       <c r="L3" s="6"/>
@@ -8601,10 +8567,10 @@
       <c r="G4" s="117">
         <v>9</v>
       </c>
-      <c r="H4" s="123"/>
-      <c r="I4" s="123"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="120"/>
+      <c r="K4" s="121"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="17.25" customHeight="1">
@@ -8614,10 +8580,10 @@
       <c r="G5" s="117">
         <v>15</v>
       </c>
-      <c r="H5" s="123"/>
-      <c r="I5" s="123"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="120"/>
+      <c r="K5" s="121"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" ht="17.25" customHeight="1">
@@ -8625,7 +8591,7 @@
         <v>22</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="120"/>
+      <c r="K6" s="121"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="17.25" customHeight="1">
@@ -8633,7 +8599,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="120"/>
+      <c r="K7" s="121"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="17.25" customHeight="1">
@@ -8641,7 +8607,7 @@
         <v>30</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="121"/>
+      <c r="K8" s="122"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="17.25" customHeight="1">
@@ -11140,7 +11106,7 @@
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45728.469061574076</v>
+        <v>45736.475918171294</v>
       </c>
       <c r="D100" s="117">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -11830,7 +11796,7 @@
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45728</v>
+        <v>45736</v>
       </c>
       <c r="D144" s="117">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
@@ -12184,10 +12150,10 @@
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="122" t="s">
+      <c r="D1" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="122"/>
+      <c r="E1" s="123"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -12200,8 +12166,8 @@
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
@@ -12875,7 +12841,7 @@
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45728</v>
+        <v>45736</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -14656,7 +14622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[IMP] xlsx: support import/export of doughnut, pyramid & horizontal bar charts
This commit adds support for exporting & importing doughnut, pyramid & horizontal
bar charts. Pyramid charts are not supported in Excel, therefore, we do a best effort
by exporting them as two grouped horizontal bar charts with a common vertical and
horizontal axes.

closes odoo/o-spreadsheet#5448

Task: 3978237
Signed-off-by: Adrien Minne (adrm) <adrm@odoo.com>
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28723"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28919"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4533F51F-F931-45DF-A942-2AE56A765B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{680A992B-769D-4DF5-8BBD-9B4319917BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
   </externalReferences>
   <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5712" r:id="rId16"/>
+    <pivotCache cacheId="11034" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3624,6 +3624,785 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2200"/>
+              <a:t>doughnut chart with hole</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>first dataset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="1F77B4"/>
+              </a:solidFill>
+              <a:ln w="14288" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-4968-47CD-A428-E1CFDB94D5E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF7F0E"/>
+              </a:solidFill>
+              <a:ln w="14288" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000016-4968-47CD-A428-E1CFDB94D5E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="AEC7E8"/>
+              </a:solidFill>
+              <a:ln w="14288" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000018-4968-47CD-A428-E1CFDB94D5E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFBB78"/>
+              </a:solidFill>
+              <a:ln w="14288" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001A-4968-47CD-A428-E1CFDB94D5E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="2CA02C"/>
+              </a:solidFill>
+              <a:ln w="14288" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001C-4968-47CD-A428-E1CFDB94D5E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="98DF8A"/>
+              </a:solidFill>
+              <a:ln w="14288" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001E-4968-47CD-A428-E1CFDB94D5E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="D62728"/>
+              </a:solidFill>
+              <a:ln w="14288" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000020-4968-47CD-A428-E1CFDB94D5E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9896"/>
+              </a:solidFill>
+              <a:ln w="14288" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000022-4968-47CD-A428-E1CFDB94D5E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9467BD"/>
+              </a:solidFill>
+              <a:ln w="14288" cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000024-4968-47CD-A428-E1CFDB94D5E6}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Emily Anderson (Emmy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sophie Allen (Saffi)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chloe Adams</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Megan Alexander (Meg)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lucy Arnold (Lulu)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hannah Alvarez</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jessica Alcock (Jess)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Charlotte Anaya</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lauren Anthony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000025-4968-47CD-A428-E1CFDB94D5E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="50"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr sz="1000" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln cmpd="sng">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>first dataset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Emily Anderson (Emmy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sophie Allen (Saffi)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chloe Adams</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Megan Alexander (Meg)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lucy Arnold (Lulu)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hannah Alvarez</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jessica Alcock (Jess)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Charlotte Anaya</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lauren Anthony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D94B-45A0-8AD6-3E4F4E7665C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>second dataset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Emily Anderson (Emmy)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sophie Allen (Saffi)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chloe Adams</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Megan Alexander (Meg)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lucy Arnold (Lulu)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hannah Alvarez</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jessica Alcock (Jess)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Charlotte Anaya</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lauren Anthony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln cmpd="sng">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D94B-45A0-8AD6-3E4F4E7665C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="998664793"/>
+        <c:axId val="344680958"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="998664793"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="344680958"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="344680958"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="998664793"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -6505,41 +7284,74 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2200"/>
+              <a:t>horizontal bar chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="1"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>first dataset</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="4472C4"/>
+              <a:srgbClr val="7030A0"/>
             </a:solidFill>
-            <a:ln cmpd="sng">
+            <a:ln>
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="1"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="ED7D31"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$27:$A$35</c:f>
@@ -6618,41 +7430,32 @@
                   <a:solidFill>
                     <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
-                  <a:ln cmpd="sng">
+                  <a:ln>
                     <a:solidFill>
-                      <a:srgbClr val="000000"/>
+                      <a:srgbClr val="7030A0"/>
                     </a:solidFill>
+                    <a:prstDash val="solid"/>
                   </a:ln>
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D94B-45A0-8AD6-3E4F4E7665C2}"/>
+              <c16:uniqueId val="{00000001-4F1A-4275-B2BE-C9AFCD205303}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>second dataset</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ED7D31"/>
+              <a:srgbClr val="C65911"/>
             </a:solidFill>
-            <a:ln cmpd="sng">
+            <a:ln>
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:srgbClr val="C65911"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="1"/>
@@ -6734,16 +7537,17 @@
                   <a:solidFill>
                     <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
-                  <a:ln cmpd="sng">
+                  <a:ln>
                     <a:solidFill>
-                      <a:srgbClr val="000000"/>
+                      <a:srgbClr val="C65911"/>
                     </a:solidFill>
+                    <a:prstDash val="solid"/>
                   </a:ln>
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D94B-45A0-8AD6-3E4F4E7665C2}"/>
+              <c16:uniqueId val="{00000002-4F1A-4275-B2BE-C9AFCD205303}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6755,17 +7559,26 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="998664793"/>
-        <c:axId val="344680958"/>
+        <c:gapWidth val="70"/>
+        <c:axId val="17781237"/>
+        <c:axId val="88853993"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="998664793"/>
+        <c:axId val="17781237"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -6780,14 +7593,14 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:overlay val="1"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -6795,7 +7608,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr sz="1000" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -6805,7 +7618,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344680958"/>
+        <c:crossAx val="88853993"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6813,32 +7626,21 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344680958"/>
+        <c:axId val="88853993"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="B7B7B7"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -6853,25 +7655,22 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:overlay val="1"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr sz="1000" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -6881,10 +7680,15 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="998664793"/>
+        <c:crossAx val="17781237"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -6894,9 +7698,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr lvl="0">
-            <a:defRPr b="0">
+            <a:defRPr sz="1000" b="0" i="0">
               <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
+                <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
@@ -6909,6 +7713,16 @@
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln cmpd="sng">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -7712,6 +8526,88 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8A2F032-405F-4BA7-AB00-B42F129443DB}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{5D2716A1-A175-44F9-BBD0-26D27F88F15C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C61D9073-4096-46BA-BD71-5483ACC71F2A}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B8A2F032-405F-4BA7-AB00-B42F129443DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7971,7 +8867,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="5712" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="11034" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -11175,7 +12071,7 @@
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45741.742819212966</v>
+        <v>45799.563060763889</v>
       </c>
       <c r="D100" s="117">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -11865,7 +12761,7 @@
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45741</v>
+        <v>45799</v>
       </c>
       <c r="D144" s="117">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
@@ -12910,7 +13806,7 @@
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45741</v>
+        <v>45799</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -14691,7 +15587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[FIX] xlsx: cannot import CF with formulas
Importing a conditional formatting rule with formulas was not working
because the formulas are not prefixed by "=" in the xlsx file.

closes odoo/o-spreadsheet#7036

Task: 4945945
X-original-commit: 14a6da6d6909b532adc8ce8b49f736022e5703b9
Signed-off-by: Rémi Rahir (rar) <rar@odoo.com>
Signed-off-by: Adrien Minne (adrm) <adrm@odoo.com>
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ABEBB5E-CC42-4D3F-B076-13470D76BC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCA15CC-80FD-451D-A815-3D3194402FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,9 @@
   <externalReferences>
     <externalReference r:id="rId15"/>
   </externalReferences>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="3062" r:id="rId16"/>
+    <pivotCache cacheId="1" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="441">
   <si>
     <t>CF =42</t>
   </si>
@@ -1376,6 +1376,9 @@
   </si>
   <si>
     <t>A1234556</t>
+  </si>
+  <si>
+    <t>CF with formulas</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1393,7 @@
     <numFmt numFmtId="168" formatCode="#,##0&quot; EUR €&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;€&quot;#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2390,7 +2393,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2409,155 +2412,11 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="47">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike/>
-        <u/>
-        <color theme="7"/>
-      </font>
-      <numFmt numFmtId="170" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="lightTrellis">
-          <fgColor theme="4"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2967,6 +2826,157 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike/>
+        <u/>
+        <color theme="7"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="lightTrellis">
+          <fgColor theme="4"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -2981,8 +2991,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{33B8EB55-D8D8-4B00-B5CF-C84A8AC9E775}">
-      <tableStyleElement type="wholeTable" dxfId="45"/>
-      <tableStyleElement type="firstRowStripe" dxfId="44"/>
+      <tableStyleElement type="wholeTable" dxfId="46"/>
+      <tableStyleElement type="firstRowStripe" dxfId="45"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -6195,7 +6205,7 @@
           </c:spPr>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!A27:A35</c:f>
+              <c:f>Sheet1!$A$27:$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -7902,7 +7912,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="3062" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -8052,7 +8062,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -8064,22 +8074,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="7">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="29">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8200,9 +8210,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8240,7 +8250,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8346,7 +8356,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8488,7 +8498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8505,7 +8515,7 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -8514,7 +8524,7 @@
     <col min="6" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -8523,7 +8533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27.75">
+    <row r="2" spans="1:12" ht="27.75" x14ac:dyDescent="0.2">
       <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
@@ -8539,7 +8549,7 @@
       <c r="I2" s="119"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
@@ -8554,7 +8564,7 @@
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -8573,7 +8583,7 @@
       <c r="K4" s="121"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="117">
         <v>42</v>
       </c>
@@ -8586,7 +8596,7 @@
       <c r="K5" s="121"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G6" s="117">
         <v>22</v>
       </c>
@@ -8594,7 +8604,7 @@
       <c r="K6" s="121"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="117">
         <v>3</v>
       </c>
@@ -8602,7 +8612,7 @@
       <c r="K7" s="121"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G8" s="117">
         <v>30</v>
       </c>
@@ -8610,7 +8620,7 @@
       <c r="K8" s="122"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="17.25" customHeight="1">
+    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
@@ -8620,7 +8630,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="117">
         <f>SUM(C4:C7)</f>
         <v>57.4</v>
@@ -8629,13 +8639,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1">
+    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="117">
         <f>-(3+C7*SUM(C4:C7))</f>
         <v>-175.2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.25" customHeight="1">
+    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="117">
         <f>SUM(C9:C11)</f>
         <v>-63.399999999999991</v>
@@ -8644,13 +8654,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.25" customHeight="1">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G13" s="117">
         <f>A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12+A13+A14+A15+A16+A17+A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.25" customHeight="1">
+    <row r="14" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
@@ -8659,32 +8669,32 @@
         <v>#CYCLE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.25" customHeight="1">
+    <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="117" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.25" customHeight="1">
+    <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="117" t="str">
         <f>C15</f>
         <v>=(+</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.25" customHeight="1">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="117" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="117" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
         <v>15</v>
@@ -8698,7 +8708,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -8708,7 +8718,7 @@
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
@@ -8722,7 +8732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="16">
         <v>10</v>
       </c>
@@ -8733,7 +8743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="16">
         <v>10.122999999999999</v>
       </c>
@@ -8744,7 +8754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="117" t="s">
         <v>20</v>
       </c>
@@ -8758,7 +8768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="117" t="s">
         <v>22</v>
       </c>
@@ -8775,7 +8785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="117" t="s">
         <v>23</v>
       </c>
@@ -8792,7 +8802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="117" t="s">
         <v>24</v>
       </c>
@@ -8809,7 +8819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="117" t="s">
         <v>25</v>
       </c>
@@ -8826,7 +8836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="117" t="s">
         <v>26</v>
       </c>
@@ -8843,7 +8853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="117" t="s">
         <v>27</v>
       </c>
@@ -8860,7 +8870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17.25" customHeight="1">
+    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="117" t="s">
         <v>28</v>
       </c>
@@ -8877,7 +8887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="17.25" customHeight="1">
+    <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="117" t="s">
         <v>29</v>
       </c>
@@ -8888,7 +8898,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17.25" customHeight="1">
+    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="117" t="s">
         <v>30</v>
       </c>
@@ -8905,7 +8915,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8955,7 +8965,7 @@
       <selection sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8967,12 +8977,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
       <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8986,7 +8996,7 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
@@ -9006,7 +9016,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9021,7 +9031,7 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
@@ -9030,7 +9040,7 @@
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="114" t="s">
         <v>423</v>
       </c>
@@ -9059,7 +9069,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="104">
         <v>4</v>
       </c>
@@ -9088,7 +9098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="104">
         <v>3</v>
       </c>
@@ -9117,7 +9127,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="104">
         <v>9</v>
       </c>
@@ -9146,7 +9156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="104">
         <v>5</v>
       </c>
@@ -9175,7 +9185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="109">
         <v>7</v>
       </c>
@@ -9253,12 +9263,12 @@
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" customHeight="1">
+    <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="117" t="s">
         <v>31</v>
       </c>
@@ -9293,7 +9303,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="117" t="s">
         <v>41</v>
       </c>
@@ -9339,7 +9349,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="117" t="s">
         <v>43</v>
       </c>
@@ -9385,7 +9395,7 @@
         <v>1217.7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1">
+    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="117" t="s">
         <v>45</v>
       </c>
@@ -9431,7 +9441,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
         <v>47</v>
       </c>
@@ -9477,7 +9487,7 @@
         <v>1246.7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17.25" customHeight="1">
+    <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
         <v>49</v>
       </c>
@@ -9523,7 +9533,7 @@
         <v>1213.7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17.25" customHeight="1">
+    <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
         <v>52</v>
       </c>
@@ -9557,7 +9567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17.25" customHeight="1">
+    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
         <v>54</v>
       </c>
@@ -9591,7 +9601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17.25" customHeight="1">
+    <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="117" t="s">
         <v>56</v>
       </c>
@@ -9622,7 +9632,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17.25" customHeight="1">
+    <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="117" t="s">
         <v>58</v>
       </c>
@@ -9638,7 +9648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17.25" customHeight="1">
+    <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="117" t="s">
         <v>59</v>
       </c>
@@ -9657,7 +9667,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="17.25" customHeight="1">
+    <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="117" t="s">
         <v>61</v>
       </c>
@@ -9688,7 +9698,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="17.25" customHeight="1">
+    <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="117" t="s">
         <v>62</v>
       </c>
@@ -9719,7 +9729,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17.25" customHeight="1">
+    <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="117" t="s">
         <v>67</v>
       </c>
@@ -9735,7 +9745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17.25" customHeight="1">
+    <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="117" t="s">
         <v>68</v>
       </c>
@@ -9751,7 +9761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.25" customHeight="1">
+    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="117" t="s">
         <v>69</v>
       </c>
@@ -9767,7 +9777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="117" t="s">
         <v>70</v>
       </c>
@@ -9783,7 +9793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="117" t="s">
         <v>71</v>
       </c>
@@ -9799,7 +9809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="117" t="s">
         <v>72</v>
       </c>
@@ -9815,7 +9825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="117" t="s">
         <v>73</v>
       </c>
@@ -9831,7 +9841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="117" t="s">
         <v>74</v>
       </c>
@@ -9847,7 +9857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="117" t="s">
         <v>76</v>
       </c>
@@ -9863,7 +9873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="117" t="s">
         <v>77</v>
       </c>
@@ -9879,7 +9889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.25" customHeight="1">
+    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="117" t="s">
         <v>78</v>
       </c>
@@ -9896,7 +9906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.25" customHeight="1">
+    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="117" t="s">
         <v>79</v>
       </c>
@@ -9912,7 +9922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.25" customHeight="1">
+    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="117" t="s">
         <v>81</v>
       </c>
@@ -9928,7 +9938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" customHeight="1">
+    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="117" t="s">
         <v>82</v>
       </c>
@@ -9944,7 +9954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" customHeight="1">
+    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="117" t="s">
         <v>83</v>
       </c>
@@ -9961,7 +9971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.25" customHeight="1">
+    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="117" t="s">
         <v>84</v>
       </c>
@@ -9977,7 +9987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.25" customHeight="1">
+    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="117" t="s">
         <v>85</v>
       </c>
@@ -9993,7 +10003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1">
+    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="117" t="s">
         <v>86</v>
       </c>
@@ -10009,7 +10019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" customHeight="1">
+    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="117" t="s">
         <v>87</v>
       </c>
@@ -10025,7 +10035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.25" customHeight="1">
+    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="117" t="s">
         <v>88</v>
       </c>
@@ -10041,7 +10051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.25" customHeight="1">
+    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="117" t="s">
         <v>89</v>
       </c>
@@ -10057,7 +10067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.25" customHeight="1">
+    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="117" t="s">
         <v>90</v>
       </c>
@@ -10073,7 +10083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.25" customHeight="1">
+    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="117" t="s">
         <v>91</v>
       </c>
@@ -10089,7 +10099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" customHeight="1">
+    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="117" t="s">
         <v>92</v>
       </c>
@@ -10105,7 +10115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17.25" customHeight="1">
+    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="117" t="s">
         <v>93</v>
       </c>
@@ -10122,7 +10132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17.25" customHeight="1">
+    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="117" t="s">
         <v>94</v>
       </c>
@@ -10138,7 +10148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.25" customHeight="1">
+    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="117" t="s">
         <v>95</v>
       </c>
@@ -10154,7 +10164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.25" customHeight="1">
+    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="117" t="s">
         <v>96</v>
       </c>
@@ -10170,7 +10180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.25" customHeight="1">
+    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="117" t="s">
         <v>97</v>
       </c>
@@ -10186,7 +10196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17.25" customHeight="1">
+    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="117" t="s">
         <v>98</v>
       </c>
@@ -10202,7 +10212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.25" customHeight="1">
+    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="117" t="s">
         <v>99</v>
       </c>
@@ -10218,7 +10228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.25" customHeight="1">
+    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="117" t="s">
         <v>100</v>
       </c>
@@ -10234,7 +10244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.25" customHeight="1">
+    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="117" t="s">
         <v>101</v>
       </c>
@@ -10250,7 +10260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.25" customHeight="1">
+    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="117" t="s">
         <v>102</v>
       </c>
@@ -10266,7 +10276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" customHeight="1">
+    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="117" t="s">
         <v>103</v>
       </c>
@@ -10282,7 +10292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17.25" customHeight="1">
+    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="117" t="s">
         <v>104</v>
       </c>
@@ -10298,7 +10308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1">
+    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="117" t="s">
         <v>105</v>
       </c>
@@ -10315,7 +10325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1">
+    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="117" t="s">
         <v>106</v>
       </c>
@@ -10332,7 +10342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1">
+    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="117" t="s">
         <v>107</v>
       </c>
@@ -10348,7 +10358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="117" t="s">
         <v>108</v>
       </c>
@@ -10364,7 +10374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1">
+    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="117" t="s">
         <v>109</v>
       </c>
@@ -10380,7 +10390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="117" t="s">
         <v>110</v>
       </c>
@@ -10396,7 +10406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="117" t="s">
         <v>111</v>
       </c>
@@ -10412,7 +10422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="117" t="s">
         <v>112</v>
       </c>
@@ -10428,7 +10438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="117" t="s">
         <v>113</v>
       </c>
@@ -10444,7 +10454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="117" t="s">
         <v>114</v>
       </c>
@@ -10460,7 +10470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="117" t="s">
         <v>115</v>
       </c>
@@ -10476,7 +10486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="117" t="s">
         <v>116</v>
       </c>
@@ -10492,7 +10502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="117" t="s">
         <v>117</v>
       </c>
@@ -10508,7 +10518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1">
+    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="117" t="s">
         <v>118</v>
       </c>
@@ -10524,7 +10534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1">
+    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="117" t="s">
         <v>119</v>
       </c>
@@ -10540,7 +10550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1">
+    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="117" t="s">
         <v>120</v>
       </c>
@@ -10556,7 +10566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1">
+    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="117" t="s">
         <v>121</v>
       </c>
@@ -10572,7 +10582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1">
+    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="117" t="s">
         <v>122</v>
       </c>
@@ -10588,7 +10598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1">
+    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="117" t="s">
         <v>123</v>
       </c>
@@ -10604,7 +10614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1">
+    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="117" t="s">
         <v>125</v>
       </c>
@@ -10620,7 +10630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1">
+    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="117" t="s">
         <v>127</v>
       </c>
@@ -10636,7 +10646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1">
+    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="117" t="s">
         <v>129</v>
       </c>
@@ -10652,7 +10662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1">
+    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="117" t="s">
         <v>130</v>
       </c>
@@ -10668,7 +10678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1">
+    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="117" t="s">
         <v>131</v>
       </c>
@@ -10684,7 +10694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1">
+    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="117" t="s">
         <v>132</v>
       </c>
@@ -10700,7 +10710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1">
+    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="117" t="s">
         <v>133</v>
       </c>
@@ -10716,7 +10726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1">
+    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="117" t="s">
         <v>134</v>
       </c>
@@ -10732,7 +10742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1">
+    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="117" t="s">
         <v>135</v>
       </c>
@@ -10748,7 +10758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1">
+    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="117" t="s">
         <v>136</v>
       </c>
@@ -10764,7 +10774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1">
+    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="117" t="s">
         <v>137</v>
       </c>
@@ -10780,7 +10790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1">
+    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="117" t="s">
         <v>138</v>
       </c>
@@ -10796,7 +10806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1">
+    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="117" t="s">
         <v>139</v>
       </c>
@@ -10812,7 +10822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1">
+    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="117" t="s">
         <v>141</v>
       </c>
@@ -10828,7 +10838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1">
+    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="117" t="s">
         <v>142</v>
       </c>
@@ -10844,7 +10854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1">
+    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="117" t="s">
         <v>143</v>
       </c>
@@ -10860,7 +10870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1">
+    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="117" t="s">
         <v>144</v>
       </c>
@@ -10876,7 +10886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1">
+    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="117" t="s">
         <v>146</v>
       </c>
@@ -10892,7 +10902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1">
+    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="117" t="s">
         <v>147</v>
       </c>
@@ -10908,7 +10918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1">
+    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="117" t="s">
         <v>148</v>
       </c>
@@ -10924,7 +10934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1">
+    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="117" t="s">
         <v>149</v>
       </c>
@@ -10940,7 +10950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1">
+    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="117" t="s">
         <v>150</v>
       </c>
@@ -10956,7 +10966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1">
+    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="117" t="s">
         <v>151</v>
       </c>
@@ -10972,7 +10982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="117" t="s">
         <v>152</v>
       </c>
@@ -10988,7 +10998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="117" t="s">
         <v>153</v>
       </c>
@@ -11004,7 +11014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="117" t="s">
         <v>154</v>
       </c>
@@ -11020,7 +11030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="117" t="s">
         <v>155</v>
       </c>
@@ -11036,7 +11046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="117" t="s">
         <v>156</v>
       </c>
@@ -11052,7 +11062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1">
+    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="117" t="s">
         <v>157</v>
       </c>
@@ -11068,7 +11078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1">
+    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="117" t="s">
         <v>158</v>
       </c>
@@ -11084,7 +11094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1">
+    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="117" t="s">
         <v>159</v>
       </c>
@@ -11100,20 +11110,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="17.25" customHeight="1">
+    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="117" t="s">
         <v>160</v>
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45736.475918171294</v>
+        <v>45903.380486458336</v>
       </c>
       <c r="D100" s="117">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="17.25" customHeight="1">
+    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="117" t="s">
         <v>161</v>
       </c>
@@ -11129,7 +11139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17.25" customHeight="1">
+    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="117" t="s">
         <v>162</v>
       </c>
@@ -11145,7 +11155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17.25" customHeight="1">
+    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="117" t="s">
         <v>163</v>
       </c>
@@ -11161,7 +11171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17.25" customHeight="1">
+    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="117" t="s">
         <v>164</v>
       </c>
@@ -11177,7 +11187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.25" customHeight="1">
+    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="117" t="s">
         <v>165</v>
       </c>
@@ -11193,7 +11203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.25" customHeight="1">
+    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="117" t="s">
         <v>166</v>
       </c>
@@ -11209,7 +11219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.25" customHeight="1">
+    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="117" t="s">
         <v>167</v>
       </c>
@@ -11225,7 +11235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17.25" customHeight="1">
+    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="117" t="s">
         <v>168</v>
       </c>
@@ -11241,7 +11251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.25" customHeight="1">
+    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="117" t="s">
         <v>169</v>
       </c>
@@ -11257,7 +11267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="17.25" customHeight="1">
+    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="117" t="s">
         <v>170</v>
       </c>
@@ -11273,7 +11283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17.25" customHeight="1">
+    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="117" t="s">
         <v>171</v>
       </c>
@@ -11289,12 +11299,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17.25" customHeight="1">
+    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="117"/>
       <c r="B112" s="117"/>
       <c r="D112" s="117"/>
     </row>
-    <row r="113" spans="1:4" ht="17.25" customHeight="1">
+    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="117" t="s">
         <v>172</v>
       </c>
@@ -11310,7 +11320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17.25" customHeight="1">
+    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="117" t="s">
         <v>173</v>
       </c>
@@ -11326,7 +11336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="17.25" customHeight="1">
+    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="117" t="s">
         <v>175</v>
       </c>
@@ -11342,7 +11352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="17.25" customHeight="1">
+    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="117" t="s">
         <v>177</v>
       </c>
@@ -11358,7 +11368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="17.25" customHeight="1">
+    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="117" t="s">
         <v>178</v>
       </c>
@@ -11374,7 +11384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="17.25" customHeight="1">
+    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="117" t="s">
         <v>179</v>
       </c>
@@ -11390,7 +11400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="17.25" customHeight="1">
+    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="117" t="s">
         <v>180</v>
       </c>
@@ -11406,7 +11416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="17.25" customHeight="1">
+    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="117" t="s">
         <v>181</v>
       </c>
@@ -11422,7 +11432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="17.25" customHeight="1">
+    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="117" t="s">
         <v>182</v>
       </c>
@@ -11438,7 +11448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="17.25" customHeight="1">
+    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="117" t="s">
         <v>183</v>
       </c>
@@ -11454,7 +11464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="17.25" customHeight="1">
+    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="117" t="s">
         <v>184</v>
       </c>
@@ -11470,7 +11480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="17.25" customHeight="1">
+    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="117" t="s">
         <v>185</v>
       </c>
@@ -11486,7 +11496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="17.25" customHeight="1">
+    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="117" t="s">
         <v>186</v>
       </c>
@@ -11502,7 +11512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="17.25" customHeight="1">
+    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="117" t="s">
         <v>187</v>
       </c>
@@ -11518,7 +11528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="17.25" customHeight="1">
+    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="117" t="s">
         <v>188</v>
       </c>
@@ -11534,7 +11544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="17.25" customHeight="1">
+    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="117" t="s">
         <v>189</v>
       </c>
@@ -11550,7 +11560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="17.25" customHeight="1">
+    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="117" t="s">
         <v>190</v>
       </c>
@@ -11566,7 +11576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="17.25" customHeight="1">
+    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="117" t="s">
         <v>191</v>
       </c>
@@ -11582,7 +11592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="17.25" customHeight="1">
+    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="117" t="s">
         <v>192</v>
       </c>
@@ -11598,7 +11608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="17.25" customHeight="1">
+    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="117" t="s">
         <v>193</v>
       </c>
@@ -11614,7 +11624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="17.25" customHeight="1">
+    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="117" t="s">
         <v>194</v>
       </c>
@@ -11630,7 +11640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="17.25" customHeight="1">
+    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="117" t="s">
         <v>195</v>
       </c>
@@ -11646,7 +11656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="17.25" customHeight="1">
+    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="117" t="s">
         <v>196</v>
       </c>
@@ -11662,7 +11672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="17.25" customHeight="1">
+    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="117" t="s">
         <v>198</v>
       </c>
@@ -11678,7 +11688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="17.25" customHeight="1">
+    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="117" t="s">
         <v>199</v>
       </c>
@@ -11694,7 +11704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="17.25" customHeight="1">
+    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="117" t="s">
         <v>200</v>
       </c>
@@ -11710,7 +11720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="17.25" customHeight="1">
+    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="117" t="s">
         <v>201</v>
       </c>
@@ -11726,7 +11736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="17.25" customHeight="1">
+    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="117" t="s">
         <v>202</v>
       </c>
@@ -11742,7 +11752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="17.25" customHeight="1">
+    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="117" t="s">
         <v>203</v>
       </c>
@@ -11758,7 +11768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="17.25" customHeight="1">
+    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="117" t="s">
         <v>205</v>
       </c>
@@ -11774,7 +11784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="17.25" customHeight="1">
+    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="117" t="s">
         <v>206</v>
       </c>
@@ -11790,20 +11800,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="17.25" customHeight="1">
+    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="117" t="s">
         <v>207</v>
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45903</v>
       </c>
       <c r="D144" s="117">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="17.25" customHeight="1">
+    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="117" t="s">
         <v>208</v>
       </c>
@@ -11819,7 +11829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="17.25" customHeight="1">
+    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="117" t="s">
         <v>210</v>
       </c>
@@ -11835,7 +11845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="17.25" customHeight="1">
+    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="117" t="s">
         <v>211</v>
       </c>
@@ -11851,7 +11861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="17.25" customHeight="1">
+    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="117" t="s">
         <v>213</v>
       </c>
@@ -11867,7 +11877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="17.25" customHeight="1">
+    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="117" t="s">
         <v>214</v>
       </c>
@@ -11883,7 +11893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="17.25" customHeight="1">
+    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="117" t="s">
         <v>215</v>
       </c>
@@ -11899,7 +11909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="17.25" customHeight="1">
+    <row r="151" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="117" t="s">
         <v>216</v>
       </c>
@@ -11915,7 +11925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="17.25" customHeight="1">
+    <row r="152" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="117" t="s">
         <v>217</v>
       </c>
@@ -11931,7 +11941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="17.25" customHeight="1">
+    <row r="153" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="117" t="s">
         <v>218</v>
       </c>
@@ -11947,7 +11957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="17.25" customHeight="1">
+    <row r="154" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="117" t="s">
         <v>219</v>
       </c>
@@ -11964,7 +11974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="17.25" customHeight="1">
+    <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="117" t="s">
         <v>220</v>
       </c>
@@ -11980,7 +11990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17.25" customHeight="1">
+    <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="117" t="s">
         <v>221</v>
       </c>
@@ -11996,7 +12006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="17.25" customHeight="1">
+    <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="117" t="s">
         <v>222</v>
       </c>
@@ -12012,7 +12022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17.25" customHeight="1">
+    <row r="158" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="117" t="s">
         <v>223</v>
       </c>
@@ -12028,7 +12038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="17.25" customHeight="1">
+    <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="117" t="s">
         <v>224</v>
       </c>
@@ -12044,7 +12054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="17.25" customHeight="1">
+    <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="117" t="s">
         <v>225</v>
       </c>
@@ -12060,7 +12070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="17.25" customHeight="1">
+    <row r="161" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="117" t="s">
         <v>226</v>
       </c>
@@ -12076,7 +12086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="17.25" customHeight="1">
+    <row r="162" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="117" t="s">
         <v>227</v>
       </c>
@@ -12092,7 +12102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="17.25" customHeight="1">
+    <row r="163" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="117" t="s">
         <v>229</v>
       </c>
@@ -12110,10 +12120,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12133,7 +12143,7 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
@@ -12143,7 +12153,7 @@
     <col min="15" max="18" width="9.140625" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>230</v>
       </c>
@@ -12161,7 +12171,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUM(A1)</f>
         <v>0</v>
@@ -12173,7 +12183,7 @@
         <v>referenced string</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" s="85" t="s">
         <v>235</v>
       </c>
@@ -12181,25 +12191,25 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" customHeight="1">
+    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1"/>
-    <row r="11" spans="1:8" outlineLevel="1"/>
-    <row r="12" spans="1:8" hidden="1" outlineLevel="2"/>
-    <row r="13" spans="1:8" hidden="1" outlineLevel="2"/>
-    <row r="14" spans="1:8" hidden="1" outlineLevel="2"/>
-    <row r="15" spans="1:8" outlineLevel="1" collapsed="1"/>
-    <row r="16" spans="1:8" outlineLevel="1"/>
-    <row r="17" outlineLevel="1"/>
-    <row r="18" outlineLevel="1"/>
+    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:8" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="17" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="18" outlineLevel="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:E2"/>
@@ -12221,14 +12231,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>239</v>
       </c>
@@ -12250,7 +12260,7 @@
       </c>
       <c r="M1" s="36"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
         <v>245</v>
       </c>
@@ -12276,7 +12286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>252</v>
       </c>
@@ -12299,7 +12309,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15">
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>256</v>
       </c>
@@ -12325,7 +12335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
         <v>262</v>
       </c>
@@ -12345,7 +12355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>266</v>
       </c>
@@ -12368,7 +12378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
         <v>271</v>
       </c>
@@ -12388,7 +12398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21">
+    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="46" t="s">
         <v>275</v>
       </c>
@@ -12411,7 +12421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="47" t="s">
         <v>280</v>
       </c>
@@ -12428,7 +12438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
         <v>283</v>
       </c>
@@ -12436,7 +12446,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.5" thickBot="1">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
         <v>285</v>
       </c>
@@ -12445,7 +12455,7 @@
       </c>
       <c r="F11" s="36"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="50" t="s">
         <v>287</v>
       </c>
@@ -12459,7 +12469,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>290</v>
       </c>
@@ -12470,7 +12480,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
         <v>291</v>
       </c>
@@ -12484,7 +12494,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>293</v>
       </c>
@@ -12495,7 +12505,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
         <v>294</v>
       </c>
@@ -12509,12 +12519,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1">
+    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1">
+    <row r="18" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
         <v>297</v>
       </c>
@@ -12526,7 +12536,7 @@
       </c>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="1:6" ht="13.5" thickBot="1">
+    <row r="19" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
         <v>300</v>
       </c>
@@ -12537,7 +12547,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51.75" thickBot="1">
+    <row r="20" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="76" t="s">
         <v>303</v>
       </c>
@@ -12551,12 +12561,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" thickBot="1">
+    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="77" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.5" thickBot="1">
+    <row r="22" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
         <v>307</v>
       </c>
@@ -12565,13 +12575,13 @@
       </c>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="13.5" thickBot="1">
+    <row r="23" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="79" t="s">
         <v>309</v>
       </c>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="80" t="s">
         <v>310</v>
       </c>
@@ -12580,20 +12590,20 @@
       </c>
       <c r="E24" s="21"/>
     </row>
-    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
-    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C26" s="67" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
-    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" s="88" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.5" thickTop="1"/>
-    <row r="30" spans="1:6">
+    <row r="29" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" s="87" t="s">
         <v>314</v>
       </c>
@@ -12608,17 +12618,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D919E811-4385-4D35-A19E-3B7E0E659A89}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1">
+    <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>315</v>
       </c>
@@ -12635,7 +12645,7 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>319</v>
       </c>
@@ -12658,7 +12668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>321</v>
       </c>
@@ -12681,7 +12691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>325</v>
       </c>
@@ -12701,7 +12711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
         <v>328</v>
       </c>
@@ -12725,7 +12735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
         <v>330</v>
       </c>
@@ -12748,7 +12758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>333</v>
       </c>
@@ -12774,7 +12784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
         <v>337</v>
       </c>
@@ -12785,7 +12795,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="38" t="s">
         <v>339</v>
       </c>
@@ -12794,7 +12804,7 @@
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1">
+    <row r="10" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>340</v>
       </c>
@@ -12812,7 +12822,7 @@
       <c r="I10" s="36"/>
       <c r="J10" s="36"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>342</v>
       </c>
@@ -12835,13 +12845,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
         <v>344</v>
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45736</v>
+        <v>45903</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -12860,7 +12870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
         <v>346</v>
       </c>
@@ -12883,7 +12893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>348</v>
       </c>
@@ -12909,7 +12919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
         <v>350</v>
       </c>
@@ -12929,7 +12939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
         <v>352</v>
       </c>
@@ -12952,7 +12962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="s">
         <v>354</v>
       </c>
@@ -12975,7 +12985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
         <v>356</v>
       </c>
@@ -12998,7 +13008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
         <v>358</v>
       </c>
@@ -13021,7 +13031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>360</v>
       </c>
@@ -13044,7 +13054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
         <v>362</v>
       </c>
@@ -13070,7 +13080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>364</v>
       </c>
@@ -13096,7 +13106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
         <v>366</v>
       </c>
@@ -13122,7 +13132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G24" s="34" t="s">
         <v>368</v>
       </c>
@@ -13139,7 +13149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
         <v>369</v>
       </c>
@@ -13165,7 +13175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G26" s="34" t="s">
         <v>371</v>
       </c>
@@ -13185,7 +13195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>372</v>
       </c>
@@ -13211,7 +13221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G28" s="34" t="s">
         <v>374</v>
       </c>
@@ -13231,7 +13241,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
       <c r="G29" s="34" t="s">
         <v>375</v>
       </c>
@@ -13251,7 +13270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G30" s="34" t="s">
         <v>376</v>
       </c>
@@ -13271,7 +13290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1">
+    <row r="31" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G31" s="35" t="s">
         <v>377</v>
       </c>
@@ -13285,7 +13304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G32" s="34" t="s">
         <v>378</v>
       </c>
@@ -13299,7 +13318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G33" s="34" t="s">
         <v>379</v>
       </c>
@@ -13313,7 +13332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G34" s="34" t="s">
         <v>380</v>
       </c>
@@ -13327,7 +13346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10">
+    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G35" s="34" t="s">
         <v>381</v>
       </c>
@@ -13341,7 +13360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10">
+    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G36" s="34" t="s">
         <v>382</v>
       </c>
@@ -13355,7 +13374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G37" s="34" t="s">
         <v>383</v>
       </c>
@@ -13369,116 +13388,116 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10">
+    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G39" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="40" priority="58">
+    <cfRule type="expression" dxfId="23" priority="59">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="39" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="47" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="38" priority="114"/>
+    <cfRule type="aboveAverage" dxfId="21" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="37" priority="73" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="20" priority="74" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="36" priority="71">
+    <cfRule type="containsBlanks" dxfId="19" priority="72">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="35" priority="70">
+    <cfRule type="containsErrors" dxfId="18" priority="71">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="34" priority="69" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="17" priority="70" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="33" priority="67" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="16" priority="68" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="67">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="31" priority="65">
+    <cfRule type="notContainsErrors" dxfId="14" priority="66">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="30" priority="64" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="13" priority="65" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="29" priority="63" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="12" priority="64" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="28" priority="115" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="116" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="27" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="26" priority="56" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="57" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:C24">
-    <cfRule type="dataBar" priority="100">
+    <cfRule type="dataBar" priority="101">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13492,7 +13511,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:C25">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13506,13 +13525,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="19" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="18" priority="96"/>
+    <cfRule type="uniqueValues" dxfId="1" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13522,7 +13541,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:J3">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13534,7 +13553,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J4">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="5"/>
@@ -13544,7 +13563,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J5">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="percent" val="10"/>
         <cfvo type="percent" val="90"/>
@@ -13554,7 +13573,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:J6">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -13564,7 +13583,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J7">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="formula" val="$J$6"/>
         <cfvo type="formula" val="$H$6"/>
@@ -13574,7 +13593,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:J11">
-    <cfRule type="iconSet" priority="36">
+    <cfRule type="iconSet" priority="37">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -13583,7 +13602,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J12">
-    <cfRule type="iconSet" priority="35">
+    <cfRule type="iconSet" priority="36">
       <iconSet iconSet="3ArrowsGray">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="2"/>
@@ -13592,7 +13611,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:J13">
-    <cfRule type="iconSet" priority="34">
+    <cfRule type="iconSet" priority="35">
       <iconSet iconSet="3Flags">
         <cfvo type="percent" val="0"/>
         <cfvo type="percentile" val="33"/>
@@ -13601,7 +13620,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:J14">
-    <cfRule type="iconSet" priority="33">
+    <cfRule type="iconSet" priority="34">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="formula" val="$I$14"/>
@@ -13610,7 +13629,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J15">
-    <cfRule type="iconSet" priority="32">
+    <cfRule type="iconSet" priority="33">
       <iconSet iconSet="3TrafficLights2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -13619,7 +13638,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:J16">
-    <cfRule type="iconSet" priority="31">
+    <cfRule type="iconSet" priority="32">
       <iconSet iconSet="3Signs">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -13628,7 +13647,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:J17">
-    <cfRule type="iconSet" priority="30">
+    <cfRule type="iconSet" priority="31">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -13637,7 +13656,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J18">
-    <cfRule type="iconSet" priority="29">
+    <cfRule type="iconSet" priority="30">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -13646,7 +13665,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:J32">
-    <cfRule type="iconSet" priority="28">
+    <cfRule type="iconSet" priority="29">
       <iconSet iconSet="3Arrows" reverse="1">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -13655,7 +13674,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:J33">
-    <cfRule type="iconSet" priority="27">
+    <cfRule type="iconSet" priority="28">
       <iconSet iconSet="3Arrows" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -13664,7 +13683,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34:J34">
-    <cfRule type="iconSet" priority="26">
+    <cfRule type="iconSet" priority="27">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="0" gte="0"/>
@@ -13673,7 +13692,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21:K21">
-    <cfRule type="iconSet" priority="18">
+    <cfRule type="iconSet" priority="19">
       <iconSet iconSet="4Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -13683,7 +13702,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:K22">
-    <cfRule type="iconSet" priority="17">
+    <cfRule type="iconSet" priority="18">
       <iconSet iconSet="4ArrowsGray">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -13693,7 +13712,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23:K23">
-    <cfRule type="iconSet" priority="16">
+    <cfRule type="iconSet" priority="17">
       <iconSet iconSet="4RedToBlack">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -13703,7 +13722,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24">
-    <cfRule type="iconSet" priority="15">
+    <cfRule type="iconSet" priority="16">
       <iconSet iconSet="4Rating">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -13713,7 +13732,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:K25">
-    <cfRule type="iconSet" priority="14">
+    <cfRule type="iconSet" priority="15">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -13723,7 +13742,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26:L26">
-    <cfRule type="iconSet" priority="13">
+    <cfRule type="iconSet" priority="14">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -13734,7 +13753,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27:L27">
-    <cfRule type="iconSet" priority="12">
+    <cfRule type="iconSet" priority="13">
       <iconSet iconSet="5ArrowsGray">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -13745,7 +13764,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28:L28">
-    <cfRule type="iconSet" priority="11">
+    <cfRule type="iconSet" priority="12">
       <iconSet iconSet="5Rating">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -13756,7 +13775,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:L29">
-    <cfRule type="iconSet" priority="10">
+    <cfRule type="iconSet" priority="11">
       <iconSet iconSet="5Quarters">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -13764,6 +13783,12 @@
         <cfvo type="percent" val="60"/>
         <cfvo type="percent" val="80"/>
       </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:C29">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>$B$23</formula>
+      <formula>2+2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13794,7 +13819,7 @@
           <xm:sqref>B25:C25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="20" id="{0776DCAB-3210-41C4-A113-32FD4847A5ED}">
+          <x14:cfRule type="iconSet" priority="21" id="{0776DCAB-3210-41C4-A113-32FD4847A5ED}">
             <x14:iconSet iconSet="3Stars">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -13810,7 +13835,7 @@
           <xm:sqref>H19:J19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="19" id="{367C8C3A-A19C-489B-B02C-135E717D92A5}">
+          <x14:cfRule type="iconSet" priority="20" id="{367C8C3A-A19C-489B-B02C-135E717D92A5}">
             <x14:iconSet iconSet="3Triangles">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -13826,7 +13851,7 @@
           <xm:sqref>H20:J20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{2F0448E0-FD4B-4CC6-8AFB-1FCD78ED3F40}">
+          <x14:cfRule type="iconSet" priority="9" id="{2F0448E0-FD4B-4CC6-8AFB-1FCD78ED3F40}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -13845,7 +13870,7 @@
           <xm:sqref>H31:J31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="25" id="{EDB615C5-C26E-42E3-8D7C-CFC96E348794}">
+          <x14:cfRule type="iconSet" priority="26" id="{EDB615C5-C26E-42E3-8D7C-CFC96E348794}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -13864,7 +13889,7 @@
           <xm:sqref>H35:J35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="24" id="{3673FAEE-9C58-4DC2-8FFB-38004FA3122F}">
+          <x14:cfRule type="iconSet" priority="25" id="{3673FAEE-9C58-4DC2-8FFB-38004FA3122F}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -13883,7 +13908,7 @@
           <xm:sqref>H36:J36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="23" id="{BEA8CADB-6314-47A4-B945-05492B4E899C}">
+          <x14:cfRule type="iconSet" priority="24" id="{BEA8CADB-6314-47A4-B945-05492B4E899C}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -13902,7 +13927,7 @@
           <xm:sqref>H37:J37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="9" id="{DD78C548-721C-42F8-BA23-99215A699C4C}">
+          <x14:cfRule type="iconSet" priority="10" id="{DD78C548-721C-42F8-BA23-99215A699C4C}">
             <x14:iconSet iconSet="5Boxes">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -13937,7 +13962,7 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
@@ -13949,12 +13974,12 @@
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="C3" s="17" t="s">
         <v>35</v>
       </c>
@@ -13980,7 +14005,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="117" t="s">
         <v>42</v>
       </c>
@@ -14011,7 +14036,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="117" t="s">
         <v>44</v>
       </c>
@@ -14042,7 +14067,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="117" t="s">
         <v>391</v>
       </c>
@@ -14075,7 +14100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>392</v>
       </c>
@@ -14101,7 +14126,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>3</v>
       </c>
@@ -14129,7 +14154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>398</v>
       </c>
@@ -14140,7 +14165,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>3</v>
       </c>
@@ -14148,7 +14173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>401</v>
       </c>
@@ -14159,7 +14184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>3</v>
       </c>
@@ -14167,7 +14192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>402</v>
       </c>
@@ -14178,7 +14203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>3</v>
       </c>
@@ -14186,7 +14211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>403</v>
       </c>
@@ -14197,7 +14222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C21">
         <v>3</v>
       </c>
@@ -14205,7 +14230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>404</v>
       </c>
@@ -14216,7 +14241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C24">
         <v>3</v>
       </c>
@@ -14224,7 +14249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>405</v>
       </c>
@@ -14235,7 +14260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C27">
         <v>3</v>
       </c>
@@ -14243,7 +14268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>391</v>
       </c>
@@ -14252,7 +14277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>406</v>
       </c>
@@ -14263,7 +14288,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="31" spans="2:4" hidden="1">
+    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>409</v>
       </c>
@@ -14271,7 +14296,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>410</v>
       </c>
@@ -14279,7 +14304,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>411</v>
       </c>
@@ -14309,7 +14334,7 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -14330,7 +14355,7 @@
     <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="92" t="s">
         <v>412</v>
       </c>
@@ -14340,7 +14365,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="117"/>
       <c r="B2" s="117"/>
       <c r="C2" s="117"/>
@@ -14348,7 +14373,7 @@
       <c r="E2" s="117"/>
       <c r="F2" s="117"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="117"/>
       <c r="B3" s="117"/>
       <c r="C3" s="89" t="s">
@@ -14358,7 +14383,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="117"/>
       <c r="B4" s="117"/>
       <c r="C4" s="89" t="s">
@@ -14392,7 +14417,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="117"/>
       <c r="B5" s="117"/>
       <c r="C5" s="90" t="s">
@@ -14405,7 +14430,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="117"/>
       <c r="B6" s="117"/>
       <c r="C6" s="91">
@@ -14418,7 +14443,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="117"/>
       <c r="B7" s="117"/>
       <c r="C7" s="90" t="s">
@@ -14431,7 +14456,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="117"/>
       <c r="B8" s="117"/>
       <c r="C8" s="91">
@@ -14444,7 +14469,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="117"/>
       <c r="B9" s="117"/>
       <c r="C9" s="90" t="s">
@@ -14457,7 +14482,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="117"/>
       <c r="B10" s="117"/>
       <c r="C10" s="91">
@@ -14470,7 +14495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="90" t="s">
         <v>44</v>
       </c>
@@ -14481,7 +14506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C12" s="91">
         <v>23000</v>
       </c>
@@ -14492,7 +14517,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C13" s="90" t="s">
         <v>50</v>
       </c>
@@ -14503,7 +14528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C14" s="91">
         <v>2</v>
       </c>
@@ -14514,7 +14539,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C15" s="90" t="s">
         <v>48</v>
       </c>
@@ -14525,7 +14550,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C16" s="91">
         <v>50024</v>
       </c>
@@ -14536,7 +14561,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="3:12">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C17" s="90" t="s">
         <v>53</v>
       </c>
@@ -14547,7 +14572,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="3:12">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C18" s="91">
         <v>189576</v>
       </c>
@@ -14558,7 +14583,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:12">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C19" s="90" t="s">
         <v>57</v>
       </c>
@@ -14569,7 +14594,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="3:12">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C20" s="91">
         <v>5000</v>
       </c>
@@ -14580,7 +14605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:12">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C21" s="90" t="s">
         <v>416</v>
       </c>
@@ -14622,33 +14647,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>418</v>
       </c>
       <c r="B2" s="117"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>420</v>
       </c>
@@ -14667,9 +14692,9 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="51">
+    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
         <v>421</v>
       </c>
@@ -14677,7 +14702,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>407</v>
       </c>
@@ -14685,7 +14710,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -14693,7 +14718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -14701,7 +14726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -14709,7 +14734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -14717,7 +14742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
[FIX] xlsx: `=undefined` when importing array formula
Steps to reproduce:

* Write an array formula =RANDARRAY(20) in Excel.
* Import the file.

Current behavior:

* The anchor cell shows #SPILL!.
* Spill cells are populated with =undefined, causing #BAD_EXPR and
  spill errors.

Desired behavior:

* Only the anchor retains the formula.
* Spill cells are empty (no phantom content), so the array spills
  correctly without #SPILL!.

Task: 4812508
X-original-commit: 7f314e81276118c8ff195e86fcaff5070835f18e
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Odoo\spreadsheet\tests\__xlsx__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhrutik Patel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67BF2DA-E551-4A38-8BB6-2C727149A759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB856E1D-492D-4977-BBBF-6527B5D7DB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,22 +33,11 @@
   </externalReferences>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2414,13 +2403,6 @@
   </cellStyles>
   <dxfs count="47">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2458,6 +2440,13 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -7981,7 +7970,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -8279,9 +8268,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8319,7 +8308,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8425,7 +8414,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8567,7 +8556,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11185,7 +11174,7 @@
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45903.455123148146</v>
+        <v>45905.920118287038</v>
       </c>
       <c r="D100" s="117">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -11875,7 +11864,7 @@
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45903</v>
+        <v>45905</v>
       </c>
       <c r="D144" s="117">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
@@ -12206,10 +12195,10 @@
     <tabColor rgb="FFFF0000"/>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -12277,8 +12266,14 @@
     <row r="14" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:8" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="17" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="18" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="e">
+        <f ca="1">RANDARRAY(2,2)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:E2"/>
@@ -12920,7 +12915,7 @@
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45903</v>
+        <v>45905</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -13593,11 +13588,17 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B29:C29">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+      <formula>$B$23</formula>
+      <formula>2+2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="2" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="1" priority="97"/>
+    <cfRule type="uniqueValues" dxfId="0" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="45">
@@ -13854,12 +13855,6 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:C29">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>$B$23</formula>
-      <formula>2+2</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>

</xml_diff>

<commit_message>
[IMP] SheetProtection: introducing the sheet protection
This revisions adds a (naive) protection for the full sheet.
The ability to block specific modifications (style, grid structure, etc)
is not strictly compatible with our collaborative approach as the server
is never aware of the current state of the spreadsheet.

Task: 5103728
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\odoo\spreadsheet\tests\__xlsx__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rar/rar-workspace/o-spreadsheet/tests/__xlsx__/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C67580FA-155A-4227-B655-21548C93F92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C7959D-379F-564A-B7D4-13925F876C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23400" yWindow="2720" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,15 @@
     <sheet name="jestImages" sheetId="15" r:id="rId12"/>
     <sheet name="jestOneCellAnchor" sheetId="16" r:id="rId13"/>
     <sheet name="jestDataValidations" sheetId="17" r:id="rId14"/>
+    <sheet name="jestLocked" sheetId="18" r:id="rId15"/>
+    <sheet name="jestPartiallyLocked" sheetId="19" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId15"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1190" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId18"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1418,7 +1420,7 @@
     <numFmt numFmtId="168" formatCode="#,##0&quot; EUR €&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;€&quot;#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2353,6 +2355,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2365,165 +2368,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
   <dxfs count="47">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike/>
-        <u/>
-        <color theme="7"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="lightTrellis">
-          <fgColor theme="4"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2941,6 +2792,157 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike/>
+        <u/>
+        <color theme="7"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="lightTrellis">
+          <fgColor theme="4"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -2984,7 +2986,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3601,7 +3603,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3964,7 +3966,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -4380,7 +4382,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -4846,7 +4848,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -5464,7 +5466,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5830,7 +5832,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -6142,7 +6144,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6573,7 +6575,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6975,7 +6977,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7278,7 +7280,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8904,7 +8906,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="1190" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -9054,7 +9056,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9066,22 +9068,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="7">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="29">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9202,9 +9204,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9242,7 +9244,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -9348,7 +9350,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9490,7 +9492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9507,16 +9509,16 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.796875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="26" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.19921875" customWidth="1"/>
+    <col min="2" max="2" width="13.796875" customWidth="1"/>
+    <col min="3" max="3" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.19921875" customWidth="1"/>
+    <col min="6" max="26" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -9525,7 +9527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27.75">
+    <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9538,25 +9540,25 @@
       <c r="H2" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="115"/>
+      <c r="I2" s="111"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="104">
         <v>8</v>
       </c>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="111">
+      <c r="K3" s="112">
         <v>5</v>
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -9569,50 +9571,50 @@
       <c r="G4" s="104">
         <v>9</v>
       </c>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="112"/>
+      <c r="K4" s="113"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="104">
         <v>42</v>
       </c>
       <c r="G5" s="104">
         <v>15</v>
       </c>
-      <c r="H5" s="115"/>
-      <c r="I5" s="115"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="112"/>
+      <c r="K5" s="113"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G6" s="104">
         <v>22</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="112"/>
+      <c r="K6" s="113"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="104">
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="112"/>
+      <c r="K7" s="113"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G8" s="104">
         <v>30</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="113"/>
+      <c r="K8" s="114"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="17.25" customHeight="1">
+    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
@@ -9622,7 +9624,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="104">
         <f>SUM(C4:C7)</f>
         <v>57.4</v>
@@ -9631,13 +9633,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1">
+    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="104">
         <f>-(3+C7*SUM(C4:C7))</f>
         <v>-175.2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.25" customHeight="1">
+    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="104">
         <f>SUM(C9:C11)</f>
         <v>-63.399999999999991</v>
@@ -9646,13 +9648,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.25" customHeight="1">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G13" s="104">
         <f>A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12+A13+A14+A15+A16+A17+A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.25" customHeight="1">
+    <row r="14" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
@@ -9661,32 +9663,32 @@
         <v>#CYCLE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.25" customHeight="1">
+    <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="104" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.25" customHeight="1">
+    <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="104" t="str">
         <f>C15</f>
         <v>=(+</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.25" customHeight="1">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="104" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="104" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
         <v>15</v>
@@ -9700,7 +9702,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -9710,7 +9712,7 @@
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
@@ -9724,7 +9726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="16">
         <v>10</v>
       </c>
@@ -9735,7 +9737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="16">
         <v>10.122999999999999</v>
       </c>
@@ -9746,7 +9748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="104" t="s">
         <v>20</v>
       </c>
@@ -9760,7 +9762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="104" t="s">
         <v>22</v>
       </c>
@@ -9777,7 +9779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="104" t="s">
         <v>23</v>
       </c>
@@ -9794,7 +9796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="104" t="s">
         <v>24</v>
       </c>
@@ -9811,7 +9813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="104" t="s">
         <v>25</v>
       </c>
@@ -9828,7 +9830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="104" t="s">
         <v>26</v>
       </c>
@@ -9845,7 +9847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="104" t="s">
         <v>27</v>
       </c>
@@ -9862,7 +9864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17.25" customHeight="1">
+    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="104" t="s">
         <v>28</v>
       </c>
@@ -9879,7 +9881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="17.25" customHeight="1">
+    <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="104" t="s">
         <v>29</v>
       </c>
@@ -9890,7 +9892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17.25" customHeight="1">
+    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="104" t="s">
         <v>30</v>
       </c>
@@ -9907,7 +9909,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9957,7 +9959,7 @@
       <selection sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9969,12 +9971,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
       <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9988,10 +9990,10 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.796875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="26" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="65.19921875" customWidth="1"/>
+    <col min="2" max="26" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10008,7 +10010,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10023,17 +10025,17 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="3" max="4" width="14.19921875" customWidth="1"/>
+    <col min="5" max="5" width="14.796875" customWidth="1"/>
+    <col min="7" max="7" width="14.19921875" customWidth="1"/>
+    <col min="8" max="8" width="20.19921875" customWidth="1"/>
+    <col min="9" max="9" width="17.19921875" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="106" t="s">
         <v>424</v>
       </c>
@@ -10065,7 +10067,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>4</v>
       </c>
@@ -10097,7 +10099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -10129,7 +10131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>9</v>
       </c>
@@ -10161,7 +10163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -10193,7 +10195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7</v>
       </c>
@@ -10267,6 +10269,34 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175FB5D6-D3ED-FD4F-886B-71BD0CB28755}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B936FE7B-5147-E945-A711-7FBABD0575D3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0630FA18-71FC-4ACD-8379-39A3603D1DD6}">
   <sheetPr>
@@ -10278,12 +10308,12 @@
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.796875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="13.7109375" customWidth="1"/>
+    <col min="1" max="26" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" customHeight="1">
+    <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="104" t="s">
         <v>31</v>
       </c>
@@ -10318,7 +10348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="104" t="s">
         <v>41</v>
       </c>
@@ -10364,7 +10394,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="104" t="s">
         <v>43</v>
       </c>
@@ -10410,7 +10440,7 @@
         <v>1217.7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1">
+    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="104" t="s">
         <v>45</v>
       </c>
@@ -10456,7 +10486,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="104" t="s">
         <v>47</v>
       </c>
@@ -10502,7 +10532,7 @@
         <v>1246.7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17.25" customHeight="1">
+    <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="104" t="s">
         <v>49</v>
       </c>
@@ -10548,7 +10578,7 @@
         <v>1213.7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17.25" customHeight="1">
+    <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="104" t="s">
         <v>52</v>
       </c>
@@ -10582,7 +10612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17.25" customHeight="1">
+    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="104" t="s">
         <v>54</v>
       </c>
@@ -10616,7 +10646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17.25" customHeight="1">
+    <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="104" t="s">
         <v>56</v>
       </c>
@@ -10647,7 +10677,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17.25" customHeight="1">
+    <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="104" t="s">
         <v>58</v>
       </c>
@@ -10663,7 +10693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17.25" customHeight="1">
+    <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="104" t="s">
         <v>59</v>
       </c>
@@ -10682,7 +10712,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="17.25" customHeight="1">
+    <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="104" t="s">
         <v>61</v>
       </c>
@@ -10713,7 +10743,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="17.25" customHeight="1">
+    <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="104" t="s">
         <v>62</v>
       </c>
@@ -10744,7 +10774,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17.25" customHeight="1">
+    <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="104" t="s">
         <v>67</v>
       </c>
@@ -10760,7 +10790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17.25" customHeight="1">
+    <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="104" t="s">
         <v>68</v>
       </c>
@@ -10776,7 +10806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.25" customHeight="1">
+    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="104" t="s">
         <v>69</v>
       </c>
@@ -10792,7 +10822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="104" t="s">
         <v>70</v>
       </c>
@@ -10808,7 +10838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="104" t="s">
         <v>71</v>
       </c>
@@ -10824,7 +10854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="104" t="s">
         <v>72</v>
       </c>
@@ -10840,7 +10870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="104" t="s">
         <v>73</v>
       </c>
@@ -10856,7 +10886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="104" t="s">
         <v>74</v>
       </c>
@@ -10872,7 +10902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="104" t="s">
         <v>76</v>
       </c>
@@ -10888,7 +10918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="104" t="s">
         <v>77</v>
       </c>
@@ -10904,7 +10934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.25" customHeight="1">
+    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="104" t="s">
         <v>78</v>
       </c>
@@ -10921,7 +10951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.25" customHeight="1">
+    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="104" t="s">
         <v>79</v>
       </c>
@@ -10937,7 +10967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.25" customHeight="1">
+    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="104" t="s">
         <v>81</v>
       </c>
@@ -10953,7 +10983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" customHeight="1">
+    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="104" t="s">
         <v>82</v>
       </c>
@@ -10969,7 +10999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" customHeight="1">
+    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="104" t="s">
         <v>83</v>
       </c>
@@ -10986,7 +11016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.25" customHeight="1">
+    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="104" t="s">
         <v>84</v>
       </c>
@@ -11002,7 +11032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.25" customHeight="1">
+    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="104" t="s">
         <v>85</v>
       </c>
@@ -11018,7 +11048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1">
+    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="104" t="s">
         <v>86</v>
       </c>
@@ -11034,7 +11064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" customHeight="1">
+    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="104" t="s">
         <v>87</v>
       </c>
@@ -11050,7 +11080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.25" customHeight="1">
+    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="104" t="s">
         <v>88</v>
       </c>
@@ -11066,7 +11096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.25" customHeight="1">
+    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="104" t="s">
         <v>89</v>
       </c>
@@ -11082,7 +11112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.25" customHeight="1">
+    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="104" t="s">
         <v>90</v>
       </c>
@@ -11098,7 +11128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.25" customHeight="1">
+    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="104" t="s">
         <v>91</v>
       </c>
@@ -11114,7 +11144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" customHeight="1">
+    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="104" t="s">
         <v>92</v>
       </c>
@@ -11130,7 +11160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17.25" customHeight="1">
+    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="104" t="s">
         <v>93</v>
       </c>
@@ -11147,7 +11177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17.25" customHeight="1">
+    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="104" t="s">
         <v>94</v>
       </c>
@@ -11163,7 +11193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.25" customHeight="1">
+    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="104" t="s">
         <v>95</v>
       </c>
@@ -11179,7 +11209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.25" customHeight="1">
+    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="104" t="s">
         <v>96</v>
       </c>
@@ -11195,7 +11225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.25" customHeight="1">
+    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="104" t="s">
         <v>97</v>
       </c>
@@ -11211,7 +11241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17.25" customHeight="1">
+    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="104" t="s">
         <v>98</v>
       </c>
@@ -11227,7 +11257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.25" customHeight="1">
+    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="104" t="s">
         <v>99</v>
       </c>
@@ -11243,7 +11273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.25" customHeight="1">
+    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="104" t="s">
         <v>100</v>
       </c>
@@ -11259,7 +11289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.25" customHeight="1">
+    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="104" t="s">
         <v>101</v>
       </c>
@@ -11275,7 +11305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.25" customHeight="1">
+    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="104" t="s">
         <v>102</v>
       </c>
@@ -11291,7 +11321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" customHeight="1">
+    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="104" t="s">
         <v>103</v>
       </c>
@@ -11307,7 +11337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17.25" customHeight="1">
+    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="104" t="s">
         <v>104</v>
       </c>
@@ -11323,7 +11353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1">
+    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="104" t="s">
         <v>105</v>
       </c>
@@ -11340,7 +11370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1">
+    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="104" t="s">
         <v>106</v>
       </c>
@@ -11357,7 +11387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1">
+    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="104" t="s">
         <v>107</v>
       </c>
@@ -11373,7 +11403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="104" t="s">
         <v>108</v>
       </c>
@@ -11389,7 +11419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1">
+    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="104" t="s">
         <v>109</v>
       </c>
@@ -11405,7 +11435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="104" t="s">
         <v>110</v>
       </c>
@@ -11421,7 +11451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="104" t="s">
         <v>111</v>
       </c>
@@ -11437,7 +11467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="104" t="s">
         <v>112</v>
       </c>
@@ -11453,7 +11483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="104" t="s">
         <v>113</v>
       </c>
@@ -11469,7 +11499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="104" t="s">
         <v>114</v>
       </c>
@@ -11485,7 +11515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="104" t="s">
         <v>115</v>
       </c>
@@ -11501,7 +11531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="104" t="s">
         <v>116</v>
       </c>
@@ -11517,7 +11547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="104" t="s">
         <v>117</v>
       </c>
@@ -11533,7 +11563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1">
+    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="104" t="s">
         <v>118</v>
       </c>
@@ -11549,7 +11579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1">
+    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="104" t="s">
         <v>119</v>
       </c>
@@ -11565,7 +11595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1">
+    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="104" t="s">
         <v>120</v>
       </c>
@@ -11581,7 +11611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1">
+    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="104" t="s">
         <v>121</v>
       </c>
@@ -11597,7 +11627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1">
+    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="104" t="s">
         <v>122</v>
       </c>
@@ -11613,7 +11643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1">
+    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="104" t="s">
         <v>123</v>
       </c>
@@ -11629,7 +11659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1">
+    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="104" t="s">
         <v>125</v>
       </c>
@@ -11645,7 +11675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1">
+    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="104" t="s">
         <v>127</v>
       </c>
@@ -11661,7 +11691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1">
+    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="104" t="s">
         <v>129</v>
       </c>
@@ -11677,7 +11707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1">
+    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="104" t="s">
         <v>130</v>
       </c>
@@ -11693,7 +11723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1">
+    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="104" t="s">
         <v>131</v>
       </c>
@@ -11709,7 +11739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1">
+    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="104" t="s">
         <v>132</v>
       </c>
@@ -11725,7 +11755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1">
+    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="104" t="s">
         <v>133</v>
       </c>
@@ -11741,7 +11771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1">
+    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="104" t="s">
         <v>134</v>
       </c>
@@ -11757,7 +11787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1">
+    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="104" t="s">
         <v>135</v>
       </c>
@@ -11773,7 +11803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1">
+    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="104" t="s">
         <v>136</v>
       </c>
@@ -11789,7 +11819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1">
+    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="104" t="s">
         <v>137</v>
       </c>
@@ -11805,7 +11835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1">
+    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="104" t="s">
         <v>138</v>
       </c>
@@ -11821,7 +11851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1">
+    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="104" t="s">
         <v>139</v>
       </c>
@@ -11837,7 +11867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1">
+    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="104" t="s">
         <v>141</v>
       </c>
@@ -11853,7 +11883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1">
+    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="104" t="s">
         <v>142</v>
       </c>
@@ -11869,7 +11899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1">
+    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="104" t="s">
         <v>143</v>
       </c>
@@ -11885,7 +11915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1">
+    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="104" t="s">
         <v>144</v>
       </c>
@@ -11901,7 +11931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1">
+    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="104" t="s">
         <v>146</v>
       </c>
@@ -11917,7 +11947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1">
+    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="104" t="s">
         <v>147</v>
       </c>
@@ -11933,7 +11963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1">
+    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="104" t="s">
         <v>148</v>
       </c>
@@ -11949,7 +11979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1">
+    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="104" t="s">
         <v>149</v>
       </c>
@@ -11965,7 +11995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1">
+    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="104" t="s">
         <v>150</v>
       </c>
@@ -11981,7 +12011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1">
+    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="104" t="s">
         <v>151</v>
       </c>
@@ -11997,7 +12027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="104" t="s">
         <v>152</v>
       </c>
@@ -12013,7 +12043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="104" t="s">
         <v>153</v>
       </c>
@@ -12029,7 +12059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="104" t="s">
         <v>154</v>
       </c>
@@ -12045,7 +12075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="104" t="s">
         <v>155</v>
       </c>
@@ -12061,7 +12091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="104" t="s">
         <v>156</v>
       </c>
@@ -12077,7 +12107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1">
+    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="104" t="s">
         <v>157</v>
       </c>
@@ -12093,7 +12123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1">
+    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="104" t="s">
         <v>158</v>
       </c>
@@ -12109,7 +12139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1">
+    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="104" t="s">
         <v>159</v>
       </c>
@@ -12125,20 +12155,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="17.25" customHeight="1">
+    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="104" t="s">
         <v>160</v>
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>46042.425886574078</v>
+        <v>46050.431470138887</v>
       </c>
       <c r="D100" s="104">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="17.25" customHeight="1">
+    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="104" t="s">
         <v>161</v>
       </c>
@@ -12154,7 +12184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17.25" customHeight="1">
+    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="104" t="s">
         <v>162</v>
       </c>
@@ -12170,7 +12200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17.25" customHeight="1">
+    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="104" t="s">
         <v>163</v>
       </c>
@@ -12186,7 +12216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17.25" customHeight="1">
+    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="104" t="s">
         <v>164</v>
       </c>
@@ -12202,7 +12232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.25" customHeight="1">
+    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="104" t="s">
         <v>165</v>
       </c>
@@ -12218,7 +12248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.25" customHeight="1">
+    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="104" t="s">
         <v>166</v>
       </c>
@@ -12234,7 +12264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.25" customHeight="1">
+    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="104" t="s">
         <v>167</v>
       </c>
@@ -12250,7 +12280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17.25" customHeight="1">
+    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="104" t="s">
         <v>168</v>
       </c>
@@ -12266,7 +12296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.25" customHeight="1">
+    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="104" t="s">
         <v>169</v>
       </c>
@@ -12282,7 +12312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="17.25" customHeight="1">
+    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="104" t="s">
         <v>170</v>
       </c>
@@ -12298,7 +12328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17.25" customHeight="1">
+    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="104" t="s">
         <v>171</v>
       </c>
@@ -12314,12 +12344,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17.25" customHeight="1">
+    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="104"/>
       <c r="B112" s="104"/>
       <c r="D112" s="104"/>
     </row>
-    <row r="113" spans="1:4" ht="17.25" customHeight="1">
+    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="104" t="s">
         <v>172</v>
       </c>
@@ -12335,7 +12365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17.25" customHeight="1">
+    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="104" t="s">
         <v>173</v>
       </c>
@@ -12351,7 +12381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="17.25" customHeight="1">
+    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="104" t="s">
         <v>175</v>
       </c>
@@ -12367,7 +12397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="17.25" customHeight="1">
+    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="104" t="s">
         <v>177</v>
       </c>
@@ -12383,7 +12413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="17.25" customHeight="1">
+    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="104" t="s">
         <v>178</v>
       </c>
@@ -12399,7 +12429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="17.25" customHeight="1">
+    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="104" t="s">
         <v>179</v>
       </c>
@@ -12415,7 +12445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="17.25" customHeight="1">
+    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="104" t="s">
         <v>180</v>
       </c>
@@ -12431,7 +12461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="17.25" customHeight="1">
+    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="104" t="s">
         <v>181</v>
       </c>
@@ -12447,7 +12477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="17.25" customHeight="1">
+    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="104" t="s">
         <v>182</v>
       </c>
@@ -12463,7 +12493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="17.25" customHeight="1">
+    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="104" t="s">
         <v>183</v>
       </c>
@@ -12479,7 +12509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="17.25" customHeight="1">
+    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="104" t="s">
         <v>184</v>
       </c>
@@ -12495,7 +12525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="17.25" customHeight="1">
+    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="104" t="s">
         <v>185</v>
       </c>
@@ -12511,7 +12541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="17.25" customHeight="1">
+    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="104" t="s">
         <v>186</v>
       </c>
@@ -12527,7 +12557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="17.25" customHeight="1">
+    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="104" t="s">
         <v>187</v>
       </c>
@@ -12543,7 +12573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="17.25" customHeight="1">
+    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="104" t="s">
         <v>188</v>
       </c>
@@ -12559,7 +12589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="17.25" customHeight="1">
+    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="104" t="s">
         <v>189</v>
       </c>
@@ -12575,7 +12605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="17.25" customHeight="1">
+    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="104" t="s">
         <v>190</v>
       </c>
@@ -12591,7 +12621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="17.25" customHeight="1">
+    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="104" t="s">
         <v>191</v>
       </c>
@@ -12607,7 +12637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="17.25" customHeight="1">
+    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="104" t="s">
         <v>192</v>
       </c>
@@ -12623,7 +12653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="17.25" customHeight="1">
+    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="104" t="s">
         <v>193</v>
       </c>
@@ -12639,7 +12669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="17.25" customHeight="1">
+    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="104" t="s">
         <v>194</v>
       </c>
@@ -12655,7 +12685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="17.25" customHeight="1">
+    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="104" t="s">
         <v>195</v>
       </c>
@@ -12671,7 +12701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="17.25" customHeight="1">
+    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="104" t="s">
         <v>196</v>
       </c>
@@ -12687,7 +12717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="17.25" customHeight="1">
+    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="104" t="s">
         <v>198</v>
       </c>
@@ -12703,7 +12733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="17.25" customHeight="1">
+    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="104" t="s">
         <v>199</v>
       </c>
@@ -12719,7 +12749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="17.25" customHeight="1">
+    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="104" t="s">
         <v>200</v>
       </c>
@@ -12735,7 +12765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="17.25" customHeight="1">
+    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="104" t="s">
         <v>201</v>
       </c>
@@ -12751,7 +12781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="17.25" customHeight="1">
+    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="104" t="s">
         <v>202</v>
       </c>
@@ -12767,7 +12797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="17.25" customHeight="1">
+    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="104" t="s">
         <v>203</v>
       </c>
@@ -12783,7 +12813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="17.25" customHeight="1">
+    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="104" t="s">
         <v>205</v>
       </c>
@@ -12799,7 +12829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="17.25" customHeight="1">
+    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="104" t="s">
         <v>206</v>
       </c>
@@ -12815,20 +12845,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="17.25" customHeight="1">
+    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="104" t="s">
         <v>207</v>
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>46042</v>
+        <v>46050</v>
       </c>
       <c r="D144" s="104">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="17.25" customHeight="1">
+    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="104" t="s">
         <v>208</v>
       </c>
@@ -12844,7 +12874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="17.25" customHeight="1">
+    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="104" t="s">
         <v>210</v>
       </c>
@@ -12860,7 +12890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="17.25" customHeight="1">
+    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="104" t="s">
         <v>211</v>
       </c>
@@ -12876,7 +12906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="17.25" customHeight="1">
+    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="104" t="s">
         <v>213</v>
       </c>
@@ -12892,7 +12922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="17.25" customHeight="1">
+    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="104" t="s">
         <v>214</v>
       </c>
@@ -12908,7 +12938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="17.25" customHeight="1">
+    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="104" t="s">
         <v>215</v>
       </c>
@@ -12924,7 +12954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="17.25" customHeight="1">
+    <row r="151" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="104" t="s">
         <v>216</v>
       </c>
@@ -12940,7 +12970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="17.25" customHeight="1">
+    <row r="152" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="104" t="s">
         <v>217</v>
       </c>
@@ -12956,7 +12986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="17.25" customHeight="1">
+    <row r="153" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="104" t="s">
         <v>218</v>
       </c>
@@ -12972,7 +13002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="17.25" customHeight="1">
+    <row r="154" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="104" t="s">
         <v>219</v>
       </c>
@@ -12989,7 +13019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="17.25" customHeight="1">
+    <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="104" t="s">
         <v>220</v>
       </c>
@@ -13005,7 +13035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17.25" customHeight="1">
+    <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="104" t="s">
         <v>221</v>
       </c>
@@ -13021,7 +13051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="17.25" customHeight="1">
+    <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="104" t="s">
         <v>222</v>
       </c>
@@ -13037,7 +13067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17.25" customHeight="1">
+    <row r="158" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="104" t="s">
         <v>223</v>
       </c>
@@ -13053,7 +13083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="17.25" customHeight="1">
+    <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="104" t="s">
         <v>224</v>
       </c>
@@ -13069,7 +13099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="17.25" customHeight="1">
+    <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="104" t="s">
         <v>225</v>
       </c>
@@ -13085,7 +13115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="17.25" customHeight="1">
+    <row r="161" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="104" t="s">
         <v>226</v>
       </c>
@@ -13101,7 +13131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="17.25" customHeight="1">
+    <row r="162" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="104" t="s">
         <v>227</v>
       </c>
@@ -13117,7 +13147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="17.25" customHeight="1">
+    <row r="163" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="104" t="s">
         <v>229</v>
       </c>
@@ -13135,10 +13165,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13158,27 +13188,27 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" outlineLevel="1"/>
-    <col min="11" max="11" width="9.140625" outlineLevel="1" collapsed="1"/>
+    <col min="6" max="6" width="14.19921875" customWidth="1"/>
+    <col min="10" max="10" width="9.19921875" outlineLevel="1"/>
+    <col min="11" max="11" width="9.19921875" outlineLevel="1" collapsed="1"/>
     <col min="12" max="14" width="0" hidden="1" outlineLevel="2"/>
-    <col min="15" max="18" width="9.140625" outlineLevel="1"/>
+    <col min="15" max="18" width="9.19921875" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>230</v>
       </c>
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="114" t="s">
+      <c r="D1" s="115" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -13186,19 +13216,19 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" s="85" t="s">
         <v>235</v>
       </c>
@@ -13206,43 +13236,43 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" customHeight="1">
+    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1"/>
-    <row r="11" spans="1:8" outlineLevel="1"/>
-    <row r="12" spans="1:8" hidden="1" outlineLevel="2"/>
-    <row r="13" spans="1:8" hidden="1" outlineLevel="2"/>
-    <row r="14" spans="1:8" hidden="1" outlineLevel="2"/>
-    <row r="15" spans="1:8" outlineLevel="1" collapsed="1"/>
-    <row r="16" spans="1:8" outlineLevel="1"/>
-    <row r="17" spans="1:2" outlineLevel="1"/>
-    <row r="18" spans="1:2" outlineLevel="1"/>
-    <row r="30" spans="1:2">
+    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:8" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" cm="1">
         <f t="array" aca="1" ref="A30:B31" ca="1">_xlfn.RANDARRAY(2,2)</f>
-        <v>0.88429772806393081</v>
+        <v>0.77093979243831789</v>
       </c>
       <c r="B30">
         <f ca="1"/>
-        <v>0.90996014711511952</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>0.89996963625071968</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <f ca="1"/>
-        <v>0.73547363754464601</v>
+        <v>4.753041610255937E-2</v>
       </c>
       <c r="B31">
         <f ca="1"/>
-        <v>0.41617961757033295</v>
+        <v>0.61224139121963739</v>
       </c>
     </row>
   </sheetData>
@@ -13266,14 +13296,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.796875" customWidth="1"/>
+    <col min="5" max="5" width="18.19921875" customWidth="1"/>
+    <col min="13" max="13" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>239</v>
       </c>
@@ -13295,7 +13325,7 @@
       </c>
       <c r="M1" s="36"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
         <v>245</v>
       </c>
@@ -13321,7 +13351,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>252</v>
       </c>
@@ -13344,7 +13374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15">
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>256</v>
       </c>
@@ -13370,7 +13400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
         <v>262</v>
       </c>
@@ -13390,7 +13420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>266</v>
       </c>
@@ -13413,7 +13443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75">
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
         <v>271</v>
       </c>
@@ -13433,7 +13463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21">
+    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>275</v>
       </c>
@@ -13456,7 +13486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="47" t="s">
         <v>280</v>
       </c>
@@ -13473,7 +13503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
         <v>283</v>
       </c>
@@ -13481,7 +13511,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.5" thickBot="1">
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
         <v>285</v>
       </c>
@@ -13490,7 +13520,7 @@
       </c>
       <c r="F11" s="36"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="50" t="s">
         <v>287</v>
       </c>
@@ -13504,7 +13534,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>290</v>
       </c>
@@ -13515,7 +13545,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
         <v>291</v>
       </c>
@@ -13529,7 +13559,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>293</v>
       </c>
@@ -13540,7 +13570,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
         <v>294</v>
       </c>
@@ -13554,12 +13584,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1">
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
         <v>297</v>
       </c>
@@ -13571,7 +13601,7 @@
       </c>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="1:6" ht="13.5" thickBot="1">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
         <v>300</v>
       </c>
@@ -13582,7 +13612,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51.75" thickBot="1">
+    <row r="20" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="76" t="s">
         <v>303</v>
       </c>
@@ -13596,12 +13626,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" thickBot="1">
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="77" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.5" thickBot="1">
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
         <v>307</v>
       </c>
@@ -13610,13 +13640,13 @@
       </c>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="13.5" thickBot="1">
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="79" t="s">
         <v>309</v>
       </c>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="24" spans="1:6" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="80" t="s">
         <v>310</v>
       </c>
@@ -13625,20 +13655,20 @@
       </c>
       <c r="E24" s="21"/>
     </row>
-    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
-    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="25" spans="1:6" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:6" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C26" s="67" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
-    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
+    <row r="27" spans="1:6" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:6" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" s="88" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.5" thickTop="1"/>
-    <row r="30" spans="1:6">
+    <row r="29" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" s="87" t="s">
         <v>314</v>
       </c>
@@ -13657,13 +13687,13 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.19921875" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>315</v>
       </c>
@@ -13680,7 +13710,7 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>319</v>
       </c>
@@ -13703,7 +13733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>321</v>
       </c>
@@ -13726,7 +13756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>325</v>
       </c>
@@ -13746,7 +13776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
         <v>328</v>
       </c>
@@ -13770,7 +13800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
         <v>330</v>
       </c>
@@ -13793,7 +13823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>333</v>
       </c>
@@ -13819,7 +13849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
         <v>337</v>
       </c>
@@ -13830,7 +13860,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="38" t="s">
         <v>339</v>
       </c>
@@ -13839,7 +13869,7 @@
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>340</v>
       </c>
@@ -13857,7 +13887,7 @@
       <c r="I10" s="36"/>
       <c r="J10" s="36"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>342</v>
       </c>
@@ -13880,13 +13910,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
         <v>344</v>
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>46042</v>
+        <v>46050</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -13905,7 +13935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
         <v>346</v>
       </c>
@@ -13928,7 +13958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>348</v>
       </c>
@@ -13954,7 +13984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
         <v>350</v>
       </c>
@@ -13974,7 +14004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
         <v>352</v>
       </c>
@@ -13997,7 +14027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="s">
         <v>354</v>
       </c>
@@ -14020,7 +14050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
         <v>356</v>
       </c>
@@ -14043,7 +14073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
         <v>358</v>
       </c>
@@ -14066,7 +14096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>360</v>
       </c>
@@ -14089,7 +14119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
         <v>362</v>
       </c>
@@ -14115,7 +14145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>364</v>
       </c>
@@ -14141,7 +14171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
         <v>366</v>
       </c>
@@ -14167,7 +14197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G24" s="34" t="s">
         <v>368</v>
       </c>
@@ -14184,7 +14214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
         <v>369</v>
       </c>
@@ -14210,7 +14240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G26" s="34" t="s">
         <v>371</v>
       </c>
@@ -14230,7 +14260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>372</v>
       </c>
@@ -14256,7 +14286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G28" s="34" t="s">
         <v>374</v>
       </c>
@@ -14276,7 +14306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
         <v>375</v>
       </c>
@@ -14305,7 +14335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G30" s="34" t="s">
         <v>377</v>
       </c>
@@ -14325,7 +14355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1">
+    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G31" s="35" t="s">
         <v>378</v>
       </c>
@@ -14339,7 +14369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G32" s="34" t="s">
         <v>379</v>
       </c>
@@ -14353,7 +14383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G33" s="34" t="s">
         <v>380</v>
       </c>
@@ -14367,7 +14397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G34" s="34" t="s">
         <v>381</v>
       </c>
@@ -14381,7 +14411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10">
+    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G35" s="34" t="s">
         <v>382</v>
       </c>
@@ -14395,7 +14425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10">
+    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G36" s="34" t="s">
         <v>383</v>
       </c>
@@ -14409,7 +14439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G37" s="34" t="s">
         <v>384</v>
       </c>
@@ -14423,110 +14453,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10">
+    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
       <c r="G39" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="41" priority="59">
+    <cfRule type="expression" dxfId="23" priority="59">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="47" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="39" priority="115"/>
+    <cfRule type="aboveAverage" dxfId="21" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="38" priority="74" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="20" priority="74" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="37" priority="72">
+    <cfRule type="containsBlanks" dxfId="19" priority="72">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="36" priority="71">
+    <cfRule type="containsErrors" dxfId="18" priority="71">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="35" priority="70" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="17" priority="70" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="34" priority="68" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="16" priority="68" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="67">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="67">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="32" priority="66">
+    <cfRule type="notContainsErrors" dxfId="14" priority="66">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="31" priority="65" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="13" priority="65" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="30" priority="64" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="12" priority="64" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="29" priority="116" percent="1" bottom="1" rank="50"/>
+    <cfRule type="top10" dxfId="11" priority="116" percent="1" bottom="1" rank="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="28" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="27" priority="57" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="57" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -14560,16 +14590,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>$B$23</formula>
       <formula>2+2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="19" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="18" priority="97"/>
+    <cfRule type="uniqueValues" dxfId="0" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="45">
@@ -14997,24 +15027,24 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" customWidth="1"/>
+    <col min="4" max="4" width="9.59765625" customWidth="1"/>
+    <col min="5" max="5" width="26.3984375" customWidth="1"/>
+    <col min="6" max="6" width="27.59765625" customWidth="1"/>
+    <col min="7" max="7" width="23.59765625" customWidth="1"/>
+    <col min="8" max="8" width="16.19921875" customWidth="1"/>
+    <col min="9" max="9" width="18.796875" customWidth="1"/>
+    <col min="10" max="10" width="17.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" s="17" t="s">
         <v>35</v>
       </c>
@@ -15040,7 +15070,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="104" t="s">
         <v>42</v>
       </c>
@@ -15071,7 +15101,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="104" t="s">
         <v>44</v>
       </c>
@@ -15102,7 +15132,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="104" t="s">
         <v>392</v>
       </c>
@@ -15135,7 +15165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>393</v>
       </c>
@@ -15161,7 +15191,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>3</v>
       </c>
@@ -15189,7 +15219,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>399</v>
       </c>
@@ -15200,7 +15230,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>3</v>
       </c>
@@ -15208,7 +15238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>402</v>
       </c>
@@ -15219,7 +15249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>3</v>
       </c>
@@ -15227,7 +15257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>403</v>
       </c>
@@ -15238,7 +15268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>3</v>
       </c>
@@ -15246,7 +15276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>404</v>
       </c>
@@ -15257,7 +15287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C21">
         <v>3</v>
       </c>
@@ -15265,7 +15295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>405</v>
       </c>
@@ -15276,7 +15306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C24">
         <v>3</v>
       </c>
@@ -15284,7 +15314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>406</v>
       </c>
@@ -15295,7 +15325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C27">
         <v>3</v>
       </c>
@@ -15303,7 +15333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>392</v>
       </c>
@@ -15312,7 +15342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>407</v>
       </c>
@@ -15323,7 +15353,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="31" spans="2:4" hidden="1">
+    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>410</v>
       </c>
@@ -15331,7 +15361,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>411</v>
       </c>
@@ -15339,7 +15369,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>412</v>
       </c>
@@ -15369,28 +15399,28 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="92" t="s">
         <v>413</v>
       </c>
@@ -15400,7 +15430,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="104"/>
       <c r="B2" s="104"/>
       <c r="C2" s="104"/>
@@ -15408,7 +15438,7 @@
       <c r="E2" s="104"/>
       <c r="F2" s="104"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="104"/>
       <c r="B3" s="104"/>
       <c r="C3" s="89" t="s">
@@ -15418,7 +15448,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="104"/>
       <c r="B4" s="104"/>
       <c r="C4" s="89" t="s">
@@ -15452,7 +15482,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="104"/>
       <c r="B5" s="104"/>
       <c r="C5" s="90" t="s">
@@ -15465,7 +15495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="104"/>
       <c r="B6" s="104"/>
       <c r="C6" s="91">
@@ -15478,7 +15508,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="104"/>
       <c r="B7" s="104"/>
       <c r="C7" s="90" t="s">
@@ -15491,7 +15521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="104"/>
       <c r="B8" s="104"/>
       <c r="C8" s="91">
@@ -15504,7 +15534,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="104"/>
       <c r="B9" s="104"/>
       <c r="C9" s="90" t="s">
@@ -15517,7 +15547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="104"/>
       <c r="B10" s="104"/>
       <c r="C10" s="91">
@@ -15530,7 +15560,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="90" t="s">
         <v>44</v>
       </c>
@@ -15541,7 +15571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C12" s="91">
         <v>23000</v>
       </c>
@@ -15552,7 +15582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C13" s="90" t="s">
         <v>50</v>
       </c>
@@ -15563,7 +15593,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C14" s="91">
         <v>2</v>
       </c>
@@ -15574,7 +15604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C15" s="90" t="s">
         <v>48</v>
       </c>
@@ -15585,7 +15615,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C16" s="91">
         <v>50024</v>
       </c>
@@ -15596,7 +15626,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="3:12">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C17" s="90" t="s">
         <v>53</v>
       </c>
@@ -15607,7 +15637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="3:12">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C18" s="91">
         <v>189576</v>
       </c>
@@ -15618,7 +15648,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:12">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C19" s="90" t="s">
         <v>57</v>
       </c>
@@ -15629,7 +15659,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="3:12">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C20" s="91">
         <v>5000</v>
       </c>
@@ -15640,7 +15670,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:12">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C21" s="90" t="s">
         <v>417</v>
       </c>
@@ -15682,33 +15712,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.796875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="26" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="65.19921875" customWidth="1"/>
+    <col min="2" max="26" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>419</v>
       </c>
       <c r="B2" s="104"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>421</v>
       </c>
@@ -15727,9 +15757,9 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="51">
+    <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
         <v>422</v>
       </c>
@@ -15737,7 +15767,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>408</v>
       </c>
@@ -15745,7 +15775,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -15753,7 +15783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -15761,7 +15791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -15769,7 +15799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -15777,7 +15807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
[IMP] cf: add top10 conditional formatting operator
This commits adds the "top10" conditional formatting operator, which
highlights the top or bottom N values in a selected range.

Task: 5367065
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Odoo\spreadsheet\tests\__xlsx__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F832354-F3E9-4BC5-A260-88E8A391D52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A476F739-B139-4713-A5CB-3C0E11EABA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
   </externalReferences>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId16"/>
+    <pivotCache cacheId="1" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1563,6 +1563,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1581,6 +1582,7 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="29">
@@ -2151,7 +2153,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2335,6 +2337,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2351,28 +2366,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="71">
     <dxf>
       <font>
         <b val="0"/>
@@ -2553,6 +2553,399 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2951,8 +3344,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{33B8EB55-D8D8-4B00-B5CF-C84A8AC9E775}">
-      <tableStyleElement type="wholeTable" dxfId="46"/>
-      <tableStyleElement type="firstRowStripe" dxfId="45"/>
+      <tableStyleElement type="wholeTable" dxfId="70"/>
+      <tableStyleElement type="firstRowStripe" dxfId="69"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -8837,7 +9230,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -8987,7 +9380,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -8999,22 +9392,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="29">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9468,10 +9861,10 @@
       <c r="G2" s="104">
         <v>5</v>
       </c>
-      <c r="H2" s="105" t="s">
+      <c r="H2" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="106"/>
+      <c r="I2" s="111"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9481,10 +9874,10 @@
       <c r="G3" s="104">
         <v>8</v>
       </c>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="107">
+      <c r="K3" s="112">
         <v>5</v>
       </c>
       <c r="L3" s="6"/>
@@ -9502,10 +9895,10 @@
       <c r="G4" s="104">
         <v>9</v>
       </c>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="108"/>
+      <c r="K4" s="113"/>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9515,10 +9908,10 @@
       <c r="G5" s="104">
         <v>15</v>
       </c>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="108"/>
+      <c r="K5" s="113"/>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9526,7 +9919,7 @@
         <v>22</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="108"/>
+      <c r="K6" s="113"/>
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9534,7 +9927,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="108"/>
+      <c r="K7" s="113"/>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9542,7 +9935,7 @@
         <v>30</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="109"/>
+      <c r="K8" s="114"/>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9840,7 +10233,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9952,7 +10345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025F2510-D243-4DA1-81DE-BBDDA9BC3681}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -9967,63 +10360,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="106" t="s">
         <v>423</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="107" t="s">
         <v>424</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="107" t="s">
         <v>425</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="107" t="s">
         <v>426</v>
       </c>
-      <c r="E1" s="113" t="s">
+      <c r="E1" s="107" t="s">
         <v>427</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="107" t="s">
         <v>428</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="107" t="s">
         <v>429</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="107" t="s">
         <v>430</v>
       </c>
-      <c r="I1" s="114" t="s">
+      <c r="I1" s="108" t="s">
         <v>431</v>
       </c>
-      <c r="J1" s="111" t="s">
+      <c r="J1" s="105" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="115">
+      <c r="A2">
         <v>4</v>
       </c>
-      <c r="B2" s="115">
+      <c r="B2">
         <v>99.5</v>
       </c>
-      <c r="C2" s="115">
-        <v>1</v>
-      </c>
-      <c r="D2" s="115" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>432</v>
       </c>
-      <c r="E2" s="116">
+      <c r="E2" s="39">
         <v>45575</v>
       </c>
-      <c r="F2" s="117">
+      <c r="F2" s="109">
         <v>0.64583333333333337</v>
       </c>
-      <c r="G2" s="117" t="s">
+      <c r="G2" s="109" t="s">
         <v>433</v>
       </c>
-      <c r="H2" s="116">
+      <c r="H2" s="39">
         <v>45292</v>
       </c>
-      <c r="I2" s="115">
+      <c r="I2">
         <v>4</v>
       </c>
       <c r="J2">
@@ -10031,31 +10424,31 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="115">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="115">
+      <c r="B3">
         <v>40</v>
       </c>
-      <c r="C3" s="115">
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" t="s">
         <v>434</v>
       </c>
-      <c r="E3" s="116">
+      <c r="E3" s="39">
         <v>45576</v>
       </c>
-      <c r="F3" s="117">
+      <c r="F3" s="109">
         <v>0.57638888888888884</v>
       </c>
-      <c r="G3" s="117" t="s">
+      <c r="G3" s="109" t="s">
         <v>435</v>
       </c>
-      <c r="H3" s="116">
+      <c r="H3" s="39">
         <v>45231</v>
       </c>
-      <c r="I3" s="115" t="s">
+      <c r="I3" t="s">
         <v>433</v>
       </c>
       <c r="J3">
@@ -10063,31 +10456,31 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="115">
+      <c r="A4">
         <v>9</v>
       </c>
-      <c r="B4" s="115">
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="115">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="115" t="s">
+      <c r="D4" t="s">
         <v>436</v>
       </c>
-      <c r="E4" s="116">
+      <c r="E4" s="39">
         <v>45574</v>
       </c>
-      <c r="F4" s="117">
+      <c r="F4" s="109">
         <v>0.73958333333333337</v>
       </c>
-      <c r="G4" s="117" t="s">
+      <c r="G4" s="109" t="s">
         <v>437</v>
       </c>
-      <c r="H4" s="116">
+      <c r="H4" s="39">
         <v>45325</v>
       </c>
-      <c r="I4" s="115">
+      <c r="I4">
         <v>3</v>
       </c>
       <c r="J4">
@@ -10095,31 +10488,31 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="115">
+      <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="115">
+      <c r="B5">
         <v>120</v>
       </c>
-      <c r="C5" s="115">
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" s="115" t="s">
+      <c r="D5" t="s">
         <v>434</v>
       </c>
-      <c r="E5" s="116">
+      <c r="E5" s="39">
         <v>45573</v>
       </c>
-      <c r="F5" s="117">
+      <c r="F5" s="109">
         <v>0.66666666666666663</v>
       </c>
-      <c r="G5" s="115" t="s">
+      <c r="G5" t="s">
         <v>438</v>
       </c>
-      <c r="H5" s="116">
+      <c r="H5" s="39">
         <v>45084</v>
       </c>
-      <c r="I5" s="115">
+      <c r="I5">
         <v>3</v>
       </c>
       <c r="J5">
@@ -10127,31 +10520,31 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="115">
+      <c r="A6">
         <v>7</v>
       </c>
-      <c r="B6" s="115">
+      <c r="B6">
         <v>12</v>
       </c>
-      <c r="C6" s="115">
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="115" t="s">
+      <c r="D6" t="s">
         <v>436</v>
       </c>
-      <c r="E6" s="116">
+      <c r="E6" s="39">
         <v>45566</v>
       </c>
-      <c r="F6" s="117">
+      <c r="F6" s="109">
         <v>0.5229166666666667</v>
       </c>
-      <c r="G6" s="115" t="s">
+      <c r="G6" t="s">
         <v>439</v>
       </c>
-      <c r="H6" s="116">
+      <c r="H6" s="39">
         <v>45420</v>
       </c>
-      <c r="I6" s="115" t="s">
+      <c r="I6" t="s">
         <v>438</v>
       </c>
       <c r="J6">
@@ -12064,7 +12457,7 @@
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45938.493500231481</v>
+        <v>45989.427180092593</v>
       </c>
       <c r="D100" s="104">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -12754,7 +13147,7 @@
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45938</v>
+        <v>45989</v>
       </c>
       <c r="D144" s="104">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
@@ -13068,10 +13461,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13108,10 +13501,10 @@
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="110" t="s">
+      <c r="D1" s="115" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="110"/>
+      <c r="E1" s="115"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -13124,8 +13517,8 @@
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
@@ -13161,21 +13554,21 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" cm="1">
         <f t="array" aca="1" ref="A30:B31" ca="1">_xlfn.RANDARRAY(2,2)</f>
-        <v>0.7272925709748963</v>
+        <v>0.38411710219623751</v>
       </c>
       <c r="B30">
         <f ca="1"/>
-        <v>0.95782684877879687</v>
+        <v>9.794149803384844E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <f ca="1"/>
-        <v>0.31704384406036645</v>
+        <v>0.66351595791263507</v>
       </c>
       <c r="B31">
         <f ca="1"/>
-        <v>8.7112099778747121E-2</v>
+        <v>5.0911295821026714E-2</v>
       </c>
     </row>
   </sheetData>
@@ -13586,8 +13979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D919E811-4385-4D35-A19E-3B7E0E659A89}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13819,7 +14212,7 @@
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45938</v>
+        <v>45989</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -14362,104 +14755,104 @@
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="23" priority="59">
+    <cfRule type="expression" dxfId="47" priority="59">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="22" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="21" priority="115"/>
+    <cfRule type="aboveAverage" dxfId="45" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="20" priority="74" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="44" priority="74" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="19" priority="72">
+    <cfRule type="containsBlanks" dxfId="43" priority="72">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="18" priority="71">
+    <cfRule type="containsErrors" dxfId="42" priority="71">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="17" priority="70" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="41" priority="70" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="16" priority="68" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="40" priority="68" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="67">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="67">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="14" priority="66">
+    <cfRule type="notContainsErrors" dxfId="38" priority="66">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="13" priority="65" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="37" priority="65" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="12" priority="64" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="36" priority="64" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="11" priority="116" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="116" percent="1" bottom="1" rank="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="10" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="9" priority="57" operator="notEqual">
+    <cfRule type="cellIs" dxfId="34" priority="57" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -14493,16 +14886,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="between">
       <formula>$B$23</formula>
       <formula>2+2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="1" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="0" priority="97"/>
+    <cfRule type="uniqueValues" dxfId="25" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="45">

</xml_diff>

<commit_message>
[IMP] charts: showValues is now exported in Excel
We can setup each chart dataset and add the value as a label, this option can now be exported and imported from excel.

closes odoo/o-spreadsheet#7608

Task: 5213598
Signed-off-by: Lucas Lefèvre (lul) <lul@odoo.com>
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A476F739-B139-4713-A5CB-3C0E11EABA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C67580FA-155A-4227-B655-21548C93F92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,9 @@
   <externalReferences>
     <externalReference r:id="rId15"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId16"/>
+    <pivotCache cacheId="1190" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1204,6 +1204,9 @@
     <t>5Rating</t>
   </si>
   <si>
+    <t>CF with formulas</t>
+  </si>
+  <si>
     <t>5Quarters</t>
   </si>
   <si>
@@ -1376,6 +1379,9 @@
     <t>Custom Formula</t>
   </si>
   <si>
+    <t>Decimal with formula</t>
+  </si>
+  <si>
     <t>option1</t>
   </si>
   <si>
@@ -1398,12 +1404,6 @@
   </si>
   <si>
     <t>A1234556</t>
-  </si>
-  <si>
-    <t>CF with formulas</t>
-  </si>
-  <si>
-    <t>Decimal with formula</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1418,7 @@
     <numFmt numFmtId="168" formatCode="#,##0&quot; EUR €&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;€&quot;#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2353,7 +2353,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2366,51 +2365,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="47">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2421,253 +2389,35 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
+        <b/>
+        <i/>
+        <strike/>
+        <u/>
+        <color theme="7"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="lightTrellis">
+          <fgColor theme="4"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2705,85 +2455,74 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor theme="9"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2996,6 +2735,29 @@
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
@@ -3179,157 +2941,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike/>
-        <u/>
-        <color theme="7"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="lightTrellis">
-          <fgColor theme="4"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -3344,8 +2955,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{33B8EB55-D8D8-4B00-B5CF-C84A8AC9E775}">
-      <tableStyleElement type="wholeTable" dxfId="70"/>
-      <tableStyleElement type="firstRowStripe" dxfId="69"/>
+      <tableStyleElement type="wholeTable" dxfId="46"/>
+      <tableStyleElement type="firstRowStripe" dxfId="45"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3373,7 +2984,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3990,7 +3601,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4353,7 +3964,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -4769,7 +4380,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -4818,6 +4429,27 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="1"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln>
@@ -5214,7 +4846,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -5832,7 +5464,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6198,7 +5830,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -6510,7 +6142,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6941,7 +6573,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7343,7 +6975,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7646,7 +7278,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7702,6 +7334,27 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="1"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln>
@@ -7822,6 +7475,27 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="1"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$27:$A$35</c:f>
@@ -9230,7 +8904,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="1190" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -9380,7 +9054,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="68" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9392,22 +9066,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="7">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9528,9 +9202,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9568,7 +9242,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -9674,7 +9348,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9816,7 +9490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9833,7 +9507,7 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -9842,7 +9516,7 @@
     <col min="6" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1">
       <c r="A1" s="21"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -9851,7 +9525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="27.75">
       <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9864,25 +9538,25 @@
       <c r="H2" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="111"/>
+      <c r="I2" s="115"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1">
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="104">
         <v>8</v>
       </c>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="112">
+      <c r="K3" s="111">
         <v>5</v>
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -9895,50 +9569,50 @@
       <c r="G4" s="104">
         <v>9</v>
       </c>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="113"/>
+      <c r="K4" s="112"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1">
       <c r="C5" s="104">
         <v>42</v>
       </c>
       <c r="G5" s="104">
         <v>15</v>
       </c>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="113"/>
+      <c r="K5" s="112"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1">
       <c r="G6" s="104">
         <v>22</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="113"/>
+      <c r="K6" s="112"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1">
       <c r="C7" s="104">
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="113"/>
+      <c r="K7" s="112"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1">
       <c r="G8" s="104">
         <v>30</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="114"/>
+      <c r="K8" s="113"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17.25" customHeight="1">
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
@@ -9948,7 +9622,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1">
       <c r="C10" s="104">
         <f>SUM(C4:C7)</f>
         <v>57.4</v>
@@ -9957,13 +9631,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17.25" customHeight="1">
       <c r="C11" s="104">
         <f>-(3+C7*SUM(C4:C7))</f>
         <v>-175.2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="17.25" customHeight="1">
       <c r="C12" s="104">
         <f>SUM(C9:C11)</f>
         <v>-63.399999999999991</v>
@@ -9972,13 +9646,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1">
       <c r="G13" s="104">
         <f>A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12+A13+A14+A15+A16+A17+A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17.25" customHeight="1">
       <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
@@ -9987,32 +9661,32 @@
         <v>#CYCLE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="17.25" customHeight="1">
       <c r="C15" s="104" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="17.25" customHeight="1">
       <c r="C16" s="104" t="str">
         <f>C15</f>
         <v>=(+</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1">
       <c r="C17" s="104" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1">
       <c r="C18" s="104" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1">
       <c r="E19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
         <v>15</v>
@@ -10026,7 +9700,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -10036,7 +9710,7 @@
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1">
       <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
@@ -10050,7 +9724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1">
       <c r="C24" s="16">
         <v>10</v>
       </c>
@@ -10061,7 +9735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1">
       <c r="C25" s="16">
         <v>10.122999999999999</v>
       </c>
@@ -10072,7 +9746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1">
       <c r="B26" s="104" t="s">
         <v>20</v>
       </c>
@@ -10086,7 +9760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1">
       <c r="A27" s="104" t="s">
         <v>22</v>
       </c>
@@ -10103,7 +9777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1">
       <c r="A28" s="104" t="s">
         <v>23</v>
       </c>
@@ -10120,7 +9794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1">
       <c r="A29" s="104" t="s">
         <v>24</v>
       </c>
@@ -10137,7 +9811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1">
       <c r="A30" s="104" t="s">
         <v>25</v>
       </c>
@@ -10154,7 +9828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1">
       <c r="A31" s="104" t="s">
         <v>26</v>
       </c>
@@ -10171,7 +9845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1">
       <c r="A32" s="104" t="s">
         <v>27</v>
       </c>
@@ -10188,7 +9862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="17.25" customHeight="1">
       <c r="A33" s="104" t="s">
         <v>28</v>
       </c>
@@ -10205,7 +9879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="17.25" customHeight="1">
       <c r="A34" s="104" t="s">
         <v>29</v>
       </c>
@@ -10216,7 +9890,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="17.25" customHeight="1">
       <c r="A35" s="104" t="s">
         <v>30</v>
       </c>
@@ -10233,7 +9907,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="50" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10283,7 +9957,7 @@
       <selection sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10295,12 +9969,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10314,7 +9988,7 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
@@ -10334,7 +10008,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10349,7 +10023,7 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
@@ -10359,39 +10033,39 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="106" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B1" s="107" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C1" s="107" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D1" s="107" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E1" s="107" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F1" s="107" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G1" s="107" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H1" s="107" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="I1" s="108" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="J1" s="105" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>4</v>
       </c>
@@ -10402,7 +10076,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E2" s="39">
         <v>45575</v>
@@ -10411,7 +10085,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G2" s="109" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="H2" s="39">
         <v>45292</v>
@@ -10423,7 +10097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>3</v>
       </c>
@@ -10434,7 +10108,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="E3" s="39">
         <v>45576</v>
@@ -10443,19 +10117,19 @@
         <v>0.57638888888888884</v>
       </c>
       <c r="G3" s="109" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="H3" s="39">
         <v>45231</v>
       </c>
       <c r="I3" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="J3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>9</v>
       </c>
@@ -10466,7 +10140,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E4" s="39">
         <v>45574</v>
@@ -10475,7 +10149,7 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="G4" s="109" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="H4" s="39">
         <v>45325</v>
@@ -10487,7 +10161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>5</v>
       </c>
@@ -10498,7 +10172,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="E5" s="39">
         <v>45573</v>
@@ -10507,7 +10181,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="G5" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H5" s="39">
         <v>45084</v>
@@ -10519,7 +10193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>7</v>
       </c>
@@ -10530,7 +10204,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E6" s="39">
         <v>45566</v>
@@ -10539,13 +10213,13 @@
         <v>0.5229166666666667</v>
       </c>
       <c r="G6" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="H6" s="39">
         <v>45420</v>
       </c>
       <c r="I6" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="J6">
         <v>15</v>
@@ -10604,12 +10278,12 @@
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="17.25" customHeight="1">
       <c r="A1" s="104" t="s">
         <v>31</v>
       </c>
@@ -10644,7 +10318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1">
       <c r="A2" s="104" t="s">
         <v>41</v>
       </c>
@@ -10690,7 +10364,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1">
       <c r="A3" s="104" t="s">
         <v>43</v>
       </c>
@@ -10736,7 +10410,7 @@
         <v>1217.7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="17.25" customHeight="1">
       <c r="A4" s="104" t="s">
         <v>45</v>
       </c>
@@ -10782,7 +10456,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1">
       <c r="A5" s="104" t="s">
         <v>47</v>
       </c>
@@ -10828,7 +10502,7 @@
         <v>1246.7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="17.25" customHeight="1">
       <c r="A6" s="104" t="s">
         <v>49</v>
       </c>
@@ -10874,7 +10548,7 @@
         <v>1213.7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="17.25" customHeight="1">
       <c r="A7" s="104" t="s">
         <v>52</v>
       </c>
@@ -10908,7 +10582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="17.25" customHeight="1">
       <c r="A8" s="104" t="s">
         <v>54</v>
       </c>
@@ -10942,7 +10616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="17.25" customHeight="1">
       <c r="A9" s="104" t="s">
         <v>56</v>
       </c>
@@ -10973,7 +10647,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="17.25" customHeight="1">
       <c r="A10" s="104" t="s">
         <v>58</v>
       </c>
@@ -10989,7 +10663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="17.25" customHeight="1">
       <c r="A11" s="104" t="s">
         <v>59</v>
       </c>
@@ -11008,7 +10682,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="17.25" customHeight="1">
       <c r="A12" s="104" t="s">
         <v>61</v>
       </c>
@@ -11039,7 +10713,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="17.25" customHeight="1">
       <c r="A13" s="104" t="s">
         <v>62</v>
       </c>
@@ -11070,7 +10744,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="17.25" customHeight="1">
       <c r="A14" s="104" t="s">
         <v>67</v>
       </c>
@@ -11086,7 +10760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="17.25" customHeight="1">
       <c r="A15" s="104" t="s">
         <v>68</v>
       </c>
@@ -11102,7 +10776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="17.25" customHeight="1">
       <c r="A16" s="104" t="s">
         <v>69</v>
       </c>
@@ -11118,7 +10792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1">
       <c r="A17" s="104" t="s">
         <v>70</v>
       </c>
@@ -11134,7 +10808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1">
       <c r="A18" s="104" t="s">
         <v>71</v>
       </c>
@@ -11150,7 +10824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1">
       <c r="A19" s="104" t="s">
         <v>72</v>
       </c>
@@ -11166,7 +10840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1">
       <c r="A20" s="104" t="s">
         <v>73</v>
       </c>
@@ -11182,7 +10856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1">
       <c r="A21" s="104" t="s">
         <v>74</v>
       </c>
@@ -11198,7 +10872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1">
       <c r="A22" s="104" t="s">
         <v>76</v>
       </c>
@@ -11214,7 +10888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1">
       <c r="A23" s="104" t="s">
         <v>77</v>
       </c>
@@ -11230,7 +10904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="17.25" customHeight="1">
       <c r="A24" s="104" t="s">
         <v>78</v>
       </c>
@@ -11247,7 +10921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="17.25" customHeight="1">
       <c r="A25" s="104" t="s">
         <v>79</v>
       </c>
@@ -11263,7 +10937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="17.25" customHeight="1">
       <c r="A26" s="104" t="s">
         <v>81</v>
       </c>
@@ -11279,7 +10953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="17.25" customHeight="1">
       <c r="A27" s="104" t="s">
         <v>82</v>
       </c>
@@ -11295,7 +10969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="17.25" customHeight="1">
       <c r="A28" s="104" t="s">
         <v>83</v>
       </c>
@@ -11312,7 +10986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="17.25" customHeight="1">
       <c r="A29" s="104" t="s">
         <v>84</v>
       </c>
@@ -11328,7 +11002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17.25" customHeight="1">
       <c r="A30" s="104" t="s">
         <v>85</v>
       </c>
@@ -11344,7 +11018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="17.25" customHeight="1">
       <c r="A31" s="104" t="s">
         <v>86</v>
       </c>
@@ -11360,7 +11034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="17.25" customHeight="1">
       <c r="A32" s="104" t="s">
         <v>87</v>
       </c>
@@ -11376,7 +11050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17.25" customHeight="1">
       <c r="A33" s="104" t="s">
         <v>88</v>
       </c>
@@ -11392,7 +11066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="17.25" customHeight="1">
       <c r="A34" s="104" t="s">
         <v>89</v>
       </c>
@@ -11408,7 +11082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17.25" customHeight="1">
       <c r="A35" s="104" t="s">
         <v>90</v>
       </c>
@@ -11424,7 +11098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="17.25" customHeight="1">
       <c r="A36" s="104" t="s">
         <v>91</v>
       </c>
@@ -11440,7 +11114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="17.25" customHeight="1">
       <c r="A37" s="104" t="s">
         <v>92</v>
       </c>
@@ -11456,7 +11130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="17.25" customHeight="1">
       <c r="A38" s="104" t="s">
         <v>93</v>
       </c>
@@ -11473,7 +11147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="17.25" customHeight="1">
       <c r="A39" s="104" t="s">
         <v>94</v>
       </c>
@@ -11489,7 +11163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="17.25" customHeight="1">
       <c r="A40" s="104" t="s">
         <v>95</v>
       </c>
@@ -11505,7 +11179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="17.25" customHeight="1">
       <c r="A41" s="104" t="s">
         <v>96</v>
       </c>
@@ -11521,7 +11195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="17.25" customHeight="1">
       <c r="A42" s="104" t="s">
         <v>97</v>
       </c>
@@ -11537,7 +11211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="17.25" customHeight="1">
       <c r="A43" s="104" t="s">
         <v>98</v>
       </c>
@@ -11553,7 +11227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="17.25" customHeight="1">
       <c r="A44" s="104" t="s">
         <v>99</v>
       </c>
@@ -11569,7 +11243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="17.25" customHeight="1">
       <c r="A45" s="104" t="s">
         <v>100</v>
       </c>
@@ -11585,7 +11259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="17.25" customHeight="1">
       <c r="A46" s="104" t="s">
         <v>101</v>
       </c>
@@ -11601,7 +11275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="17.25" customHeight="1">
       <c r="A47" s="104" t="s">
         <v>102</v>
       </c>
@@ -11617,7 +11291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="17.25" customHeight="1">
       <c r="A48" s="104" t="s">
         <v>103</v>
       </c>
@@ -11633,7 +11307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="17.25" customHeight="1">
       <c r="A49" s="104" t="s">
         <v>104</v>
       </c>
@@ -11649,7 +11323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="17.25" customHeight="1">
       <c r="A50" s="104" t="s">
         <v>105</v>
       </c>
@@ -11666,7 +11340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="17.25" customHeight="1">
       <c r="A51" s="104" t="s">
         <v>106</v>
       </c>
@@ -11683,7 +11357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="17.25" customHeight="1">
       <c r="A52" s="104" t="s">
         <v>107</v>
       </c>
@@ -11699,7 +11373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1">
       <c r="A53" s="104" t="s">
         <v>108</v>
       </c>
@@ -11715,7 +11389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="17.25" customHeight="1">
       <c r="A54" s="104" t="s">
         <v>109</v>
       </c>
@@ -11731,7 +11405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1">
       <c r="A55" s="104" t="s">
         <v>110</v>
       </c>
@@ -11747,7 +11421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1">
       <c r="A56" s="104" t="s">
         <v>111</v>
       </c>
@@ -11763,7 +11437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1">
       <c r="A57" s="104" t="s">
         <v>112</v>
       </c>
@@ -11779,7 +11453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1">
       <c r="A58" s="104" t="s">
         <v>113</v>
       </c>
@@ -11795,7 +11469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1">
       <c r="A59" s="104" t="s">
         <v>114</v>
       </c>
@@ -11811,7 +11485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1">
       <c r="A60" s="104" t="s">
         <v>115</v>
       </c>
@@ -11827,7 +11501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1">
       <c r="A61" s="104" t="s">
         <v>116</v>
       </c>
@@ -11843,7 +11517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1">
       <c r="A62" s="104" t="s">
         <v>117</v>
       </c>
@@ -11859,7 +11533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="17.25" customHeight="1">
       <c r="A63" s="104" t="s">
         <v>118</v>
       </c>
@@ -11875,7 +11549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="17.25" customHeight="1">
       <c r="A64" s="104" t="s">
         <v>119</v>
       </c>
@@ -11891,7 +11565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="17.25" customHeight="1">
       <c r="A65" s="104" t="s">
         <v>120</v>
       </c>
@@ -11907,7 +11581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="17.25" customHeight="1">
       <c r="A66" s="104" t="s">
         <v>121</v>
       </c>
@@ -11923,7 +11597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="17.25" customHeight="1">
       <c r="A67" s="104" t="s">
         <v>122</v>
       </c>
@@ -11939,7 +11613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="17.25" customHeight="1">
       <c r="A68" s="104" t="s">
         <v>123</v>
       </c>
@@ -11955,7 +11629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="17.25" customHeight="1">
       <c r="A69" s="104" t="s">
         <v>125</v>
       </c>
@@ -11971,7 +11645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="17.25" customHeight="1">
       <c r="A70" s="104" t="s">
         <v>127</v>
       </c>
@@ -11987,7 +11661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="17.25" customHeight="1">
       <c r="A71" s="104" t="s">
         <v>129</v>
       </c>
@@ -12003,7 +11677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="17.25" customHeight="1">
       <c r="A72" s="104" t="s">
         <v>130</v>
       </c>
@@ -12019,7 +11693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="17.25" customHeight="1">
       <c r="A73" s="104" t="s">
         <v>131</v>
       </c>
@@ -12035,7 +11709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="17.25" customHeight="1">
       <c r="A74" s="104" t="s">
         <v>132</v>
       </c>
@@ -12051,7 +11725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="17.25" customHeight="1">
       <c r="A75" s="104" t="s">
         <v>133</v>
       </c>
@@ -12067,7 +11741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="17.25" customHeight="1">
       <c r="A76" s="104" t="s">
         <v>134</v>
       </c>
@@ -12083,7 +11757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="17.25" customHeight="1">
       <c r="A77" s="104" t="s">
         <v>135</v>
       </c>
@@ -12099,7 +11773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="17.25" customHeight="1">
       <c r="A78" s="104" t="s">
         <v>136</v>
       </c>
@@ -12115,7 +11789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="17.25" customHeight="1">
       <c r="A79" s="104" t="s">
         <v>137</v>
       </c>
@@ -12131,7 +11805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="17.25" customHeight="1">
       <c r="A80" s="104" t="s">
         <v>138</v>
       </c>
@@ -12147,7 +11821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="17.25" customHeight="1">
       <c r="A81" s="104" t="s">
         <v>139</v>
       </c>
@@ -12163,7 +11837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="17.25" customHeight="1">
       <c r="A82" s="104" t="s">
         <v>141</v>
       </c>
@@ -12179,7 +11853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="17.25" customHeight="1">
       <c r="A83" s="104" t="s">
         <v>142</v>
       </c>
@@ -12195,7 +11869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="17.25" customHeight="1">
       <c r="A84" s="104" t="s">
         <v>143</v>
       </c>
@@ -12211,7 +11885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="17.25" customHeight="1">
       <c r="A85" s="104" t="s">
         <v>144</v>
       </c>
@@ -12227,7 +11901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="17.25" customHeight="1">
       <c r="A86" s="104" t="s">
         <v>146</v>
       </c>
@@ -12243,7 +11917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="17.25" customHeight="1">
       <c r="A87" s="104" t="s">
         <v>147</v>
       </c>
@@ -12259,7 +11933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="17.25" customHeight="1">
       <c r="A88" s="104" t="s">
         <v>148</v>
       </c>
@@ -12275,7 +11949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="17.25" customHeight="1">
       <c r="A89" s="104" t="s">
         <v>149</v>
       </c>
@@ -12291,7 +11965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="17.25" customHeight="1">
       <c r="A90" s="104" t="s">
         <v>150</v>
       </c>
@@ -12307,7 +11981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="17.25" customHeight="1">
       <c r="A91" s="104" t="s">
         <v>151</v>
       </c>
@@ -12323,7 +11997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1">
       <c r="A92" s="104" t="s">
         <v>152</v>
       </c>
@@ -12339,7 +12013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1">
       <c r="A93" s="104" t="s">
         <v>153</v>
       </c>
@@ -12355,7 +12029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1">
       <c r="A94" s="104" t="s">
         <v>154</v>
       </c>
@@ -12371,7 +12045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1">
       <c r="A95" s="104" t="s">
         <v>155</v>
       </c>
@@ -12387,7 +12061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1">
       <c r="A96" s="104" t="s">
         <v>156</v>
       </c>
@@ -12403,7 +12077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="17.25" customHeight="1">
       <c r="A97" s="104" t="s">
         <v>157</v>
       </c>
@@ -12419,7 +12093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="17.25" customHeight="1">
       <c r="A98" s="104" t="s">
         <v>158</v>
       </c>
@@ -12435,7 +12109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="17.25" customHeight="1">
       <c r="A99" s="104" t="s">
         <v>159</v>
       </c>
@@ -12451,20 +12125,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="17.25" customHeight="1">
       <c r="A100" s="104" t="s">
         <v>160</v>
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45989.427180092593</v>
+        <v>46042.425886574078</v>
       </c>
       <c r="D100" s="104">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="17.25" customHeight="1">
       <c r="A101" s="104" t="s">
         <v>161</v>
       </c>
@@ -12480,7 +12154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="17.25" customHeight="1">
       <c r="A102" s="104" t="s">
         <v>162</v>
       </c>
@@ -12496,7 +12170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="17.25" customHeight="1">
       <c r="A103" s="104" t="s">
         <v>163</v>
       </c>
@@ -12512,7 +12186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="17.25" customHeight="1">
       <c r="A104" s="104" t="s">
         <v>164</v>
       </c>
@@ -12528,7 +12202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="17.25" customHeight="1">
       <c r="A105" s="104" t="s">
         <v>165</v>
       </c>
@@ -12544,7 +12218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="17.25" customHeight="1">
       <c r="A106" s="104" t="s">
         <v>166</v>
       </c>
@@ -12560,7 +12234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="17.25" customHeight="1">
       <c r="A107" s="104" t="s">
         <v>167</v>
       </c>
@@ -12576,7 +12250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="17.25" customHeight="1">
       <c r="A108" s="104" t="s">
         <v>168</v>
       </c>
@@ -12592,7 +12266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="17.25" customHeight="1">
       <c r="A109" s="104" t="s">
         <v>169</v>
       </c>
@@ -12608,7 +12282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="17.25" customHeight="1">
       <c r="A110" s="104" t="s">
         <v>170</v>
       </c>
@@ -12624,7 +12298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="17.25" customHeight="1">
       <c r="A111" s="104" t="s">
         <v>171</v>
       </c>
@@ -12640,12 +12314,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="17.25" customHeight="1">
       <c r="A112" s="104"/>
       <c r="B112" s="104"/>
       <c r="D112" s="104"/>
     </row>
-    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="17.25" customHeight="1">
       <c r="A113" s="104" t="s">
         <v>172</v>
       </c>
@@ -12661,7 +12335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="17.25" customHeight="1">
       <c r="A114" s="104" t="s">
         <v>173</v>
       </c>
@@ -12677,7 +12351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="17.25" customHeight="1">
       <c r="A115" s="104" t="s">
         <v>175</v>
       </c>
@@ -12693,7 +12367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="17.25" customHeight="1">
       <c r="A116" s="104" t="s">
         <v>177</v>
       </c>
@@ -12709,7 +12383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="17.25" customHeight="1">
       <c r="A117" s="104" t="s">
         <v>178</v>
       </c>
@@ -12725,7 +12399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="17.25" customHeight="1">
       <c r="A118" s="104" t="s">
         <v>179</v>
       </c>
@@ -12741,7 +12415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="17.25" customHeight="1">
       <c r="A119" s="104" t="s">
         <v>180</v>
       </c>
@@ -12757,7 +12431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="17.25" customHeight="1">
       <c r="A120" s="104" t="s">
         <v>181</v>
       </c>
@@ -12773,7 +12447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="17.25" customHeight="1">
       <c r="A121" s="104" t="s">
         <v>182</v>
       </c>
@@ -12789,7 +12463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="17.25" customHeight="1">
       <c r="A122" s="104" t="s">
         <v>183</v>
       </c>
@@ -12805,7 +12479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="17.25" customHeight="1">
       <c r="A123" s="104" t="s">
         <v>184</v>
       </c>
@@ -12821,7 +12495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="17.25" customHeight="1">
       <c r="A124" s="104" t="s">
         <v>185</v>
       </c>
@@ -12837,7 +12511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="17.25" customHeight="1">
       <c r="A125" s="104" t="s">
         <v>186</v>
       </c>
@@ -12853,7 +12527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="17.25" customHeight="1">
       <c r="A126" s="104" t="s">
         <v>187</v>
       </c>
@@ -12869,7 +12543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="17.25" customHeight="1">
       <c r="A127" s="104" t="s">
         <v>188</v>
       </c>
@@ -12885,7 +12559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="17.25" customHeight="1">
       <c r="A128" s="104" t="s">
         <v>189</v>
       </c>
@@ -12901,7 +12575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="17.25" customHeight="1">
       <c r="A129" s="104" t="s">
         <v>190</v>
       </c>
@@ -12917,7 +12591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="17.25" customHeight="1">
       <c r="A130" s="104" t="s">
         <v>191</v>
       </c>
@@ -12933,7 +12607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="17.25" customHeight="1">
       <c r="A131" s="104" t="s">
         <v>192</v>
       </c>
@@ -12949,7 +12623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="17.25" customHeight="1">
       <c r="A132" s="104" t="s">
         <v>193</v>
       </c>
@@ -12965,7 +12639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="17.25" customHeight="1">
       <c r="A133" s="104" t="s">
         <v>194</v>
       </c>
@@ -12981,7 +12655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="17.25" customHeight="1">
       <c r="A134" s="104" t="s">
         <v>195</v>
       </c>
@@ -12997,7 +12671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="17.25" customHeight="1">
       <c r="A135" s="104" t="s">
         <v>196</v>
       </c>
@@ -13013,7 +12687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="17.25" customHeight="1">
       <c r="A136" s="104" t="s">
         <v>198</v>
       </c>
@@ -13029,7 +12703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="17.25" customHeight="1">
       <c r="A137" s="104" t="s">
         <v>199</v>
       </c>
@@ -13045,7 +12719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="17.25" customHeight="1">
       <c r="A138" s="104" t="s">
         <v>200</v>
       </c>
@@ -13061,7 +12735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="17.25" customHeight="1">
       <c r="A139" s="104" t="s">
         <v>201</v>
       </c>
@@ -13077,7 +12751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="17.25" customHeight="1">
       <c r="A140" s="104" t="s">
         <v>202</v>
       </c>
@@ -13093,7 +12767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="17.25" customHeight="1">
       <c r="A141" s="104" t="s">
         <v>203</v>
       </c>
@@ -13109,7 +12783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="17.25" customHeight="1">
       <c r="A142" s="104" t="s">
         <v>205</v>
       </c>
@@ -13125,7 +12799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="17.25" customHeight="1">
       <c r="A143" s="104" t="s">
         <v>206</v>
       </c>
@@ -13141,20 +12815,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="17.25" customHeight="1">
       <c r="A144" s="104" t="s">
         <v>207</v>
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45989</v>
+        <v>46042</v>
       </c>
       <c r="D144" s="104">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="17.25" customHeight="1">
       <c r="A145" s="104" t="s">
         <v>208</v>
       </c>
@@ -13170,7 +12844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="17.25" customHeight="1">
       <c r="A146" s="104" t="s">
         <v>210</v>
       </c>
@@ -13186,7 +12860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="17.25" customHeight="1">
       <c r="A147" s="104" t="s">
         <v>211</v>
       </c>
@@ -13202,7 +12876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="17.25" customHeight="1">
       <c r="A148" s="104" t="s">
         <v>213</v>
       </c>
@@ -13218,7 +12892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="17.25" customHeight="1">
       <c r="A149" s="104" t="s">
         <v>214</v>
       </c>
@@ -13234,7 +12908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" ht="17.25" customHeight="1">
       <c r="A150" s="104" t="s">
         <v>215</v>
       </c>
@@ -13250,7 +12924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="17.25" customHeight="1">
       <c r="A151" s="104" t="s">
         <v>216</v>
       </c>
@@ -13266,7 +12940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="17.25" customHeight="1">
       <c r="A152" s="104" t="s">
         <v>217</v>
       </c>
@@ -13282,7 +12956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="17.25" customHeight="1">
       <c r="A153" s="104" t="s">
         <v>218</v>
       </c>
@@ -13298,7 +12972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" ht="17.25" customHeight="1">
       <c r="A154" s="104" t="s">
         <v>219</v>
       </c>
@@ -13315,7 +12989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="17.25" customHeight="1">
       <c r="A155" s="104" t="s">
         <v>220</v>
       </c>
@@ -13331,7 +13005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="17.25" customHeight="1">
       <c r="A156" s="104" t="s">
         <v>221</v>
       </c>
@@ -13347,7 +13021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" ht="17.25" customHeight="1">
       <c r="A157" s="104" t="s">
         <v>222</v>
       </c>
@@ -13363,7 +13037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" ht="17.25" customHeight="1">
       <c r="A158" s="104" t="s">
         <v>223</v>
       </c>
@@ -13379,7 +13053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="17.25" customHeight="1">
       <c r="A159" s="104" t="s">
         <v>224</v>
       </c>
@@ -13395,7 +13069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" ht="17.25" customHeight="1">
       <c r="A160" s="104" t="s">
         <v>225</v>
       </c>
@@ -13411,7 +13085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" ht="17.25" customHeight="1">
       <c r="A161" s="104" t="s">
         <v>226</v>
       </c>
@@ -13427,7 +13101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="17.25" customHeight="1">
       <c r="A162" s="104" t="s">
         <v>227</v>
       </c>
@@ -13443,7 +13117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" ht="17.25" customHeight="1">
       <c r="A163" s="104" t="s">
         <v>229</v>
       </c>
@@ -13461,10 +13135,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13484,7 +13158,7 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
@@ -13494,17 +13168,17 @@
     <col min="15" max="18" width="9.140625" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>230</v>
       </c>
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="114" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="115"/>
+      <c r="E1" s="114"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -13512,19 +13186,19 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="D3" s="85" t="s">
         <v>235</v>
       </c>
@@ -13532,43 +13206,43 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="75" customHeight="1">
       <c r="A5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" outlineLevel="1"/>
+    <row r="11" spans="1:8" outlineLevel="1"/>
+    <row r="12" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="13" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="14" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="15" spans="1:8" outlineLevel="1" collapsed="1"/>
+    <row r="16" spans="1:8" outlineLevel="1"/>
+    <row r="17" spans="1:2" outlineLevel="1"/>
+    <row r="18" spans="1:2" outlineLevel="1"/>
+    <row r="30" spans="1:2">
       <c r="A30" cm="1">
         <f t="array" aca="1" ref="A30:B31" ca="1">_xlfn.RANDARRAY(2,2)</f>
-        <v>0.38411710219623751</v>
+        <v>0.88429772806393081</v>
       </c>
       <c r="B30">
         <f ca="1"/>
-        <v>9.794149803384844E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.90996014711511952</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31">
         <f ca="1"/>
-        <v>0.66351595791263507</v>
+        <v>0.73547363754464601</v>
       </c>
       <c r="B31">
         <f ca="1"/>
-        <v>5.0911295821026714E-2</v>
+        <v>0.41617961757033295</v>
       </c>
     </row>
   </sheetData>
@@ -13592,14 +13266,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1">
       <c r="A1" s="68" t="s">
         <v>239</v>
       </c>
@@ -13621,7 +13295,7 @@
       </c>
       <c r="M1" s="36"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="40" t="s">
         <v>245</v>
       </c>
@@ -13647,7 +13321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="41" t="s">
         <v>252</v>
       </c>
@@ -13670,7 +13344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15">
       <c r="A4" s="42" t="s">
         <v>256</v>
       </c>
@@ -13696,7 +13370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="43" t="s">
         <v>262</v>
       </c>
@@ -13716,7 +13390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="44" t="s">
         <v>266</v>
       </c>
@@ -13739,7 +13413,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="45" t="s">
         <v>271</v>
       </c>
@@ -13759,7 +13433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="21">
       <c r="A8" s="46" t="s">
         <v>275</v>
       </c>
@@ -13782,7 +13456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="47" t="s">
         <v>280</v>
       </c>
@@ -13799,7 +13473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="48" t="s">
         <v>283</v>
       </c>
@@ -13807,7 +13481,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1">
       <c r="A11" s="49" t="s">
         <v>285</v>
       </c>
@@ -13816,7 +13490,7 @@
       </c>
       <c r="F11" s="36"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1">
       <c r="A12" s="50" t="s">
         <v>287</v>
       </c>
@@ -13830,7 +13504,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A13" s="51" t="s">
         <v>290</v>
       </c>
@@ -13841,7 +13515,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A14" s="52" t="s">
         <v>291</v>
       </c>
@@ -13855,7 +13529,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A15" s="53" t="s">
         <v>293</v>
       </c>
@@ -13866,7 +13540,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
       <c r="A16" s="54" t="s">
         <v>294</v>
       </c>
@@ -13880,12 +13554,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.5" thickBot="1">
       <c r="A17" s="55" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.5" thickBot="1">
       <c r="A18" s="74" t="s">
         <v>297</v>
       </c>
@@ -13897,7 +13571,7 @@
       </c>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13.5" thickBot="1">
       <c r="A19" s="75" t="s">
         <v>300</v>
       </c>
@@ -13908,7 +13582,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="51.75" thickBot="1">
       <c r="A20" s="76" t="s">
         <v>303</v>
       </c>
@@ -13922,12 +13596,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.5" thickBot="1">
       <c r="A21" s="77" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.5" thickBot="1">
       <c r="A22" s="78" t="s">
         <v>307</v>
       </c>
@@ -13936,13 +13610,13 @@
       </c>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.5" thickBot="1">
       <c r="A23" s="79" t="s">
         <v>309</v>
       </c>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="A24" s="80" t="s">
         <v>310</v>
       </c>
@@ -13951,20 +13625,20 @@
       </c>
       <c r="E24" s="21"/>
     </row>
-    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C26" s="67" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C28" s="88" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="13.5" thickTop="1"/>
+    <row r="30" spans="1:6">
       <c r="C30" s="87" t="s">
         <v>314</v>
       </c>
@@ -13979,17 +13653,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D919E811-4385-4D35-A19E-3B7E0E659A89}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.5" thickBot="1">
       <c r="A1" s="37" t="s">
         <v>315</v>
       </c>
@@ -14006,7 +13680,7 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="38" t="s">
         <v>319</v>
       </c>
@@ -14029,7 +13703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="38" t="s">
         <v>321</v>
       </c>
@@ -14052,7 +13726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="38" t="s">
         <v>325</v>
       </c>
@@ -14072,7 +13746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="38" t="s">
         <v>328</v>
       </c>
@@ -14096,7 +13770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="38" t="s">
         <v>330</v>
       </c>
@@ -14119,7 +13793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="38" t="s">
         <v>333</v>
       </c>
@@ -14145,7 +13819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="38" t="s">
         <v>337</v>
       </c>
@@ -14156,7 +13830,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="38" t="s">
         <v>339</v>
       </c>
@@ -14165,7 +13839,7 @@
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.5" thickBot="1">
       <c r="A10" s="38" t="s">
         <v>340</v>
       </c>
@@ -14183,7 +13857,7 @@
       <c r="I10" s="36"/>
       <c r="J10" s="36"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="38" t="s">
         <v>342</v>
       </c>
@@ -14206,13 +13880,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="38" t="s">
         <v>344</v>
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45989</v>
+        <v>46042</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -14231,7 +13905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="38" t="s">
         <v>346</v>
       </c>
@@ -14254,7 +13928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="38" t="s">
         <v>348</v>
       </c>
@@ -14280,7 +13954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="38" t="s">
         <v>350</v>
       </c>
@@ -14300,7 +13974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="38" t="s">
         <v>352</v>
       </c>
@@ -14323,7 +13997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="38" t="s">
         <v>354</v>
       </c>
@@ -14346,7 +14020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="38" t="s">
         <v>356</v>
       </c>
@@ -14369,7 +14043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="38" t="s">
         <v>358</v>
       </c>
@@ -14392,7 +14066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="38" t="s">
         <v>360</v>
       </c>
@@ -14415,7 +14089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="38" t="s">
         <v>362</v>
       </c>
@@ -14441,7 +14115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="38" t="s">
         <v>364</v>
       </c>
@@ -14467,7 +14141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="38" t="s">
         <v>366</v>
       </c>
@@ -14493,7 +14167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="G24" s="34" t="s">
         <v>368</v>
       </c>
@@ -14510,7 +14184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="38" t="s">
         <v>369</v>
       </c>
@@ -14536,7 +14210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="G26" s="34" t="s">
         <v>371</v>
       </c>
@@ -14556,7 +14230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="21" t="s">
         <v>372</v>
       </c>
@@ -14582,7 +14256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="G28" s="34" t="s">
         <v>374</v>
       </c>
@@ -14602,9 +14276,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="38" t="s">
-        <v>440</v>
+        <v>375</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -14613,7 +14287,7 @@
         <v>10</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H29">
         <v>5</v>
@@ -14631,9 +14305,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="G30" s="34" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H30">
         <v>5</v>
@@ -14651,9 +14325,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="13.5" thickBot="1">
       <c r="G31" s="35" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H31" s="36">
         <v>5</v>
@@ -14665,9 +14339,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="G32" s="34" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H32">
         <v>5</v>
@@ -14679,9 +14353,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:10">
       <c r="G33" s="34" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H33">
         <v>5</v>
@@ -14693,9 +14367,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:10">
       <c r="G34" s="34" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H34">
         <v>5</v>
@@ -14707,9 +14381,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:10">
       <c r="G35" s="34" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H35">
         <v>5</v>
@@ -14721,9 +14395,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:10">
       <c r="G36" s="34" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H36">
         <v>5</v>
@@ -14735,9 +14409,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:10">
       <c r="G37" s="34" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H37">
         <v>5</v>
@@ -14749,110 +14423,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="7:10">
       <c r="G39" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="47" priority="59">
+    <cfRule type="expression" dxfId="41" priority="59">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="45" priority="115"/>
+    <cfRule type="aboveAverage" dxfId="39" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="44" priority="74" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="38" priority="74" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="43" priority="72">
+    <cfRule type="containsBlanks" dxfId="37" priority="72">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="42" priority="71">
+    <cfRule type="containsErrors" dxfId="36" priority="71">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="41" priority="70" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="35" priority="70" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="40" priority="68" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="34" priority="68" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="67">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="67">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="38" priority="66">
+    <cfRule type="notContainsErrors" dxfId="32" priority="66">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="37" priority="65" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="31" priority="65" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="36" priority="64" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="30" priority="64" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="24" priority="116" percent="1" bottom="1" rank="50"/>
+    <cfRule type="top10" dxfId="29" priority="116" percent="1" bottom="1" rank="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="35" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="34" priority="57" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="57" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -14886,16 +14560,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="between">
       <formula>$B$23</formula>
       <formula>2+2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="26" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="25" priority="97"/>
+    <cfRule type="uniqueValues" dxfId="18" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="45">
@@ -15323,7 +14997,7 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
@@ -15335,12 +15009,12 @@
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15">
       <c r="C3" s="17" t="s">
         <v>35</v>
       </c>
@@ -15348,25 +15022,25 @@
         <v>36</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="104" t="s">
         <v>42</v>
       </c>
@@ -15397,7 +15071,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="C5" s="104" t="s">
         <v>44</v>
       </c>
@@ -15428,9 +15102,9 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="C6" s="104" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D6" s="104">
         <f>SUBTOTAL(109,Table3[Age])</f>
@@ -15461,9 +15135,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="B8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -15472,22 +15146,22 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="J8" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="C9">
         <v>3</v>
       </c>
@@ -15515,18 +15189,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="B11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C11" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D11" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="C12">
         <v>3</v>
       </c>
@@ -15534,9 +15208,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="B14" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -15545,7 +15219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="C15">
         <v>3</v>
       </c>
@@ -15553,9 +15227,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -15564,7 +15238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="C18">
         <v>3</v>
       </c>
@@ -15572,9 +15246,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -15583,7 +15257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="C21">
         <v>3</v>
       </c>
@@ -15591,9 +15265,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -15602,7 +15276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4">
       <c r="C24">
         <v>3</v>
       </c>
@@ -15610,9 +15284,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -15621,7 +15295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4">
       <c r="C27">
         <v>3</v>
       </c>
@@ -15629,45 +15303,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4">
       <c r="C28" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D28">
         <f>SUBTOTAL(109,Table4910[Column2])</f>
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C30" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D30" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" hidden="1">
       <c r="C31" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D31" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
       <c r="C32" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D32" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -15695,7 +15369,7 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -15716,9 +15390,9 @@
     <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15">
       <c r="A1" s="92" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -15726,7 +15400,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="104"/>
       <c r="B2" s="104"/>
       <c r="C2" s="104"/>
@@ -15734,21 +15408,21 @@
       <c r="E2" s="104"/>
       <c r="F2" s="104"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="104"/>
       <c r="B3" s="104"/>
       <c r="C3" s="89" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D3" s="89" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="104"/>
       <c r="B4" s="104"/>
       <c r="C4" s="89" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D4">
         <v>12.1</v>
@@ -15775,10 +15449,10 @@
         <v>12052</v>
       </c>
       <c r="L4" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="104"/>
       <c r="B5" s="104"/>
       <c r="C5" s="90" t="s">
@@ -15791,7 +15465,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="104"/>
       <c r="B6" s="104"/>
       <c r="C6" s="91">
@@ -15804,7 +15478,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="104"/>
       <c r="B7" s="104"/>
       <c r="C7" s="90" t="s">
@@ -15817,7 +15491,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="104"/>
       <c r="B8" s="104"/>
       <c r="C8" s="91">
@@ -15830,7 +15504,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="104"/>
       <c r="B9" s="104"/>
       <c r="C9" s="90" t="s">
@@ -15843,7 +15517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="104"/>
       <c r="B10" s="104"/>
       <c r="C10" s="91">
@@ -15856,7 +15530,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="C11" s="90" t="s">
         <v>44</v>
       </c>
@@ -15867,7 +15541,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="C12" s="91">
         <v>23000</v>
       </c>
@@ -15878,7 +15552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="C13" s="90" t="s">
         <v>50</v>
       </c>
@@ -15889,7 +15563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="C14" s="91">
         <v>2</v>
       </c>
@@ -15900,7 +15574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="C15" s="90" t="s">
         <v>48</v>
       </c>
@@ -15911,7 +15585,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="C16" s="91">
         <v>50024</v>
       </c>
@@ -15922,7 +15596,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:12">
       <c r="C17" s="90" t="s">
         <v>53</v>
       </c>
@@ -15933,7 +15607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:12">
       <c r="C18" s="91">
         <v>189576</v>
       </c>
@@ -15944,7 +15618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:12">
       <c r="C19" s="90" t="s">
         <v>57</v>
       </c>
@@ -15955,7 +15629,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:12">
       <c r="C20" s="91">
         <v>5000</v>
       </c>
@@ -15966,9 +15640,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:12">
       <c r="C21" s="90" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D21">
         <v>9</v>
@@ -16008,35 +15682,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47BF70-BA80-4124-B359-67CBCB635390}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B2" s="104"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -16053,25 +15727,25 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="51">
       <c r="A1" s="99" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B7" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -16079,7 +15753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -16087,7 +15761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -16095,7 +15769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -16103,7 +15777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
[IMP] named ranges: add support of xlsx import/export
This commit introduces the support for named ranges in the import and
export of XLSX files.

Task: 5462359
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\odoo\spreadsheet\tests\__xlsx__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A476F739-B139-4713-A5CB-3C0E11EABA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2670164-D2FF-4FC4-8346-4E80CDC15C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="18240" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,14 @@
   <externalReferences>
     <externalReference r:id="rId15"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="My_Named_Range">jestMiscTest!$A$8:$B$10</definedName>
+    <definedName name="Table_Col_Named_Range">Table10[Col1]</definedName>
+    <definedName name="Table_Named_Range">Table10[]</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +60,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2372,7 +2377,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="47">
     <dxf>
       <font>
         <b val="0"/>
@@ -2584,194 +2589,6 @@
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
@@ -2783,207 +2600,6 @@
           <bgColor theme="9"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3344,8 +2960,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{33B8EB55-D8D8-4B00-B5CF-C84A8AC9E775}">
-      <tableStyleElement type="wholeTable" dxfId="70"/>
-      <tableStyleElement type="firstRowStripe" dxfId="69"/>
+      <tableStyleElement type="wholeTable" dxfId="46"/>
+      <tableStyleElement type="firstRowStripe" dxfId="45"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -9230,7 +8846,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -9380,7 +8996,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="68" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9392,22 +9008,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="29">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10233,7 +9849,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="50" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12457,7 +12073,7 @@
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45989.427180092593</v>
+        <v>46029.480459375001</v>
       </c>
       <c r="D100" s="104">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
@@ -13147,7 +12763,7 @@
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45989</v>
+        <v>46029</v>
       </c>
       <c r="D144" s="104">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
@@ -13461,10 +13077,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13554,21 +13170,21 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" cm="1">
         <f t="array" aca="1" ref="A30:B31" ca="1">_xlfn.RANDARRAY(2,2)</f>
-        <v>0.38411710219623751</v>
+        <v>0.41590783928391839</v>
       </c>
       <c r="B30">
         <f ca="1"/>
-        <v>9.794149803384844E-2</v>
+        <v>0.76978102266325354</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <f ca="1"/>
-        <v>0.66351595791263507</v>
+        <v>0.97897293827371779</v>
       </c>
       <c r="B31">
         <f ca="1"/>
-        <v>5.0911295821026714E-2</v>
+        <v>0.59326442241169897</v>
       </c>
     </row>
   </sheetData>
@@ -13979,7 +13595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D919E811-4385-4D35-A19E-3B7E0E659A89}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -14212,7 +13828,7 @@
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45989</v>
+        <v>46029</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -14755,104 +14371,104 @@
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="47" priority="59">
+    <cfRule type="expression" dxfId="23" priority="59">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="47" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="45" priority="115"/>
+    <cfRule type="aboveAverage" dxfId="21" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="44" priority="74" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="20" priority="74" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="43" priority="72">
+    <cfRule type="containsBlanks" dxfId="19" priority="72">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="42" priority="71">
+    <cfRule type="containsErrors" dxfId="18" priority="71">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="41" priority="70" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="17" priority="70" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="40" priority="68" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="16" priority="68" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="67">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="67">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="38" priority="66">
+    <cfRule type="notContainsErrors" dxfId="14" priority="66">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="37" priority="65" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="13" priority="65" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="36" priority="64" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="12" priority="64" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="24" priority="116" percent="1" bottom="1" rank="50"/>
+    <cfRule type="top10" dxfId="11" priority="116" percent="1" bottom="1" rank="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="35" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="34" priority="57" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="57" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -14886,16 +14502,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>$B$23</formula>
       <formula>2+2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="26" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="25" priority="97"/>
+    <cfRule type="uniqueValues" dxfId="0" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="45">
@@ -16047,15 +15663,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE31E21-0350-44E7-AF13-4CA140505B30}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
         <v>421</v>
       </c>
@@ -16063,7 +15679,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>407</v>
       </c>
@@ -16071,7 +15687,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -16079,7 +15695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -16087,27 +15703,119 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="M10" cm="1">
+        <f t="array" ref="M10:N14">Table10[]</f>
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f>_xlfn.CONCAT("This formulas uses a named range ", SUM(My_Named_Range))</f>
+        <v>This formulas uses a named range 12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f>_xlfn.CONCAT("This formulas uses a full table named range ", SUM(Table_Named_Range))</f>
+        <v>This formulas uses a full table named range 30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f>_xlfn.CONCAT("This formulas uses a partial table named range ", SUM(Table_Col_Named_Range))</f>
+        <v>This formulas uses a partial table named range 15</v>
+      </c>
+      <c r="L17" cm="1">
+        <f t="array" ref="L17:M21">Table_Named_Range</f>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <v>5</v>
+      </c>
+      <c r="M21">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FIX] data validation: import formula from excel
When importing a data validation rule with formulas
the "=" was missing after the import

Task: 4975550
</commit_message>
<xml_diff>
--- a/tests/__xlsx__/xlsx_demo_data.xlsx
+++ b/tests/__xlsx__/xlsx_demo_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhrutik Patel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DA6F05-B302-48AE-B11C-1FB2528D58DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{880E0E36-3FD6-4555-B701-A081A5B535D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,9 @@
   <externalReferences>
     <externalReference r:id="rId15"/>
   </externalReferences>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId16"/>
+    <pivotCache cacheId="5782" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,6 +46,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="442">
   <si>
     <t>CF =42</t>
   </si>
@@ -1201,6 +1202,9 @@
   </si>
   <si>
     <t>5Rating</t>
+  </si>
+  <si>
+    <t>CF with formulas</t>
   </si>
   <si>
     <t>5Quarters</t>
@@ -1375,6 +1379,9 @@
     <t>Custom Formula</t>
   </si>
   <si>
+    <t>Decimal with formula</t>
+  </si>
+  <si>
     <t>option1</t>
   </si>
   <si>
@@ -1397,9 +1404,6 @@
   </si>
   <si>
     <t>A1234556</t>
-  </si>
-  <si>
-    <t>CF with formulas</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1418,7 @@
     <numFmt numFmtId="168" formatCode="#,##0&quot; EUR €&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;€&quot;#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2208,7 +2212,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2414,7 +2418,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2427,13 +2430,169 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1493241F-B85D-4F84-BBA0-86191B8FD032}"/>
   </cellStyles>
   <dxfs count="47">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike/>
+        <u/>
+        <color theme="7"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="lightTrellis">
+          <fgColor theme="4"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2847,157 +3006,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike/>
-        <u/>
-        <color theme="7"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="lightTrellis">
-          <fgColor theme="4"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -3041,7 +3049,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3642,7 +3650,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -4074,7 +4082,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -4692,7 +4700,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5058,7 +5066,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -5357,7 +5365,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5774,7 +5782,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6176,7 +6184,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6466,7 +6474,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -7933,7 +7941,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9B3CE3F5-58D8-48A3-B9C6-24D1506C9F5C}" name="PivotTable1" cacheId="5782" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:L21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -8083,7 +8091,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}" name="Table3" displayName="Table3" ref="C3:J6" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="C3:J5" xr:uid="{09C35CC7-7259-4A97-8FEA-EDB47375DF08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -8095,22 +8103,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35">
+    <tableColumn id="1" xr3:uid="{C4EE018E-238B-42BA-9035-DB01FA5420D3}" name="Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C1F6911F-9482-4C98-BBFB-21D9CAA66DA4}" name="Age" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{3CE9F5DA-0A57-4696-B4E0-53601C3B7798}" name="Rank" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{34912838-665C-4472-B558-25990E5B148D}" name="Rank+Age =E4+D4" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[Rank]]+Table3[[#This Row],[Age]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33">
+    <tableColumn id="7" xr3:uid="{89D90022-7073-4067-BAF8-1587D27C4AFB}" name="Data =SUM(E4:E5)" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="7">
       <calculatedColumnFormula>SUM(Table3[Rank])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
+    <tableColumn id="8" xr3:uid="{B2A7E5BB-A379-492B-9484-72F2FD1FF3A0}" name="All =SUM(E3:E6)" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5">
       <calculatedColumnFormula>SUM(Table3[[#All],[Rank]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="29">
+    <tableColumn id="9" xr3:uid="{3C532A69-E4BC-4A20-A922-4BCAA0D3FEC9}" name="Totals =E6" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3">
       <calculatedColumnFormula>Table3[[#Totals],[Rank]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27">
+    <tableColumn id="10" xr3:uid="{35E9E9C3-9148-468A-85B6-19290CEB6F00}" name="Headers =E3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
       <calculatedColumnFormula>Table3[[#Headers],[Rank]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8536,7 +8544,7 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -8545,7 +8553,7 @@
     <col min="6" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1">
       <c r="A1" s="21"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -8554,7 +8562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="27.75">
       <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
@@ -8567,25 +8575,25 @@
       <c r="H2" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="119"/>
+      <c r="I2" s="125"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1">
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="117">
         <v>8</v>
       </c>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="120">
+      <c r="K3" s="119">
         <v>5</v>
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -8598,50 +8606,50 @@
       <c r="G4" s="117">
         <v>9</v>
       </c>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="125"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="121"/>
+      <c r="K4" s="120"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1">
       <c r="C5" s="117">
         <v>42</v>
       </c>
       <c r="G5" s="117">
         <v>15</v>
       </c>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="125"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="121"/>
+      <c r="K5" s="120"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1">
       <c r="G6" s="117">
         <v>22</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="K6" s="121"/>
+      <c r="K6" s="120"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1">
       <c r="C7" s="117">
         <v>3</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="121"/>
+      <c r="K7" s="120"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1">
       <c r="G8" s="117">
         <v>30</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="122"/>
+      <c r="K8" s="121"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17.25" customHeight="1">
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
@@ -8651,7 +8659,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1">
       <c r="C10" s="117">
         <f>SUM(C4:C7)</f>
         <v>57.4</v>
@@ -8660,13 +8668,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17.25" customHeight="1">
       <c r="C11" s="117">
         <f>-(3+C7*SUM(C4:C7))</f>
         <v>-175.2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="17.25" customHeight="1">
       <c r="C12" s="117">
         <f>SUM(C9:C11)</f>
         <v>-63.399999999999991</v>
@@ -8675,13 +8683,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1">
       <c r="G13" s="117">
         <f>A1+A2+A3+A4+A5+A6+A7+A8+A9+A10+A11+A12+A13+A14+A15+A16+A17+A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17.25" customHeight="1">
       <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
@@ -8690,32 +8698,32 @@
         <v>#CYCLE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="17.25" customHeight="1">
       <c r="C15" s="117" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="17.25" customHeight="1">
       <c r="C16" s="117" t="str">
         <f>C15</f>
         <v>=(+</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1">
       <c r="C17" s="117" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1">
       <c r="C18" s="117" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1">
       <c r="E19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
         <v>15</v>
@@ -8729,7 +8737,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -8739,7 +8747,7 @@
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1">
       <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
@@ -8753,7 +8761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1">
       <c r="C24" s="16">
         <v>10</v>
       </c>
@@ -8764,7 +8772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1">
       <c r="C25" s="16">
         <v>10.122999999999999</v>
       </c>
@@ -8775,7 +8783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1">
       <c r="B26" s="117" t="s">
         <v>20</v>
       </c>
@@ -8789,7 +8797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1">
       <c r="A27" s="117" t="s">
         <v>22</v>
       </c>
@@ -8806,7 +8814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1">
       <c r="A28" s="117" t="s">
         <v>23</v>
       </c>
@@ -8823,7 +8831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1">
       <c r="A29" s="117" t="s">
         <v>24</v>
       </c>
@@ -8840,7 +8848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1">
       <c r="A30" s="117" t="s">
         <v>25</v>
       </c>
@@ -8857,7 +8865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1">
       <c r="A31" s="117" t="s">
         <v>26</v>
       </c>
@@ -8874,7 +8882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1">
       <c r="A32" s="117" t="s">
         <v>27</v>
       </c>
@@ -8891,7 +8899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="17.25" customHeight="1">
       <c r="A33" s="117" t="s">
         <v>28</v>
       </c>
@@ -8908,7 +8916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="17.25" customHeight="1">
       <c r="A34" s="117" t="s">
         <v>29</v>
       </c>
@@ -8919,7 +8927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="17.25" customHeight="1">
       <c r="A35" s="117" t="s">
         <v>30</v>
       </c>
@@ -8936,7 +8944,7 @@
     <mergeCell ref="K3:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C100 B21">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
       <formula>42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8986,7 +8994,7 @@
       <selection sqref="A1:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8998,12 +9006,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9017,7 +9025,7 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
@@ -9037,7 +9045,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9046,51 +9054,54 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025F2510-D243-4DA1-81DE-BBDDA9BC3681}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="9" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="114" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B1" s="115" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C1" s="115" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D1" s="115" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E1" s="115" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F1" s="115" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G1" s="115" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H1" s="115" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="I1" s="116" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>432</v>
+      </c>
+      <c r="J1" s="123" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="104">
         <v>4</v>
       </c>
@@ -9101,7 +9112,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="105" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E2" s="106">
         <v>45575</v>
@@ -9110,7 +9121,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G2" s="107" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="H2" s="106">
         <v>45292</v>
@@ -9118,8 +9129,11 @@
       <c r="I2" s="108">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="124">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="104">
         <v>3</v>
       </c>
@@ -9130,7 +9144,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="105" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="E3" s="106">
         <v>45576</v>
@@ -9139,16 +9153,19 @@
         <v>0.57638888888888884</v>
       </c>
       <c r="G3" s="107" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="H3" s="106">
         <v>45231</v>
       </c>
       <c r="I3" s="108" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>435</v>
+      </c>
+      <c r="J3" s="124">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="104">
         <v>9</v>
       </c>
@@ -9159,7 +9176,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="105" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E4" s="106">
         <v>45574</v>
@@ -9168,7 +9185,7 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="G4" s="107" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="H4" s="106">
         <v>45325</v>
@@ -9176,8 +9193,11 @@
       <c r="I4" s="108">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="124">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="104">
         <v>5</v>
       </c>
@@ -9188,7 +9208,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="105" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="E5" s="106">
         <v>45573</v>
@@ -9197,7 +9217,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="G5" s="105" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H5" s="106">
         <v>45084</v>
@@ -9205,8 +9225,11 @@
       <c r="I5" s="108">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="124">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="109">
         <v>7</v>
       </c>
@@ -9217,7 +9240,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="110" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E6" s="111">
         <v>45566</v>
@@ -9226,17 +9249,20 @@
         <v>0.5229166666666667</v>
       </c>
       <c r="G6" s="110" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="H6" s="111">
         <v>45420</v>
       </c>
       <c r="I6" s="113" t="s">
-        <v>438</v>
+        <v>440</v>
+      </c>
+      <c r="J6" s="124">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations count="10">
     <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6" xr:uid="{B9309757-E2F4-49A1-880B-2F47F04364D6}">
       <formula1>1</formula1>
       <formula2>5</formula2>
@@ -9268,6 +9294,10 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{1E18A174-B5CF-4015-B7DC-F1491351E054}">
       <formula1>"option1,option2,option3"</formula1>
     </dataValidation>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6" xr:uid="{E43B85E8-D498-4841-B610-8D8CED09FAA7}">
+      <formula1>$A$2</formula1>
+      <formula2>2+10</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9284,12 +9314,12 @@
       <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="17.25" customHeight="1">
       <c r="A1" s="117" t="s">
         <v>31</v>
       </c>
@@ -9324,7 +9354,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1">
       <c r="A2" s="117" t="s">
         <v>41</v>
       </c>
@@ -9370,7 +9400,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1">
       <c r="A3" s="117" t="s">
         <v>43</v>
       </c>
@@ -9416,7 +9446,7 @@
         <v>1217.7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="17.25" customHeight="1">
       <c r="A4" s="117" t="s">
         <v>45</v>
       </c>
@@ -9462,7 +9492,7 @@
         <v>1230.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1">
       <c r="A5" s="117" t="s">
         <v>47</v>
       </c>
@@ -9508,7 +9538,7 @@
         <v>1246.7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="17.25" customHeight="1">
       <c r="A6" s="117" t="s">
         <v>49</v>
       </c>
@@ -9554,7 +9584,7 @@
         <v>1213.7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="17.25" customHeight="1">
       <c r="A7" s="117" t="s">
         <v>52</v>
       </c>
@@ -9588,7 +9618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="17.25" customHeight="1">
       <c r="A8" s="117" t="s">
         <v>54</v>
       </c>
@@ -9622,7 +9652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="17.25" customHeight="1">
       <c r="A9" s="117" t="s">
         <v>56</v>
       </c>
@@ -9653,7 +9683,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="17.25" customHeight="1">
       <c r="A10" s="117" t="s">
         <v>58</v>
       </c>
@@ -9669,7 +9699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="17.25" customHeight="1">
       <c r="A11" s="117" t="s">
         <v>59</v>
       </c>
@@ -9688,7 +9718,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="17.25" customHeight="1">
       <c r="A12" s="117" t="s">
         <v>61</v>
       </c>
@@ -9719,7 +9749,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="17.25" customHeight="1">
       <c r="A13" s="117" t="s">
         <v>62</v>
       </c>
@@ -9750,7 +9780,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="17.25" customHeight="1">
       <c r="A14" s="117" t="s">
         <v>67</v>
       </c>
@@ -9766,7 +9796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="17.25" customHeight="1">
       <c r="A15" s="117" t="s">
         <v>68</v>
       </c>
@@ -9782,7 +9812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="17.25" customHeight="1">
       <c r="A16" s="117" t="s">
         <v>69</v>
       </c>
@@ -9798,7 +9828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="17.25" customHeight="1">
       <c r="A17" s="117" t="s">
         <v>70</v>
       </c>
@@ -9814,7 +9844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17.25" customHeight="1">
       <c r="A18" s="117" t="s">
         <v>71</v>
       </c>
@@ -9830,7 +9860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17.25" customHeight="1">
       <c r="A19" s="117" t="s">
         <v>72</v>
       </c>
@@ -9846,7 +9876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17.25" customHeight="1">
       <c r="A20" s="117" t="s">
         <v>73</v>
       </c>
@@ -9862,7 +9892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="17.25" customHeight="1">
       <c r="A21" s="117" t="s">
         <v>74</v>
       </c>
@@ -9878,7 +9908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="17.25" customHeight="1">
       <c r="A22" s="117" t="s">
         <v>76</v>
       </c>
@@ -9894,7 +9924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="17.25" customHeight="1">
       <c r="A23" s="117" t="s">
         <v>77</v>
       </c>
@@ -9910,7 +9940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="17.25" customHeight="1">
       <c r="A24" s="117" t="s">
         <v>78</v>
       </c>
@@ -9927,7 +9957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="17.25" customHeight="1">
       <c r="A25" s="117" t="s">
         <v>79</v>
       </c>
@@ -9943,7 +9973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="17.25" customHeight="1">
       <c r="A26" s="117" t="s">
         <v>81</v>
       </c>
@@ -9959,7 +9989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="17.25" customHeight="1">
       <c r="A27" s="117" t="s">
         <v>82</v>
       </c>
@@ -9975,7 +10005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="17.25" customHeight="1">
       <c r="A28" s="117" t="s">
         <v>83</v>
       </c>
@@ -9992,7 +10022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="17.25" customHeight="1">
       <c r="A29" s="117" t="s">
         <v>84</v>
       </c>
@@ -10008,7 +10038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17.25" customHeight="1">
       <c r="A30" s="117" t="s">
         <v>85</v>
       </c>
@@ -10024,7 +10054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="17.25" customHeight="1">
       <c r="A31" s="117" t="s">
         <v>86</v>
       </c>
@@ -10040,7 +10070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="17.25" customHeight="1">
       <c r="A32" s="117" t="s">
         <v>87</v>
       </c>
@@ -10056,7 +10086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17.25" customHeight="1">
       <c r="A33" s="117" t="s">
         <v>88</v>
       </c>
@@ -10072,7 +10102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="17.25" customHeight="1">
       <c r="A34" s="117" t="s">
         <v>89</v>
       </c>
@@ -10088,7 +10118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17.25" customHeight="1">
       <c r="A35" s="117" t="s">
         <v>90</v>
       </c>
@@ -10104,7 +10134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="17.25" customHeight="1">
       <c r="A36" s="117" t="s">
         <v>91</v>
       </c>
@@ -10120,7 +10150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="17.25" customHeight="1">
       <c r="A37" s="117" t="s">
         <v>92</v>
       </c>
@@ -10136,7 +10166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="17.25" customHeight="1">
       <c r="A38" s="117" t="s">
         <v>93</v>
       </c>
@@ -10153,7 +10183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="17.25" customHeight="1">
       <c r="A39" s="117" t="s">
         <v>94</v>
       </c>
@@ -10169,7 +10199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="17.25" customHeight="1">
       <c r="A40" s="117" t="s">
         <v>95</v>
       </c>
@@ -10185,7 +10215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="17.25" customHeight="1">
       <c r="A41" s="117" t="s">
         <v>96</v>
       </c>
@@ -10201,7 +10231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="17.25" customHeight="1">
       <c r="A42" s="117" t="s">
         <v>97</v>
       </c>
@@ -10217,7 +10247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="17.25" customHeight="1">
       <c r="A43" s="117" t="s">
         <v>98</v>
       </c>
@@ -10233,7 +10263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="17.25" customHeight="1">
       <c r="A44" s="117" t="s">
         <v>99</v>
       </c>
@@ -10249,7 +10279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="17.25" customHeight="1">
       <c r="A45" s="117" t="s">
         <v>100</v>
       </c>
@@ -10265,7 +10295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="17.25" customHeight="1">
       <c r="A46" s="117" t="s">
         <v>101</v>
       </c>
@@ -10281,7 +10311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="17.25" customHeight="1">
       <c r="A47" s="117" t="s">
         <v>102</v>
       </c>
@@ -10297,7 +10327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="17.25" customHeight="1">
       <c r="A48" s="117" t="s">
         <v>103</v>
       </c>
@@ -10313,7 +10343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="17.25" customHeight="1">
       <c r="A49" s="117" t="s">
         <v>104</v>
       </c>
@@ -10329,7 +10359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="17.25" customHeight="1">
       <c r="A50" s="117" t="s">
         <v>105</v>
       </c>
@@ -10346,7 +10376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="17.25" customHeight="1">
       <c r="A51" s="117" t="s">
         <v>106</v>
       </c>
@@ -10363,7 +10393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="17.25" customHeight="1">
       <c r="A52" s="117" t="s">
         <v>107</v>
       </c>
@@ -10379,7 +10409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1">
       <c r="A53" s="117" t="s">
         <v>108</v>
       </c>
@@ -10395,7 +10425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="17.25" customHeight="1">
       <c r="A54" s="117" t="s">
         <v>109</v>
       </c>
@@ -10411,7 +10441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1">
       <c r="A55" s="117" t="s">
         <v>110</v>
       </c>
@@ -10427,7 +10457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1">
       <c r="A56" s="117" t="s">
         <v>111</v>
       </c>
@@ -10443,7 +10473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1">
       <c r="A57" s="117" t="s">
         <v>112</v>
       </c>
@@ -10459,7 +10489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1">
       <c r="A58" s="117" t="s">
         <v>113</v>
       </c>
@@ -10475,7 +10505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1">
       <c r="A59" s="117" t="s">
         <v>114</v>
       </c>
@@ -10491,7 +10521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1">
       <c r="A60" s="117" t="s">
         <v>115</v>
       </c>
@@ -10507,7 +10537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1">
       <c r="A61" s="117" t="s">
         <v>116</v>
       </c>
@@ -10523,7 +10553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1">
       <c r="A62" s="117" t="s">
         <v>117</v>
       </c>
@@ -10539,7 +10569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="17.25" customHeight="1">
       <c r="A63" s="117" t="s">
         <v>118</v>
       </c>
@@ -10555,7 +10585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="17.25" customHeight="1">
       <c r="A64" s="117" t="s">
         <v>119</v>
       </c>
@@ -10571,7 +10601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="17.25" customHeight="1">
       <c r="A65" s="117" t="s">
         <v>120</v>
       </c>
@@ -10587,7 +10617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="17.25" customHeight="1">
       <c r="A66" s="117" t="s">
         <v>121</v>
       </c>
@@ -10603,7 +10633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="17.25" customHeight="1">
       <c r="A67" s="117" t="s">
         <v>122</v>
       </c>
@@ -10619,7 +10649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="17.25" customHeight="1">
       <c r="A68" s="117" t="s">
         <v>123</v>
       </c>
@@ -10635,7 +10665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="17.25" customHeight="1">
       <c r="A69" s="117" t="s">
         <v>125</v>
       </c>
@@ -10651,7 +10681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="17.25" customHeight="1">
       <c r="A70" s="117" t="s">
         <v>127</v>
       </c>
@@ -10667,7 +10697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="17.25" customHeight="1">
       <c r="A71" s="117" t="s">
         <v>129</v>
       </c>
@@ -10683,7 +10713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="17.25" customHeight="1">
       <c r="A72" s="117" t="s">
         <v>130</v>
       </c>
@@ -10699,7 +10729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="17.25" customHeight="1">
       <c r="A73" s="117" t="s">
         <v>131</v>
       </c>
@@ -10715,7 +10745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="17.25" customHeight="1">
       <c r="A74" s="117" t="s">
         <v>132</v>
       </c>
@@ -10731,7 +10761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="17.25" customHeight="1">
       <c r="A75" s="117" t="s">
         <v>133</v>
       </c>
@@ -10747,7 +10777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="17.25" customHeight="1">
       <c r="A76" s="117" t="s">
         <v>134</v>
       </c>
@@ -10763,7 +10793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="17.25" customHeight="1">
       <c r="A77" s="117" t="s">
         <v>135</v>
       </c>
@@ -10779,7 +10809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="17.25" customHeight="1">
       <c r="A78" s="117" t="s">
         <v>136</v>
       </c>
@@ -10795,7 +10825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="17.25" customHeight="1">
       <c r="A79" s="117" t="s">
         <v>137</v>
       </c>
@@ -10811,7 +10841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="17.25" customHeight="1">
       <c r="A80" s="117" t="s">
         <v>138</v>
       </c>
@@ -10827,7 +10857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="17.25" customHeight="1">
       <c r="A81" s="117" t="s">
         <v>139</v>
       </c>
@@ -10843,7 +10873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="17.25" customHeight="1">
       <c r="A82" s="117" t="s">
         <v>141</v>
       </c>
@@ -10859,7 +10889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="17.25" customHeight="1">
       <c r="A83" s="117" t="s">
         <v>142</v>
       </c>
@@ -10875,7 +10905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="17.25" customHeight="1">
       <c r="A84" s="117" t="s">
         <v>143</v>
       </c>
@@ -10891,7 +10921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="17.25" customHeight="1">
       <c r="A85" s="117" t="s">
         <v>144</v>
       </c>
@@ -10907,7 +10937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="17.25" customHeight="1">
       <c r="A86" s="117" t="s">
         <v>146</v>
       </c>
@@ -10923,7 +10953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="17.25" customHeight="1">
       <c r="A87" s="117" t="s">
         <v>147</v>
       </c>
@@ -10939,7 +10969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="17.25" customHeight="1">
       <c r="A88" s="117" t="s">
         <v>148</v>
       </c>
@@ -10955,7 +10985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="17.25" customHeight="1">
       <c r="A89" s="117" t="s">
         <v>149</v>
       </c>
@@ -10971,7 +11001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="17.25" customHeight="1">
       <c r="A90" s="117" t="s">
         <v>150</v>
       </c>
@@ -10987,7 +11017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="17.25" customHeight="1">
       <c r="A91" s="117" t="s">
         <v>151</v>
       </c>
@@ -11003,7 +11033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1">
       <c r="A92" s="117" t="s">
         <v>152</v>
       </c>
@@ -11019,7 +11049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1">
       <c r="A93" s="117" t="s">
         <v>153</v>
       </c>
@@ -11035,7 +11065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1">
       <c r="A94" s="117" t="s">
         <v>154</v>
       </c>
@@ -11051,7 +11081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1">
       <c r="A95" s="117" t="s">
         <v>155</v>
       </c>
@@ -11067,7 +11097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1">
       <c r="A96" s="117" t="s">
         <v>156</v>
       </c>
@@ -11083,7 +11113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="17.25" customHeight="1">
       <c r="A97" s="117" t="s">
         <v>157</v>
       </c>
@@ -11099,7 +11129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="17.25" customHeight="1">
       <c r="A98" s="117" t="s">
         <v>158</v>
       </c>
@@ -11115,7 +11145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="17.25" customHeight="1">
       <c r="A99" s="117" t="s">
         <v>159</v>
       </c>
@@ -11131,20 +11161,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="17.25" customHeight="1">
       <c r="A100" s="117" t="s">
         <v>160</v>
       </c>
       <c r="B100" s="19">
         <f ca="1">NOW()</f>
-        <v>45905.868253935187</v>
+        <v>46044.440208912034</v>
       </c>
       <c r="D100" s="117">
         <f ca="1">IF(ISNUMBER(B100),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="17.25" customHeight="1">
       <c r="A101" s="117" t="s">
         <v>161</v>
       </c>
@@ -11160,7 +11190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="17.25" customHeight="1">
       <c r="A102" s="117" t="s">
         <v>162</v>
       </c>
@@ -11176,7 +11206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="17.25" customHeight="1">
       <c r="A103" s="117" t="s">
         <v>163</v>
       </c>
@@ -11192,7 +11222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="17.25" customHeight="1">
       <c r="A104" s="117" t="s">
         <v>164</v>
       </c>
@@ -11208,7 +11238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="17.25" customHeight="1">
       <c r="A105" s="117" t="s">
         <v>165</v>
       </c>
@@ -11224,7 +11254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="17.25" customHeight="1">
       <c r="A106" s="117" t="s">
         <v>166</v>
       </c>
@@ -11240,7 +11270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="17.25" customHeight="1">
       <c r="A107" s="117" t="s">
         <v>167</v>
       </c>
@@ -11256,7 +11286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="17.25" customHeight="1">
       <c r="A108" s="117" t="s">
         <v>168</v>
       </c>
@@ -11272,7 +11302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="17.25" customHeight="1">
       <c r="A109" s="117" t="s">
         <v>169</v>
       </c>
@@ -11288,7 +11318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="17.25" customHeight="1">
       <c r="A110" s="117" t="s">
         <v>170</v>
       </c>
@@ -11304,7 +11334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="17.25" customHeight="1">
       <c r="A111" s="117" t="s">
         <v>171</v>
       </c>
@@ -11320,12 +11350,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="17.25" customHeight="1">
       <c r="A112" s="117"/>
       <c r="B112" s="117"/>
       <c r="D112" s="117"/>
     </row>
-    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="17.25" customHeight="1">
       <c r="A113" s="117" t="s">
         <v>172</v>
       </c>
@@ -11341,7 +11371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="17.25" customHeight="1">
       <c r="A114" s="117" t="s">
         <v>173</v>
       </c>
@@ -11357,7 +11387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="17.25" customHeight="1">
       <c r="A115" s="117" t="s">
         <v>175</v>
       </c>
@@ -11373,7 +11403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="17.25" customHeight="1">
       <c r="A116" s="117" t="s">
         <v>177</v>
       </c>
@@ -11389,7 +11419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="17.25" customHeight="1">
       <c r="A117" s="117" t="s">
         <v>178</v>
       </c>
@@ -11405,7 +11435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="17.25" customHeight="1">
       <c r="A118" s="117" t="s">
         <v>179</v>
       </c>
@@ -11421,7 +11451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="17.25" customHeight="1">
       <c r="A119" s="117" t="s">
         <v>180</v>
       </c>
@@ -11437,7 +11467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="17.25" customHeight="1">
       <c r="A120" s="117" t="s">
         <v>181</v>
       </c>
@@ -11453,7 +11483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="17.25" customHeight="1">
       <c r="A121" s="117" t="s">
         <v>182</v>
       </c>
@@ -11469,7 +11499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="17.25" customHeight="1">
       <c r="A122" s="117" t="s">
         <v>183</v>
       </c>
@@ -11485,7 +11515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="17.25" customHeight="1">
       <c r="A123" s="117" t="s">
         <v>184</v>
       </c>
@@ -11501,7 +11531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="17.25" customHeight="1">
       <c r="A124" s="117" t="s">
         <v>185</v>
       </c>
@@ -11517,7 +11547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="17.25" customHeight="1">
       <c r="A125" s="117" t="s">
         <v>186</v>
       </c>
@@ -11533,7 +11563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="17.25" customHeight="1">
       <c r="A126" s="117" t="s">
         <v>187</v>
       </c>
@@ -11549,7 +11579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="17.25" customHeight="1">
       <c r="A127" s="117" t="s">
         <v>188</v>
       </c>
@@ -11565,7 +11595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="17.25" customHeight="1">
       <c r="A128" s="117" t="s">
         <v>189</v>
       </c>
@@ -11581,7 +11611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="17.25" customHeight="1">
       <c r="A129" s="117" t="s">
         <v>190</v>
       </c>
@@ -11597,7 +11627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="17.25" customHeight="1">
       <c r="A130" s="117" t="s">
         <v>191</v>
       </c>
@@ -11613,7 +11643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="17.25" customHeight="1">
       <c r="A131" s="117" t="s">
         <v>192</v>
       </c>
@@ -11629,7 +11659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="17.25" customHeight="1">
       <c r="A132" s="117" t="s">
         <v>193</v>
       </c>
@@ -11645,7 +11675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="17.25" customHeight="1">
       <c r="A133" s="117" t="s">
         <v>194</v>
       </c>
@@ -11661,7 +11691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="17.25" customHeight="1">
       <c r="A134" s="117" t="s">
         <v>195</v>
       </c>
@@ -11677,7 +11707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="17.25" customHeight="1">
       <c r="A135" s="117" t="s">
         <v>196</v>
       </c>
@@ -11693,7 +11723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="17.25" customHeight="1">
       <c r="A136" s="117" t="s">
         <v>198</v>
       </c>
@@ -11709,7 +11739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="17.25" customHeight="1">
       <c r="A137" s="117" t="s">
         <v>199</v>
       </c>
@@ -11725,7 +11755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="17.25" customHeight="1">
       <c r="A138" s="117" t="s">
         <v>200</v>
       </c>
@@ -11741,7 +11771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="17.25" customHeight="1">
       <c r="A139" s="117" t="s">
         <v>201</v>
       </c>
@@ -11757,7 +11787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="17.25" customHeight="1">
       <c r="A140" s="117" t="s">
         <v>202</v>
       </c>
@@ -11773,7 +11803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="17.25" customHeight="1">
       <c r="A141" s="117" t="s">
         <v>203</v>
       </c>
@@ -11789,7 +11819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="17.25" customHeight="1">
       <c r="A142" s="117" t="s">
         <v>205</v>
       </c>
@@ -11805,7 +11835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="17.25" customHeight="1">
       <c r="A143" s="117" t="s">
         <v>206</v>
       </c>
@@ -11821,20 +11851,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="17.25" customHeight="1">
       <c r="A144" s="117" t="s">
         <v>207</v>
       </c>
       <c r="B144" s="18">
         <f ca="1">TODAY()</f>
-        <v>45905</v>
+        <v>46044</v>
       </c>
       <c r="D144" s="117">
         <f ca="1">IF(ISNUMBER(B144),1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="17.25" customHeight="1">
       <c r="A145" s="117" t="s">
         <v>208</v>
       </c>
@@ -11850,7 +11880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="17.25" customHeight="1">
       <c r="A146" s="117" t="s">
         <v>210</v>
       </c>
@@ -11866,7 +11896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="17.25" customHeight="1">
       <c r="A147" s="117" t="s">
         <v>211</v>
       </c>
@@ -11882,7 +11912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="17.25" customHeight="1">
       <c r="A148" s="117" t="s">
         <v>213</v>
       </c>
@@ -11898,7 +11928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="17.25" customHeight="1">
       <c r="A149" s="117" t="s">
         <v>214</v>
       </c>
@@ -11914,7 +11944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" ht="17.25" customHeight="1">
       <c r="A150" s="117" t="s">
         <v>215</v>
       </c>
@@ -11930,7 +11960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="17.25" customHeight="1">
       <c r="A151" s="117" t="s">
         <v>216</v>
       </c>
@@ -11946,7 +11976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="17.25" customHeight="1">
       <c r="A152" s="117" t="s">
         <v>217</v>
       </c>
@@ -11962,7 +11992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="17.25" customHeight="1">
       <c r="A153" s="117" t="s">
         <v>218</v>
       </c>
@@ -11978,7 +12008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" ht="17.25" customHeight="1">
       <c r="A154" s="117" t="s">
         <v>219</v>
       </c>
@@ -11995,7 +12025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="17.25" customHeight="1">
       <c r="A155" s="117" t="s">
         <v>220</v>
       </c>
@@ -12011,7 +12041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="17.25" customHeight="1">
       <c r="A156" s="117" t="s">
         <v>221</v>
       </c>
@@ -12027,7 +12057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" ht="17.25" customHeight="1">
       <c r="A157" s="117" t="s">
         <v>222</v>
       </c>
@@ -12043,7 +12073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" ht="17.25" customHeight="1">
       <c r="A158" s="117" t="s">
         <v>223</v>
       </c>
@@ -12059,7 +12089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="17.25" customHeight="1">
       <c r="A159" s="117" t="s">
         <v>224</v>
       </c>
@@ -12075,7 +12105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" ht="17.25" customHeight="1">
       <c r="A160" s="117" t="s">
         <v>225</v>
       </c>
@@ -12091,7 +12121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" ht="17.25" customHeight="1">
       <c r="A161" s="117" t="s">
         <v>226</v>
       </c>
@@ -12107,7 +12137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="17.25" customHeight="1">
       <c r="A162" s="117" t="s">
         <v>227</v>
       </c>
@@ -12123,7 +12153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" ht="17.25" customHeight="1">
       <c r="A163" s="117" t="s">
         <v>229</v>
       </c>
@@ -12141,10 +12171,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D180">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12164,7 +12194,7 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
@@ -12174,17 +12204,17 @@
     <col min="15" max="18" width="9.140625" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>230</v>
       </c>
       <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="122" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="123"/>
+      <c r="E1" s="122"/>
       <c r="F1" t="s">
         <v>233</v>
       </c>
@@ -12192,19 +12222,19 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
         <f>SUM(A1)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
       <c r="H2" t="str">
         <f>[1]Feuil1!$A$1</f>
         <v>referenced string</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="D3" s="85" t="s">
         <v>235</v>
       </c>
@@ -12212,28 +12242,28 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="75" customHeight="1">
       <c r="A5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" outlineLevel="1"/>
+    <row r="11" spans="1:8" outlineLevel="1"/>
+    <row r="12" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="13" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="14" spans="1:8" hidden="1" outlineLevel="2"/>
+    <row r="15" spans="1:8" outlineLevel="1" collapsed="1"/>
+    <row r="16" spans="1:8" outlineLevel="1"/>
+    <row r="17" spans="1:1" outlineLevel="1"/>
+    <row r="18" spans="1:1" outlineLevel="1"/>
+    <row r="30" spans="1:1">
       <c r="A30" t="e" cm="1">
-        <f t="array" aca="1" ref="A30" ca="1">RANDARRAY(2, 2)</f>
+        <f t="array" aca="1" ref="A30" ca="1">_xludf.RANDARRAY(2, 2)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -12258,14 +12288,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1">
       <c r="A1" s="68" t="s">
         <v>239</v>
       </c>
@@ -12287,7 +12317,7 @@
       </c>
       <c r="M1" s="36"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="40" t="s">
         <v>245</v>
       </c>
@@ -12313,7 +12343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="41" t="s">
         <v>252</v>
       </c>
@@ -12336,7 +12366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15">
       <c r="A4" s="42" t="s">
         <v>256</v>
       </c>
@@ -12362,7 +12392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="43" t="s">
         <v>262</v>
       </c>
@@ -12382,7 +12412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="44" t="s">
         <v>266</v>
       </c>
@@ -12405,7 +12435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="45" t="s">
         <v>271</v>
       </c>
@@ -12425,7 +12455,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="21">
       <c r="A8" s="46" t="s">
         <v>275</v>
       </c>
@@ -12448,7 +12478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="47" t="s">
         <v>280</v>
       </c>
@@ -12465,7 +12495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="48" t="s">
         <v>283</v>
       </c>
@@ -12473,7 +12503,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1">
       <c r="A11" s="49" t="s">
         <v>285</v>
       </c>
@@ -12482,7 +12512,7 @@
       </c>
       <c r="F11" s="36"/>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="18.75" customHeight="1">
       <c r="A12" s="50" t="s">
         <v>287</v>
       </c>
@@ -12496,7 +12526,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A13" s="51" t="s">
         <v>290</v>
       </c>
@@ -12507,7 +12537,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A14" s="52" t="s">
         <v>291</v>
       </c>
@@ -12521,7 +12551,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
       <c r="A15" s="53" t="s">
         <v>293</v>
       </c>
@@ -12532,7 +12562,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
       <c r="A16" s="54" t="s">
         <v>294</v>
       </c>
@@ -12546,12 +12576,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.5" thickBot="1">
       <c r="A17" s="55" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.5" thickBot="1">
       <c r="A18" s="74" t="s">
         <v>297</v>
       </c>
@@ -12563,7 +12593,7 @@
       </c>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13.5" thickBot="1">
       <c r="A19" s="75" t="s">
         <v>300</v>
       </c>
@@ -12574,7 +12604,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="51.75" thickBot="1">
       <c r="A20" s="76" t="s">
         <v>303</v>
       </c>
@@ -12588,12 +12618,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.5" thickBot="1">
       <c r="A21" s="77" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.5" thickBot="1">
       <c r="A22" s="78" t="s">
         <v>307</v>
       </c>
@@ -12602,13 +12632,13 @@
       </c>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.5" thickBot="1">
       <c r="A23" s="79" t="s">
         <v>309</v>
       </c>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="A24" s="80" t="s">
         <v>310</v>
       </c>
@@ -12617,20 +12647,20 @@
       </c>
       <c r="E24" s="21"/>
     </row>
-    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="26" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C26" s="67" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="14.25" thickTop="1" thickBot="1"/>
+    <row r="28" spans="1:6" ht="14.25" thickTop="1" thickBot="1">
       <c r="C28" s="88" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="13.5" thickTop="1"/>
+    <row r="30" spans="1:6">
       <c r="C30" s="87" t="s">
         <v>314</v>
       </c>
@@ -12645,17 +12675,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D919E811-4385-4D35-A19E-3B7E0E659A89}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.5" thickBot="1">
       <c r="A1" s="37" t="s">
         <v>315</v>
       </c>
@@ -12672,7 +12702,7 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="38" t="s">
         <v>319</v>
       </c>
@@ -12695,7 +12725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="38" t="s">
         <v>321</v>
       </c>
@@ -12718,7 +12748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="38" t="s">
         <v>325</v>
       </c>
@@ -12738,7 +12768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="38" t="s">
         <v>328</v>
       </c>
@@ -12762,7 +12792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="38" t="s">
         <v>330</v>
       </c>
@@ -12785,7 +12815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="38" t="s">
         <v>333</v>
       </c>
@@ -12811,7 +12841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="38" t="s">
         <v>337</v>
       </c>
@@ -12822,7 +12852,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="38" t="s">
         <v>339</v>
       </c>
@@ -12831,7 +12861,7 @@
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.5" thickBot="1">
       <c r="A10" s="38" t="s">
         <v>340</v>
       </c>
@@ -12849,7 +12879,7 @@
       <c r="I10" s="36"/>
       <c r="J10" s="36"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="38" t="s">
         <v>342</v>
       </c>
@@ -12872,13 +12902,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="38" t="s">
         <v>344</v>
       </c>
       <c r="B12" s="39">
         <f ca="1">TODAY()</f>
-        <v>45905</v>
+        <v>46044</v>
       </c>
       <c r="C12" s="39">
         <f>DATE(2010,10,2)</f>
@@ -12897,7 +12927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="38" t="s">
         <v>346</v>
       </c>
@@ -12920,7 +12950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="38" t="s">
         <v>348</v>
       </c>
@@ -12946,7 +12976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="38" t="s">
         <v>350</v>
       </c>
@@ -12966,7 +12996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="38" t="s">
         <v>352</v>
       </c>
@@ -12989,7 +13019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="38" t="s">
         <v>354</v>
       </c>
@@ -13012,7 +13042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="38" t="s">
         <v>356</v>
       </c>
@@ -13035,7 +13065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="38" t="s">
         <v>358</v>
       </c>
@@ -13058,7 +13088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="38" t="s">
         <v>360</v>
       </c>
@@ -13081,7 +13111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="38" t="s">
         <v>362</v>
       </c>
@@ -13107,7 +13137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="38" t="s">
         <v>364</v>
       </c>
@@ -13133,7 +13163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="38" t="s">
         <v>366</v>
       </c>
@@ -13159,7 +13189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="G24" s="34" t="s">
         <v>368</v>
       </c>
@@ -13176,7 +13206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="38" t="s">
         <v>369</v>
       </c>
@@ -13202,7 +13232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="G26" s="34" t="s">
         <v>371</v>
       </c>
@@ -13222,7 +13252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="21" t="s">
         <v>372</v>
       </c>
@@ -13248,7 +13278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="G28" s="34" t="s">
         <v>374</v>
       </c>
@@ -13268,9 +13298,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="38" t="s">
-        <v>440</v>
+        <v>375</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -13279,7 +13309,7 @@
         <v>10</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H29">
         <v>5</v>
@@ -13297,9 +13327,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="G30" s="34" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H30">
         <v>5</v>
@@ -13317,9 +13347,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="13.5" thickBot="1">
       <c r="G31" s="35" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H31" s="36">
         <v>5</v>
@@ -13331,9 +13361,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="G32" s="34" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H32">
         <v>5</v>
@@ -13345,9 +13375,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:10">
       <c r="G33" s="34" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H33">
         <v>5</v>
@@ -13359,9 +13389,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:10">
       <c r="G34" s="34" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H34">
         <v>5</v>
@@ -13373,9 +13403,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:10">
       <c r="G35" s="34" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H35">
         <v>5</v>
@@ -13387,9 +13417,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:10">
       <c r="G36" s="34" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H36">
         <v>5</v>
@@ -13401,9 +13431,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:10">
       <c r="G37" s="34" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H37">
         <v>5</v>
@@ -13415,110 +13445,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="7:10">
       <c r="G39" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="23" priority="59">
+    <cfRule type="expression" dxfId="41" priority="59">
       <formula>ODD(B15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:B27">
-    <cfRule type="cellIs" dxfId="22" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="aboveAverage" dxfId="21" priority="115"/>
+    <cfRule type="aboveAverage" dxfId="39" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="beginsWith" dxfId="20" priority="74" operator="beginsWith" text="rule">
+    <cfRule type="beginsWith" dxfId="38" priority="74" operator="beginsWith" text="rule">
       <formula>LEFT(B3,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="containsBlanks" dxfId="19" priority="72">
+    <cfRule type="containsBlanks" dxfId="37" priority="72">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="containsErrors" dxfId="18" priority="71">
+    <cfRule type="containsErrors" dxfId="36" priority="71">
       <formula>ISERROR(B5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="containsText" dxfId="17" priority="70" operator="containsText" text="rule">
+    <cfRule type="containsText" dxfId="35" priority="70" operator="containsText" text="rule">
       <formula>NOT(ISERROR(SEARCH("rule",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="endsWith" dxfId="16" priority="68" operator="endsWith" text="rule">
+    <cfRule type="endsWith" dxfId="34" priority="68" operator="endsWith" text="rule">
       <formula>RIGHT(B8,LEN("rule"))="rule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C9">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="67">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="67">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="notContainsErrors" dxfId="14" priority="66">
+    <cfRule type="notContainsErrors" dxfId="32" priority="66">
       <formula>NOT(ISERROR(B10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="notContainsText" dxfId="13" priority="65" operator="notContains" text="rule">
+    <cfRule type="notContainsText" dxfId="31" priority="65" operator="notContains" text="rule">
       <formula>ISERROR(SEARCH("rule",B11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C12">
-    <cfRule type="timePeriod" dxfId="12" priority="64" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="30" priority="64" timePeriod="today">
       <formula>FLOOR(B12,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:C13">
-    <cfRule type="top10" dxfId="11" priority="116" rank="1"/>
+    <cfRule type="top10" dxfId="29" priority="116" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="10" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="46" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="cellIs" dxfId="9" priority="57" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="57" operator="notEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C18">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C20">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:C21">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="between">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="notBetween">
       <formula>2</formula>
       <formula>4</formula>
     </cfRule>
@@ -13552,16 +13582,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="between">
       <formula>$B$23</formula>
       <formula>2+2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="duplicateValues" dxfId="1" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:D14">
-    <cfRule type="uniqueValues" dxfId="0" priority="97"/>
+    <cfRule type="uniqueValues" dxfId="18" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
     <cfRule type="colorScale" priority="45">
@@ -13989,7 +14019,7 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
@@ -14001,12 +14031,12 @@
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15">
       <c r="C3" s="17" t="s">
         <v>35</v>
       </c>
@@ -14014,25 +14044,25 @@
         <v>36</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="117" t="s">
         <v>42</v>
       </c>
@@ -14063,7 +14093,7 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="C5" s="117" t="s">
         <v>44</v>
       </c>
@@ -14094,9 +14124,9 @@
         <v>Rank</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="C6" s="117" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D6" s="117">
         <f>SUBTOTAL(109,Table3[Age])</f>
@@ -14127,9 +14157,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="B8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -14138,22 +14168,22 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="J8" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="C9">
         <v>3</v>
       </c>
@@ -14181,18 +14211,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="B11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C11" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D11" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="C12">
         <v>3</v>
       </c>
@@ -14200,9 +14230,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="B14" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -14211,7 +14241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="C15">
         <v>3</v>
       </c>
@@ -14219,9 +14249,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -14230,7 +14260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="C18">
         <v>3</v>
       </c>
@@ -14238,9 +14268,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -14249,7 +14279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="C21">
         <v>3</v>
       </c>
@@ -14257,9 +14287,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -14268,7 +14298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4">
       <c r="C24">
         <v>3</v>
       </c>
@@ -14276,9 +14306,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -14287,7 +14317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4">
       <c r="C27">
         <v>3</v>
       </c>
@@ -14295,45 +14325,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4">
       <c r="C28" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D28">
         <f>SUBTOTAL(109,Table4910[Column2])</f>
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C30" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D30" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" hidden="1">
       <c r="C31" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D31" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
       <c r="C32" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D32" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -14361,7 +14391,7 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -14382,9 +14412,9 @@
     <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15">
       <c r="A1" s="92" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -14392,7 +14422,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="117"/>
       <c r="B2" s="117"/>
       <c r="C2" s="117"/>
@@ -14400,21 +14430,21 @@
       <c r="E2" s="117"/>
       <c r="F2" s="117"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="117"/>
       <c r="B3" s="117"/>
       <c r="C3" s="89" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D3" s="89" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="117"/>
       <c r="B4" s="117"/>
       <c r="C4" s="89" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D4">
         <v>12.1</v>
@@ -14441,10 +14471,10 @@
         <v>12052</v>
       </c>
       <c r="L4" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="117"/>
       <c r="B5" s="117"/>
       <c r="C5" s="90" t="s">
@@ -14457,7 +14487,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="117"/>
       <c r="B6" s="117"/>
       <c r="C6" s="91">
@@ -14470,7 +14500,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="117"/>
       <c r="B7" s="117"/>
       <c r="C7" s="90" t="s">
@@ -14483,7 +14513,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="117"/>
       <c r="B8" s="117"/>
       <c r="C8" s="91">
@@ -14496,7 +14526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="117"/>
       <c r="B9" s="117"/>
       <c r="C9" s="90" t="s">
@@ -14509,7 +14539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="117"/>
       <c r="B10" s="117"/>
       <c r="C10" s="91">
@@ -14522,7 +14552,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="C11" s="90" t="s">
         <v>44</v>
       </c>
@@ -14533,7 +14563,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="C12" s="91">
         <v>23000</v>
       </c>
@@ -14544,7 +14574,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="C13" s="90" t="s">
         <v>50</v>
       </c>
@@ -14555,7 +14585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="C14" s="91">
         <v>2</v>
       </c>
@@ -14566,7 +14596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="C15" s="90" t="s">
         <v>48</v>
       </c>
@@ -14577,7 +14607,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="C16" s="91">
         <v>50024</v>
       </c>
@@ -14588,7 +14618,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:12">
       <c r="C17" s="90" t="s">
         <v>53</v>
       </c>
@@ -14599,7 +14629,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:12">
       <c r="C18" s="91">
         <v>189576</v>
       </c>
@@ -14610,7 +14640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:12">
       <c r="C19" s="90" t="s">
         <v>57</v>
       </c>
@@ -14621,7 +14651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:12">
       <c r="C20" s="91">
         <v>5000</v>
       </c>
@@ -14632,9 +14662,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:12">
       <c r="C21" s="90" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D21">
         <v>9</v>
@@ -14678,31 +14708,31 @@
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B2" s="117"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -14719,25 +14749,25 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="51">
       <c r="A1" s="99" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B7" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -14745,7 +14775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -14753,7 +14783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -14761,7 +14791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -14769,7 +14799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>5</v>
       </c>

</xml_diff>